<commit_message>
changed ui, fixed training data bug
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDS_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDS_2020_2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\irpa_db\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE48486F-A6E4-4DB5-84A4-E5983F70C39F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D66353-55EC-436F-BD6C-77BA703BDE38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="23" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="27" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="23" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1303" uniqueCount="644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1305" uniqueCount="646">
   <si>
     <t>Answer</t>
   </si>
@@ -1539,9 +1539,6 @@
   </si>
   <si>
     <t>What is the average need-based loan for students who were awarded any need-based self-help aid?</t>
-  </si>
-  <si>
-    <t>The total number of [enrollment_status] instructional faculty who are [gender] is &lt;value&gt;</t>
   </si>
   <si>
     <t>The total number of [enrollment_status] instructional faculty who have a [degree_level] degree is &lt;value&gt;</t>
@@ -1717,49 +1714,25 @@
     <t>What other units are recommended for admission?</t>
   </si>
   <si>
-    <t>How many Computer and information scienses degrees are conferred?</t>
-  </si>
-  <si>
-    <t>There are 15.7% bachelor's degrees conferred are Computer and information scienses, CIP is 11</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
     <t>How many Engineering degrees are conferred?</t>
   </si>
   <si>
-    <t>There are 73.1% bachelor's degrees conferred are Engineering , CIP is 14</t>
-  </si>
-  <si>
     <t>How many Biological/life sciences degrees are conferred?</t>
   </si>
   <si>
-    <t>There are 2.2% bachelor's degrees conferred are  Biological/life sciences , CIP is 26</t>
-  </si>
-  <si>
     <t>How many Mathematics and statistics degrees are conferred?</t>
   </si>
   <si>
-    <t>There are 5.2% bachelor's degrees conferred are Mathematics and statistics, CIP is 27</t>
-  </si>
-  <si>
     <t>How many Interdisciplinary studies degrees are conferred?</t>
   </si>
   <si>
-    <t>There are 0.7% bachelor's degrees conferred are Interdisciplinary studies, CIP is 30</t>
-  </si>
-  <si>
     <t>How many Physical sciences degrees are conferred?</t>
   </si>
   <si>
-    <t>There are 3.0% bachelor's degrees conferred are Physical sciences, CIP is 40</t>
-  </si>
-  <si>
     <t>How many Social sciences degrees are conferred?</t>
-  </si>
-  <si>
-    <t>There are 0.2% bachelor's degrees conferred are Social sciences, CIP is 45</t>
   </si>
   <si>
     <t>Of previous units, how many lab units are recommended for admission?</t>
@@ -2007,6 +1980,39 @@
   </si>
   <si>
     <t>The amount of [need_non_need_base_aid] (xor [self-help_aid] {[financial_aid_type] scholarship or grants} (xor {tuition [*waiver]} (xor [*parent] [*student]) loan)))</t>
+  </si>
+  <si>
+    <t>What majors does Rose-Hulman offer?</t>
+  </si>
+  <si>
+    <t>15.7% bachelor's degrees conferred are Computer and information science</t>
+  </si>
+  <si>
+    <t>73.1% bachelor's degrees conferred are Engineering</t>
+  </si>
+  <si>
+    <t>2.2% bachelor's degrees conferred are  Biological/life sciences.</t>
+  </si>
+  <si>
+    <t>5.2% bachelor's degrees conferred are Mathematics and statistics.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7% bachelor's degrees conferred are Interdisciplinary studies.</t>
+  </si>
+  <si>
+    <t>3.0% bachelor's degrees conferred are Physical sciences</t>
+  </si>
+  <si>
+    <t>0.2% bachelor's degrees conferred are Social sciences</t>
+  </si>
+  <si>
+    <t>How many Computer and information degrees are conferred?</t>
+  </si>
+  <si>
+    <t>Rose-Hulman offers deree in  Computer science,  engineering degrees, biological/life sciences,  physical sciences and social sciences</t>
+  </si>
+  <si>
+    <t>The total number of [enrollment_status] instructional faculty {who are [gender]} is &lt;value&gt;</t>
   </si>
 </sst>
 </file>
@@ -2384,8 +2390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E422E2F-D9FA-411F-968E-DE340F994DF5}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2687,7 +2693,7 @@
         <v>266</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>618</v>
+        <v>609</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -2864,7 +2870,7 @@
         <v>266</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>617</v>
+        <v>608</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -2996,7 +3002,7 @@
         <v>266</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>616</v>
+        <v>607</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -3173,7 +3179,7 @@
         <v>266</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>611</v>
+        <v>602</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -3184,7 +3190,7 @@
         <v>196</v>
       </c>
       <c r="D17" t="s">
-        <v>578</v>
+        <v>569</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -3268,7 +3274,7 @@
         <v>467</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>579</v>
+        <v>570</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -3289,7 +3295,7 @@
         <v>266</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>610</v>
+        <v>601</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -3494,7 +3500,7 @@
         <v>31</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -3628,7 +3634,7 @@
         <v>266</v>
       </c>
       <c r="B36" t="s">
-        <v>612</v>
+        <v>603</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -3697,7 +3703,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>98</v>
@@ -3835,7 +3841,7 @@
         <v>266</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>613</v>
+        <v>604</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -3967,7 +3973,7 @@
         <v>266</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>614</v>
+        <v>605</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -4140,7 +4146,7 @@
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>159</v>
@@ -4151,7 +4157,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>318</v>
@@ -4702,7 +4708,7 @@
         <v>266</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -5255,206 +5261,206 @@
     </row>
     <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>581</v>
+        <v>572</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>582</v>
+        <v>573</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>583</v>
+        <v>574</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>640</v>
+        <v>631</v>
       </c>
       <c r="B3" s="6">
         <v>45017</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>583</v>
+        <v>574</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>641</v>
+        <v>632</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>584</v>
+        <v>575</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>583</v>
+        <v>574</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>642</v>
+        <v>633</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>586</v>
+        <v>577</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>587</v>
+        <v>578</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>583</v>
+        <v>574</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>588</v>
+        <v>579</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>589</v>
+        <v>580</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>583</v>
+        <v>574</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>590</v>
+        <v>581</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>591</v>
+        <v>582</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>583</v>
+        <v>574</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>592</v>
+        <v>583</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>593</v>
+        <v>584</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>583</v>
+        <v>574</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>594</v>
+        <v>585</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>639</v>
+        <v>630</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>583</v>
+        <v>574</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>595</v>
+        <v>586</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>596</v>
+        <v>587</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>583</v>
+        <v>574</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>597</v>
+        <v>588</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>585</v>
+        <v>576</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>583</v>
+        <v>574</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>598</v>
+        <v>589</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>585</v>
+        <v>576</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>583</v>
+        <v>574</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>599</v>
+        <v>590</v>
       </c>
       <c r="B14" s="6">
         <v>1500</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>583</v>
+        <v>574</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>600</v>
+        <v>591</v>
       </c>
       <c r="B15" s="6">
         <v>1500</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>583</v>
+        <v>574</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>601</v>
+        <v>592</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>602</v>
+        <v>593</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>583</v>
+        <v>574</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>603</v>
+        <v>594</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>604</v>
+        <v>595</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>583</v>
+        <v>574</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>605</v>
+        <v>596</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>606</v>
+        <v>597</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>583</v>
+        <v>574</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>607</v>
+        <v>598</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>606</v>
+        <v>597</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>583</v>
+        <v>574</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>608</v>
+        <v>599</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>609</v>
+        <v>600</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>583</v>
+        <v>574</v>
       </c>
     </row>
   </sheetData>
@@ -5467,7 +5473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E00C0EE-B5EA-4C5D-A3F6-0409760A68CF}">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -5559,7 +5565,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>387</v>
@@ -5567,7 +5573,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>388</v>
@@ -5575,7 +5581,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>389</v>
@@ -5583,7 +5589,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>381</v>
@@ -5591,7 +5597,7 @@
     </row>
     <row r="15" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>381</v>
@@ -5599,7 +5605,7 @@
     </row>
     <row r="16" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>381</v>
@@ -5672,7 +5678,7 @@
         <v>266</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>643</v>
+        <v>634</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -6499,10 +6505,10 @@
     </row>
     <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>619</v>
+        <v>610</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>620</v>
+        <v>611</v>
       </c>
       <c r="C2" t="s">
         <v>196</v>
@@ -6510,10 +6516,10 @@
     </row>
     <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
+        <v>612</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>621</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>630</v>
       </c>
       <c r="C3" t="s">
         <v>196</v>
@@ -6521,10 +6527,10 @@
     </row>
     <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
+        <v>613</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>622</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>631</v>
       </c>
       <c r="C4" t="s">
         <v>196</v>
@@ -6532,10 +6538,10 @@
     </row>
     <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>632</v>
+        <v>623</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>623</v>
+        <v>614</v>
       </c>
       <c r="C5" t="s">
         <v>196</v>
@@ -6543,10 +6549,10 @@
     </row>
     <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>633</v>
+        <v>624</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>634</v>
+        <v>625</v>
       </c>
       <c r="C6" t="s">
         <v>196</v>
@@ -6554,57 +6560,57 @@
     </row>
     <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>624</v>
+        <v>615</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>625</v>
+        <v>616</v>
       </c>
       <c r="C7" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
+        <v>617</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>626</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>635</v>
-      </c>
       <c r="C8" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>627</v>
+        <v>618</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>638</v>
+        <v>629</v>
       </c>
       <c r="C9" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
+        <v>619</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>628</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>637</v>
-      </c>
       <c r="C10" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>629</v>
+        <v>620</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>636</v>
+        <v>627</v>
       </c>
       <c r="C11" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
   </sheetData>
@@ -6636,7 +6642,7 @@
     </row>
     <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B2">
         <v>33</v>
@@ -6644,7 +6650,7 @@
     </row>
     <row r="3" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -6652,7 +6658,7 @@
     </row>
     <row r="4" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B4">
         <v>8</v>
@@ -6660,7 +6666,7 @@
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -6685,7 +6691,7 @@
         <v>266</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -6838,7 +6844,7 @@
         <v>266</v>
       </c>
       <c r="B13" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -6878,7 +6884,7 @@
         <v>314</v>
       </c>
       <c r="B18" t="s">
-        <v>567</v>
+        <v>558</v>
       </c>
     </row>
   </sheetData>
@@ -6890,8 +6896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C2A9967-94EA-41CF-ACB5-C81483AD239D}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6959,7 +6965,7 @@
         <v>266</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>489</v>
+        <v>645</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -7003,7 +7009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2758D6-F888-4498-88A0-7DFBF7091CA2}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -7104,7 +7110,7 @@
         <v>266</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -7172,10 +7178,10 @@
     </row>
     <row r="2" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>496</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>497</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>498</v>
       </c>
       <c r="C2" t="s">
         <v>196</v>
@@ -7186,7 +7192,7 @@
         <v>442</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C3" t="s">
         <v>196</v>
@@ -7270,15 +7276,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B3">
         <v>76</v>
@@ -7286,7 +7292,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B4">
         <v>216</v>
@@ -7294,7 +7300,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B5">
         <v>129</v>
@@ -7302,7 +7308,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -7310,7 +7316,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -7318,7 +7324,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -7326,7 +7332,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -7407,7 +7413,7 @@
     </row>
     <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -7415,7 +7421,7 @@
     </row>
     <row r="3" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B3">
         <v>33</v>
@@ -7423,7 +7429,7 @@
     </row>
     <row r="4" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B4">
         <v>31</v>
@@ -7431,7 +7437,7 @@
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -7439,7 +7445,7 @@
     </row>
     <row r="6" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -7447,7 +7453,7 @@
     </row>
     <row r="7" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -7455,7 +7461,7 @@
     </row>
     <row r="8" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -7500,16 +7506,16 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A321CDB-4432-42F8-8542-C3389F944EAE}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.21875" customWidth="1"/>
-    <col min="2" max="2" width="34.21875" customWidth="1"/>
+    <col min="1" max="1" width="44" customWidth="1"/>
+    <col min="2" max="2" width="52.6640625" customWidth="1"/>
     <col min="3" max="3" width="26.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7524,81 +7530,89 @@
         <v>317</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>547</v>
+        <v>643</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>548</v>
+        <v>636</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
+        <v>547</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>637</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>548</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>638</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>549</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>639</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>550</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B6" s="5" t="s">
+        <v>640</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>551</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>552</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>553</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>554</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>555</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>556</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>557</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>558</v>
-      </c>
       <c r="B7" s="5" t="s">
-        <v>559</v>
+        <v>641</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>560</v>
+        <v>552</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>561</v>
+        <v>642</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>549</v>
+        <v>546</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>635</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>644</v>
       </c>
     </row>
   </sheetData>
@@ -7631,7 +7645,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>568</v>
+        <v>559</v>
       </c>
       <c r="B2">
         <v>36</v>
@@ -7639,7 +7653,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>569</v>
+        <v>560</v>
       </c>
       <c r="B3">
         <v>34</v>
@@ -7647,7 +7661,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>570</v>
+        <v>561</v>
       </c>
       <c r="B4">
         <v>31</v>
@@ -7655,7 +7669,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>571</v>
+        <v>562</v>
       </c>
       <c r="B5">
         <v>356</v>
@@ -7663,7 +7677,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>577</v>
+        <v>568</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -7671,7 +7685,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>572</v>
+        <v>563</v>
       </c>
       <c r="B7">
         <v>36</v>
@@ -7679,7 +7693,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>573</v>
+        <v>564</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -7687,7 +7701,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>574</v>
+        <v>565</v>
       </c>
       <c r="B9">
         <v>31</v>
@@ -7695,7 +7709,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>575</v>
+        <v>566</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -7719,7 +7733,7 @@
         <v>266</v>
       </c>
       <c r="B13" t="s">
-        <v>576</v>
+        <v>567</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -7954,7 +7968,7 @@
         <v>266</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -8023,7 +8037,7 @@
     </row>
     <row r="2" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B2" s="5">
         <v>4</v>
@@ -8034,7 +8048,7 @@
     </row>
     <row r="3" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B3" s="5">
         <v>4</v>
@@ -8045,7 +8059,7 @@
     </row>
     <row r="4" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B4" s="5">
         <v>3</v>
@@ -8056,7 +8070,7 @@
     </row>
     <row r="5" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B5" s="5">
         <v>3</v>
@@ -8067,7 +8081,7 @@
     </row>
     <row r="6" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B6" s="5">
         <v>0</v>
@@ -8078,7 +8092,7 @@
     </row>
     <row r="7" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B7" s="5">
         <v>2</v>
@@ -8089,7 +8103,7 @@
     </row>
     <row r="8" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -8100,7 +8114,7 @@
     </row>
     <row r="9" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B9" s="5">
         <v>0</v>
@@ -8111,7 +8125,7 @@
     </row>
     <row r="10" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B10" s="5">
         <v>0</v>
@@ -8122,7 +8136,7 @@
     </row>
     <row r="11" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B11" s="5">
         <v>0</v>
@@ -8133,7 +8147,7 @@
     </row>
     <row r="12" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B12" s="5">
         <v>0</v>
@@ -8144,10 +8158,10 @@
     </row>
     <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>563</v>
+        <v>554</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>564</v>
+        <v>555</v>
       </c>
       <c r="C13" t="s">
         <v>196</v>
@@ -8171,7 +8185,7 @@
         <v>266</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>565</v>
+        <v>556</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -8236,7 +8250,7 @@
     </row>
     <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -8244,7 +8258,7 @@
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -8252,7 +8266,7 @@
     </row>
     <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -8260,7 +8274,7 @@
     </row>
     <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>562</v>
+        <v>553</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -8268,7 +8282,7 @@
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -8276,7 +8290,7 @@
     </row>
     <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -8284,7 +8298,7 @@
     </row>
     <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -8292,7 +8306,7 @@
     </row>
     <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -8300,7 +8314,7 @@
     </row>
     <row r="10" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -8308,7 +8322,7 @@
     </row>
     <row r="11" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -8316,7 +8330,7 @@
     </row>
     <row r="12" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -8341,7 +8355,7 @@
         <v>266</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>566</v>
+        <v>557</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
refactored metadata, work on get available options
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDS_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDS_2020_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\irpa_main\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A364D1D3-24AB-4EEB-B9B5-C48E85B0B24D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D58973C-7844-44AC-B0B7-10399FFDCCA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="17" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="23" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="678">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1374" uniqueCount="678">
   <si>
     <t>Answer</t>
   </si>
@@ -1559,9 +1559,6 @@
     <t>What is the amount of non-need-based state and other self-help work study awarded to students?</t>
   </si>
   <si>
-    <t>The number of [gender] [is_first_time] [is_first_year] [undergraduate_grade_level] [degree-goal] [student_level] students enrolled is &lt;value&gt;</t>
-  </si>
-  <si>
     <t>The (xor [*percentage] number) of students {who graduated (xor {[range] [number] years and [number] years} {[range] [number] years}) in the [initial_final] [year] cohort is &lt;value&gt;</t>
   </si>
   <si>
@@ -1875,9 +1872,6 @@
     <t>The amount of [need_non_need_base_aid] (xor [self-help_aid] {[financial_aid_type] scholarship or grants} (xor {tuition [*waiver]} (xor [*parent] [*student]) loan)))</t>
   </si>
   <si>
-    <t>What majors does Rose-Hulman offer?</t>
-  </si>
-  <si>
     <t>15.7% bachelor's degrees conferred are Computer and information science</t>
   </si>
   <si>
@@ -1905,24 +1899,6 @@
     <t>The total number of [enrollment_status] instructional faculty {who are [gender]} is &lt;value&gt;</t>
   </si>
   <si>
-    <t>Total first-time, first-year (freshman) men who applied?</t>
-  </si>
-  <si>
-    <t>Total first-time, first-year (freshman) women who applied</t>
-  </si>
-  <si>
-    <t>Total full-time, first-time, first-year (freshman) men who enrolled</t>
-  </si>
-  <si>
-    <t>Total part-time, first-time, first-year (freshman) men who enrolled</t>
-  </si>
-  <si>
-    <t>Total full-time, first-time, first-year (freshman) women who enrolled</t>
-  </si>
-  <si>
-    <t>Total part-time, first-time, first-year (freshman) women who enrolled</t>
-  </si>
-  <si>
     <t>Do you have a policy of placing students on a waiting list?</t>
   </si>
   <si>
@@ -2022,12 +1998,6 @@
     <t>The level of applicant's interest is considered in admission decisions.</t>
   </si>
   <si>
-    <t>What is the total first-time, first-year (freshman) male who were admitted</t>
-  </si>
-  <si>
-    <t>What is the total first-time, first-year (freshman)  female who were admitted</t>
-  </si>
-  <si>
     <t>Rose-Hulman offers degree in  Computer science,  engineering degrees, biological/life sciences,  physical sciences and social sciences</t>
   </si>
   <si>
@@ -2113,6 +2083,36 @@
   </si>
   <si>
     <t>How many male transfer students//applicants are enrolled?</t>
+  </si>
+  <si>
+    <t>What majors does Rose-Hulman award?</t>
+  </si>
+  <si>
+    <t>The number of [gender] [is_first_time] [is_first_year] [undergraduate_grade_level] [enrollment_status] [degree-goal] [student_level] students enrolled is &lt;value&gt;</t>
+  </si>
+  <si>
+    <t>Total first-time, first-year (freshman) female students who applied</t>
+  </si>
+  <si>
+    <t>Total first-time, first-year (freshman) male students who applied?</t>
+  </si>
+  <si>
+    <t>What is the total first-time, first-year (freshman) male students  who were admitted</t>
+  </si>
+  <si>
+    <t>What is the total first-time, first-year (freshman)  female students who were admitted</t>
+  </si>
+  <si>
+    <t>Total full-time, first-time, first-year (freshman) male students who enrolled</t>
+  </si>
+  <si>
+    <t>Total part-time, first-time, first-year (freshman) male students who enrolled</t>
+  </si>
+  <si>
+    <t>Total full-time, first-time, first-year (freshman) female students who enrolled</t>
+  </si>
+  <si>
+    <t>Total part-time, first-time, first-year (freshman) female students who enrolled</t>
   </si>
 </sst>
 </file>
@@ -2712,8 +2712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3551768-8BC9-4E69-8C86-830DF8B3DA69}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2736,10 +2736,10 @@
     </row>
     <row r="2" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>614</v>
+        <v>606</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>625</v>
+        <v>617</v>
       </c>
       <c r="C2" t="s">
         <v>183</v>
@@ -2747,10 +2747,10 @@
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>615</v>
+        <v>607</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="C3" t="s">
         <v>183</v>
@@ -2758,10 +2758,10 @@
     </row>
     <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>616</v>
+        <v>608</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>617</v>
+        <v>609</v>
       </c>
       <c r="C4" t="s">
         <v>183</v>
@@ -2769,10 +2769,10 @@
     </row>
     <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>618</v>
+        <v>610</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>619</v>
+        <v>611</v>
       </c>
       <c r="C5" t="s">
         <v>183</v>
@@ -2787,7 +2787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5DC138E-AAA1-4452-BC05-6992F74BED09}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="74" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="74" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -2811,7 +2811,7 @@
     </row>
     <row r="2" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B2" s="5">
         <v>4</v>
@@ -2822,7 +2822,7 @@
     </row>
     <row r="3" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B3" s="5">
         <v>4</v>
@@ -2833,7 +2833,7 @@
     </row>
     <row r="4" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B4" s="5">
         <v>3</v>
@@ -2844,7 +2844,7 @@
     </row>
     <row r="5" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B5" s="5">
         <v>3</v>
@@ -2855,7 +2855,7 @@
     </row>
     <row r="6" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B6" s="5">
         <v>0</v>
@@ -2866,7 +2866,7 @@
     </row>
     <row r="7" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B7" s="5">
         <v>2</v>
@@ -2877,7 +2877,7 @@
     </row>
     <row r="8" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -2888,7 +2888,7 @@
     </row>
     <row r="9" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B9" s="5">
         <v>0</v>
@@ -2899,7 +2899,7 @@
     </row>
     <row r="10" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B10" s="5">
         <v>0</v>
@@ -2910,7 +2910,7 @@
     </row>
     <row r="11" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B11" s="5">
         <v>0</v>
@@ -2921,7 +2921,7 @@
     </row>
     <row r="12" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B12" s="5">
         <v>0</v>
@@ -2932,10 +2932,10 @@
     </row>
     <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
+        <v>525</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>526</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>527</v>
       </c>
       <c r="C13" t="s">
         <v>183</v>
@@ -2959,7 +2959,7 @@
         <v>253</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>627</v>
+        <v>619</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -3024,7 +3024,7 @@
     </row>
     <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3032,7 +3032,7 @@
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -3040,7 +3040,7 @@
     </row>
     <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -3048,7 +3048,7 @@
     </row>
     <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -3056,7 +3056,7 @@
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -3064,7 +3064,7 @@
     </row>
     <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -3072,7 +3072,7 @@
     </row>
     <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -3080,7 +3080,7 @@
     </row>
     <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -3088,7 +3088,7 @@
     </row>
     <row r="10" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -3096,7 +3096,7 @@
     </row>
     <row r="11" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -3104,7 +3104,7 @@
     </row>
     <row r="12" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -3129,7 +3129,7 @@
         <v>253</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>626</v>
+        <v>618</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -3173,8 +3173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0908D19-61E8-460E-9695-3943D19E115C}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="105" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A4" zoomScale="105" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="58.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3422,7 +3422,7 @@
         <v>253</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -3599,7 +3599,7 @@
         <v>253</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -3731,7 +3731,7 @@
         <v>253</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -3908,7 +3908,7 @@
         <v>253</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -3919,7 +3919,7 @@
         <v>183</v>
       </c>
       <c r="D17" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -4003,7 +4003,7 @@
         <v>440</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -4024,7 +4024,7 @@
         <v>253</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -4229,7 +4229,7 @@
         <v>24</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -4363,7 +4363,7 @@
         <v>253</v>
       </c>
       <c r="B36" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -4408,8 +4408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F776689-DE3B-468A-9224-18F5400CC444}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4428,7 +4428,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>652</v>
+        <v>642</v>
       </c>
       <c r="B2" s="5">
         <v>387</v>
@@ -4436,7 +4436,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>651</v>
+        <v>641</v>
       </c>
       <c r="B3" s="5">
         <v>143</v>
@@ -4444,7 +4444,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>650</v>
+        <v>640</v>
       </c>
       <c r="B4" s="5">
         <v>1</v>
@@ -4452,7 +4452,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>657</v>
+        <v>647</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>
@@ -4492,7 +4492,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>653</v>
+        <v>643</v>
       </c>
       <c r="B10" s="5">
         <v>1082</v>
@@ -4500,7 +4500,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>654</v>
+        <v>644</v>
       </c>
       <c r="B11" s="5">
         <v>329</v>
@@ -4508,7 +4508,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>655</v>
+        <v>645</v>
       </c>
       <c r="B12" s="5">
         <v>15</v>
@@ -4516,7 +4516,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>656</v>
+        <v>646</v>
       </c>
       <c r="B13" s="5">
         <v>1</v>
@@ -4668,7 +4668,7 @@
         <v>253</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>493</v>
+        <v>669</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -4737,7 +4737,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>91</v>
@@ -4875,7 +4875,7 @@
         <v>253</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -5007,7 +5007,7 @@
         <v>253</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -5182,7 +5182,7 @@
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>146</v>
@@ -5193,7 +5193,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>291</v>
@@ -5356,7 +5356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{869E4568-D908-477D-923D-F4116B90EDC7}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -5376,7 +5376,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>675</v>
+        <v>665</v>
       </c>
       <c r="B2" s="6">
         <v>59</v>
@@ -5384,7 +5384,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>676</v>
+        <v>666</v>
       </c>
       <c r="B3" s="6">
         <v>30</v>
@@ -5392,7 +5392,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>677</v>
+        <v>667</v>
       </c>
       <c r="B4" s="6">
         <v>9</v>
@@ -5400,7 +5400,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>672</v>
+        <v>662</v>
       </c>
       <c r="B5" s="6">
         <v>23</v>
@@ -5408,7 +5408,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>673</v>
+        <v>663</v>
       </c>
       <c r="B6" s="6">
         <v>13</v>
@@ -5416,7 +5416,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>674</v>
+        <v>664</v>
       </c>
       <c r="B7" s="6">
         <v>2</v>
@@ -5992,206 +5992,206 @@
     </row>
     <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>534</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>535</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>536</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B3" s="6">
         <v>45017</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
+        <v>539</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>540</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>541</v>
-      </c>
       <c r="C6" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
+        <v>541</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>542</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>543</v>
-      </c>
       <c r="C7" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
+        <v>543</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>544</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>545</v>
-      </c>
       <c r="C8" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
+        <v>545</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>546</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>547</v>
-      </c>
       <c r="C9" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
+        <v>548</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>549</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>550</v>
-      </c>
       <c r="C11" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B14" s="6">
         <v>1500</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B15" s="6">
         <v>1500</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
+        <v>554</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>555</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>556</v>
-      </c>
       <c r="C16" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
+        <v>556</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>557</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>558</v>
-      </c>
       <c r="C17" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
+        <v>558</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>559</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>560</v>
-      </c>
       <c r="C18" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
+        <v>561</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>562</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>563</v>
-      </c>
       <c r="C20" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
   </sheetData>
@@ -6409,7 +6409,7 @@
         <v>253</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -6726,7 +6726,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>664</v>
+        <v>654</v>
       </c>
       <c r="B2" s="5">
         <v>226</v>
@@ -6734,7 +6734,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>663</v>
+        <v>653</v>
       </c>
       <c r="B3" s="5">
         <v>104</v>
@@ -6742,7 +6742,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>659</v>
+        <v>649</v>
       </c>
       <c r="B4" s="5">
         <v>93</v>
@@ -6758,7 +6758,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>660</v>
+        <v>650</v>
       </c>
       <c r="B6" s="5">
         <v>3</v>
@@ -6766,7 +6766,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>661</v>
+        <v>651</v>
       </c>
       <c r="B7" s="5">
         <v>127</v>
@@ -6774,7 +6774,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>662</v>
+        <v>652</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -6814,7 +6814,7 @@
         <v>253</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>658</v>
+        <v>648</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -6849,12 +6849,12 @@
         <v>183</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>287</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
   </sheetData>
@@ -7397,10 +7397,10 @@
     </row>
     <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>572</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>573</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>574</v>
       </c>
       <c r="C2" t="s">
         <v>183</v>
@@ -7408,10 +7408,10 @@
     </row>
     <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C3" t="s">
         <v>183</v>
@@ -7419,10 +7419,10 @@
     </row>
     <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C4" t="s">
         <v>183</v>
@@ -7430,10 +7430,10 @@
     </row>
     <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C5" t="s">
         <v>183</v>
@@ -7441,10 +7441,10 @@
     </row>
     <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
+        <v>586</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>587</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>588</v>
       </c>
       <c r="C6" t="s">
         <v>183</v>
@@ -7452,57 +7452,57 @@
     </row>
     <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
+        <v>577</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>578</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>579</v>
-      </c>
       <c r="C7" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C8" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C9" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C10" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C11" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
   </sheetData>
@@ -7583,7 +7583,7 @@
         <v>253</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -8241,7 +8241,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8264,87 +8264,90 @@
     </row>
     <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>598</v>
+        <v>668</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>649</v>
+        <v>639</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>517</v>
       </c>
     </row>
   </sheetData>
@@ -8377,7 +8380,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>667</v>
+        <v>657</v>
       </c>
       <c r="B2">
         <v>36</v>
@@ -8385,7 +8388,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>666</v>
+        <v>656</v>
       </c>
       <c r="B3">
         <v>34</v>
@@ -8393,7 +8396,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>668</v>
+        <v>658</v>
       </c>
       <c r="B4">
         <v>31</v>
@@ -8401,7 +8404,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B5">
         <v>356</v>
@@ -8409,7 +8412,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>669</v>
+        <v>659</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -8417,7 +8420,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>670</v>
+        <v>660</v>
       </c>
       <c r="B7">
         <v>36</v>
@@ -8425,7 +8428,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>671</v>
+        <v>661</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -8433,7 +8436,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B9">
         <v>31</v>
@@ -8441,7 +8444,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -8465,7 +8468,7 @@
         <v>253</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>665</v>
+        <v>655</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -8700,7 +8703,7 @@
         <v>253</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -8768,7 +8771,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>628</v>
+        <v>620</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -8776,7 +8779,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>629</v>
+        <v>621</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -8784,7 +8787,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>630</v>
+        <v>622</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -8792,7 +8795,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>631</v>
+        <v>623</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -8800,7 +8803,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>633</v>
+        <v>625</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -8808,7 +8811,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>632</v>
+        <v>624</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -8816,7 +8819,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>634</v>
+        <v>626</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -8824,7 +8827,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>635</v>
+        <v>627</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -8832,7 +8835,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>636</v>
+        <v>628</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -8840,7 +8843,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>637</v>
+        <v>629</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -8848,7 +8851,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>638</v>
+        <v>630</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -8856,7 +8859,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>639</v>
+        <v>631</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -8864,7 +8867,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>640</v>
+        <v>632</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -8872,7 +8875,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>641</v>
+        <v>633</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -8880,7 +8883,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>642</v>
+        <v>634</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -8888,7 +8891,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>643</v>
+        <v>635</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -8896,7 +8899,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>644</v>
+        <v>636</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -8904,7 +8907,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>645</v>
+        <v>637</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -8912,7 +8915,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>646</v>
+        <v>638</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -8950,7 +8953,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8969,7 +8972,7 @@
     </row>
     <row r="2" spans="1:2" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>608</v>
+        <v>671</v>
       </c>
       <c r="B2" s="5">
         <v>3338</v>
@@ -8977,7 +8980,7 @@
     </row>
     <row r="3" spans="1:2" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>609</v>
+        <v>670</v>
       </c>
       <c r="B3" s="13">
         <v>1038</v>
@@ -8988,7 +8991,7 @@
         <v>259</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -9002,7 +9005,7 @@
         <v>253</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>624</v>
+        <v>616</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -9047,7 +9050,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9066,15 +9069,15 @@
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>647</v>
+        <v>672</v>
       </c>
       <c r="B2" s="13">
         <v>2502</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>648</v>
+        <v>673</v>
       </c>
       <c r="B3" s="5">
         <v>851</v>
@@ -9085,7 +9088,7 @@
         <v>259</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -9099,7 +9102,7 @@
         <v>253</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>623</v>
+        <v>615</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -9144,7 +9147,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9163,7 +9166,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>610</v>
+        <v>674</v>
       </c>
       <c r="B2" s="5">
         <v>401</v>
@@ -9171,7 +9174,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>611</v>
+        <v>675</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
@@ -9179,7 +9182,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>612</v>
+        <v>676</v>
       </c>
       <c r="B4" s="5">
         <v>145</v>
@@ -9187,7 +9190,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>613</v>
+        <v>677</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>
@@ -9198,7 +9201,7 @@
         <v>259</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -9211,7 +9214,7 @@
         <v>253</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>622</v>
+        <v>614</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
worked on word2vec document retrieval
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDS_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDS_2020_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\irpa_main\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D58973C-7844-44AC-B0B7-10399FFDCCA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C214895-07A6-4C1D-A73C-F3706FCFF42F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="23" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <sheet name="Freshman Profile_Class Rank" sheetId="18" r:id="rId21"/>
     <sheet name="Transfer Admission_General" sheetId="5" r:id="rId22"/>
     <sheet name="Transfer Admission_Statistic" sheetId="17" r:id="rId23"/>
-    <sheet name="Academic Offering Policy" sheetId="27" r:id="rId24"/>
+    <sheet name="Academic Offering and Policy" sheetId="27" r:id="rId24"/>
     <sheet name="Student Life_Categories" sheetId="7" r:id="rId25"/>
     <sheet name="Student Life_Offered" sheetId="8" r:id="rId26"/>
     <sheet name="Annual Expense" sheetId="35" r:id="rId27"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1374" uniqueCount="678">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1375" uniqueCount="679">
   <si>
     <t>Answer</t>
   </si>
@@ -1932,9 +1932,6 @@
     <t xml:space="preserve">The number of first-time, first-year [gender] freshmen who applied to Rose-Hulman is &lt;value&gt; </t>
   </si>
   <si>
-    <t>Rose-Hulman have a policu of placing student on the waiting list. The number of qualified applicants offered a place on waiting list is 119, the number of accepting a place on the waiting list is 43, the number of wait-listed students admitted 14</t>
-  </si>
-  <si>
     <t>The number of [^subject] units recommended to be taken by students during high school for admission to Rose-Hulman  is &lt;value&gt;</t>
   </si>
   <si>
@@ -2113,6 +2110,12 @@
   </si>
   <si>
     <t>Total part-time, first-time, first-year (freshman) female students who enrolled</t>
+  </si>
+  <si>
+    <t>Special study programs offered at Rose-Hulman, and disciplinary areas students are required to complete coursework in</t>
+  </si>
+  <si>
+    <t>Rose-Hulman have a policy of placing student on the waiting list. The number of qualified applicants offered a place on waiting list is 119, the number of accepting a place on the waiting list is 43, the number of wait-listed students admitted 14</t>
   </si>
 </sst>
 </file>
@@ -2494,7 +2497,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2712,8 +2715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3551768-8BC9-4E69-8C86-830DF8B3DA69}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2739,7 +2742,7 @@
         <v>606</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>617</v>
+        <v>678</v>
       </c>
       <c r="C2" t="s">
         <v>183</v>
@@ -2787,7 +2790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5DC138E-AAA1-4452-BC05-6992F74BED09}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="74" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="74" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -2959,7 +2962,7 @@
         <v>253</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -3129,7 +3132,7 @@
         <v>253</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -4428,7 +4431,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B2" s="5">
         <v>387</v>
@@ -4436,7 +4439,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B3" s="5">
         <v>143</v>
@@ -4444,7 +4447,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B4" s="5">
         <v>1</v>
@@ -4452,7 +4455,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>
@@ -4492,7 +4495,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B10" s="5">
         <v>1082</v>
@@ -4500,7 +4503,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B11" s="5">
         <v>329</v>
@@ -4508,7 +4511,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B12" s="5">
         <v>15</v>
@@ -4516,7 +4519,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B13" s="5">
         <v>1</v>
@@ -4668,7 +4671,7 @@
         <v>253</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -5357,7 +5360,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5376,7 +5379,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B2" s="6">
         <v>59</v>
@@ -5384,7 +5387,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B3" s="6">
         <v>30</v>
@@ -5392,7 +5395,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B4" s="6">
         <v>9</v>
@@ -5400,7 +5403,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B5" s="6">
         <v>23</v>
@@ -5408,7 +5411,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B6" s="6">
         <v>13</v>
@@ -5416,7 +5419,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B7" s="6">
         <v>2</v>
@@ -5484,8 +5487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40ABA4F2-212D-4CBD-893A-EB2683BB9A32}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5536,11 +5539,13 @@
         <v>257</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="B5"/>
+      <c r="B5" s="5" t="s">
+        <v>677</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -6726,7 +6731,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B2" s="5">
         <v>226</v>
@@ -6734,7 +6739,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B3" s="5">
         <v>104</v>
@@ -6742,7 +6747,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B4" s="5">
         <v>93</v>
@@ -6758,7 +6763,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B6" s="5">
         <v>3</v>
@@ -6766,7 +6771,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B7" s="5">
         <v>127</v>
@@ -6774,7 +6779,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -6814,7 +6819,7 @@
         <v>253</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -8341,10 +8346,10 @@
     </row>
     <row r="9" spans="1:3" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>517</v>
@@ -8380,7 +8385,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B2">
         <v>36</v>
@@ -8388,7 +8393,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B3">
         <v>34</v>
@@ -8396,7 +8401,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B4">
         <v>31</v>
@@ -8412,7 +8417,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -8420,7 +8425,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B7">
         <v>36</v>
@@ -8428,7 +8433,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -8468,7 +8473,7 @@
         <v>253</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -8771,7 +8776,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -8779,7 +8784,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -8787,7 +8792,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -8795,7 +8800,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -8803,7 +8808,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -8811,7 +8816,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -8819,7 +8824,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -8827,7 +8832,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -8835,7 +8840,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -8843,7 +8848,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -8851,7 +8856,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -8859,7 +8864,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -8867,7 +8872,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -8875,7 +8880,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -8883,7 +8888,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -8891,7 +8896,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -8899,7 +8904,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -8907,7 +8912,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -8915,7 +8920,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -8972,7 +8977,7 @@
     </row>
     <row r="2" spans="1:2" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B2" s="5">
         <v>3338</v>
@@ -8980,7 +8985,7 @@
     </row>
     <row r="3" spans="1:2" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B3" s="13">
         <v>1038</v>
@@ -9069,7 +9074,7 @@
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B2" s="13">
         <v>2502</v>
@@ -9077,7 +9082,7 @@
     </row>
     <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B3" s="5">
         <v>851</v>
@@ -9166,7 +9171,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B2" s="5">
         <v>401</v>
@@ -9174,7 +9179,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
@@ -9182,7 +9187,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B4" s="5">
         <v>145</v>
@@ -9190,7 +9195,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>

</xml_diff>

<commit_message>
added slots and action for statistics
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDS_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDS_2020_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\irpa_main\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0DA0AD-9F30-4190-8484-4F53B9119915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31D016F-1B8F-4E90-B166-8D2F9A2293F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="19" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="23" r:id="rId1"/>
@@ -35,8 +35,8 @@
     <sheet name="Freshman Profile_Percentile" sheetId="2" r:id="rId20"/>
     <sheet name="Freshman Profile_GPA" sheetId="4" r:id="rId21"/>
     <sheet name="Freshman Profile_Class Rank" sheetId="18" r:id="rId22"/>
-    <sheet name="Transfer Admission_General" sheetId="5" r:id="rId23"/>
-    <sheet name="Transfer Admission_Statistic" sheetId="17" r:id="rId24"/>
+    <sheet name="Transfer Admission_Statistic" sheetId="17" r:id="rId23"/>
+    <sheet name="Transfer Admission_General" sheetId="5" r:id="rId24"/>
     <sheet name="Academic Offering and Policy" sheetId="27" r:id="rId25"/>
     <sheet name="Student Life_Categories" sheetId="7" r:id="rId26"/>
     <sheet name="Student Life_Offered" sheetId="8" r:id="rId27"/>
@@ -3775,7 +3775,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="B8" numberStoredAsText="1"/>
   </ignoredErrors>
@@ -4087,7 +4087,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4200,7 +4200,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5190,6 +5190,134 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{869E4568-D908-477D-923D-F4116B90EDC7}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="61.44140625" customWidth="1"/>
+    <col min="2" max="2" width="59" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>655</v>
+      </c>
+      <c r="B2" s="6">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>656</v>
+      </c>
+      <c r="B3" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>657</v>
+      </c>
+      <c r="B4" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>652</v>
+      </c>
+      <c r="B5" s="6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>653</v>
+      </c>
+      <c r="B6" s="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>654</v>
+      </c>
+      <c r="B7" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="B8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B10" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B12" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B13" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B14" t="s">
+        <v>221</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75CD6236-1D5E-43C4-8447-268AAEF1A0C5}">
   <dimension ref="A1:C28"/>
   <sheetViews>
@@ -5486,134 +5614,6 @@
         <v>258</v>
       </c>
       <c r="B28" t="s">
-        <v>221</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{869E4568-D908-477D-923D-F4116B90EDC7}">
-  <dimension ref="A1:B14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="61.44140625" customWidth="1"/>
-    <col min="2" max="2" width="59" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>655</v>
-      </c>
-      <c r="B2" s="6">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>656</v>
-      </c>
-      <c r="B3" s="6">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>657</v>
-      </c>
-      <c r="B4" s="6">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>652</v>
-      </c>
-      <c r="B5" s="6">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>653</v>
-      </c>
-      <c r="B6" s="6">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>654</v>
-      </c>
-      <c r="B7" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="B8" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="B10" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="B11" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="B12" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="B13" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="B14" t="s">
         <v>221</v>
       </c>
     </row>
@@ -6340,7 +6340,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6598,7 +6598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354727B8-DF4A-4CB3-BBB4-023F92A30B71}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -6754,7 +6754,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8939,7 +8939,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9143,7 +9143,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added call to update for unanswered question, finalized client input data and fixed training data
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDS_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDS_2020_2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\irpa_main\rhit_IRPA_2023\NewCDSDataFromClient\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\RHIT_IRPA_@\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1E80ED-9E72-418F-AD77-F1C2A8497DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B637AC-02DE-4D46-9238-D236CF824FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="23" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="23" r:id="rId1"/>
@@ -19,43 +19,44 @@
     <sheet name="Enrollment_Race First time year" sheetId="13" r:id="rId4"/>
     <sheet name="Cohort_2014" sheetId="10" r:id="rId5"/>
     <sheet name="Cohort_Retention 2019" sheetId="41" r:id="rId6"/>
-    <sheet name="Basis For Selection" sheetId="1" r:id="rId7"/>
-    <sheet name="Admission_Applied" sheetId="40" r:id="rId8"/>
-    <sheet name="Admission_Admitted" sheetId="39" r:id="rId9"/>
-    <sheet name="Admission_Enrolled" sheetId="37" r:id="rId10"/>
-    <sheet name="Admission_Condition" sheetId="38" r:id="rId11"/>
-    <sheet name="Admission_High School Required" sheetId="29" r:id="rId12"/>
-    <sheet name="Admission_High School Recommend" sheetId="28" r:id="rId13"/>
-    <sheet name="Admission_Policies" sheetId="9" r:id="rId14"/>
-    <sheet name="Freshman Profile_SAT comp range" sheetId="14" r:id="rId15"/>
-    <sheet name="Freshman Profile_SAT sub range " sheetId="3" r:id="rId16"/>
-    <sheet name="Freshman Profile_ACT comp range" sheetId="15" r:id="rId17"/>
-    <sheet name="Freshman Profile_ACT sub range" sheetId="11" r:id="rId18"/>
-    <sheet name="Freshman Profile_Submit" sheetId="34" r:id="rId19"/>
-    <sheet name="Freshman Profile_Percentile" sheetId="2" r:id="rId20"/>
-    <sheet name="Freshman Profile_GPA" sheetId="4" r:id="rId21"/>
-    <sheet name="Freshman Profile_Class Rank" sheetId="18" r:id="rId22"/>
-    <sheet name="Transfer Admission_Statistic" sheetId="17" r:id="rId23"/>
-    <sheet name="Transfer Admission_General" sheetId="5" r:id="rId24"/>
-    <sheet name="Academic Offering and Policy" sheetId="27" r:id="rId25"/>
-    <sheet name="Student Life_CategoryFreshman" sheetId="7" r:id="rId26"/>
-    <sheet name="Student Life_CategoryUndergrad" sheetId="44" r:id="rId27"/>
-    <sheet name="Student Life_Offered" sheetId="8" r:id="rId28"/>
-    <sheet name="Annual Expense_General" sheetId="35" r:id="rId29"/>
-    <sheet name="Annual Expense_CommuterResident" sheetId="43" r:id="rId30"/>
-    <sheet name="Annual Expense_Policy" sheetId="42" r:id="rId31"/>
-    <sheet name="Financial Aid_Awarded" sheetId="19" r:id="rId32"/>
-    <sheet name="Financial Aid_Awarded Freshman" sheetId="20" r:id="rId33"/>
-    <sheet name="Financial Aid_Awarded Undergrad" sheetId="21" r:id="rId34"/>
-    <sheet name="Financial Aid_Awarded Part-Time" sheetId="22" r:id="rId35"/>
-    <sheet name="Financial Aid_Type" sheetId="36" r:id="rId36"/>
-    <sheet name="Faculty And Class Size_Gender" sheetId="24" r:id="rId37"/>
-    <sheet name="Faculty And Class Size_Degree" sheetId="25" r:id="rId38"/>
-    <sheet name="Faculty And Class Size_Ra" sheetId="30" r:id="rId39"/>
-    <sheet name="Faculty And Class Size_Other" sheetId="26" r:id="rId40"/>
-    <sheet name="Faculty And Class Size_Section" sheetId="31" r:id="rId41"/>
-    <sheet name="Faculty And Class Size_Subsec" sheetId="32" r:id="rId42"/>
-    <sheet name="Degree Conferred" sheetId="33" r:id="rId43"/>
+    <sheet name="Admission_Applied" sheetId="40" r:id="rId7"/>
+    <sheet name="Admission_Admitted" sheetId="39" r:id="rId8"/>
+    <sheet name="Admission_Enrolled" sheetId="37" r:id="rId9"/>
+    <sheet name="Admission_Condition" sheetId="38" r:id="rId10"/>
+    <sheet name="Admission_High School Required" sheetId="29" r:id="rId11"/>
+    <sheet name="Admission_High School Recommend" sheetId="28" r:id="rId12"/>
+    <sheet name="Admission_Policies" sheetId="9" r:id="rId13"/>
+    <sheet name="Basis For Selection" sheetId="1" r:id="rId14"/>
+    <sheet name="SAT ACT Policy" sheetId="45" r:id="rId15"/>
+    <sheet name="Freshman Profile_SAT comp range" sheetId="14" r:id="rId16"/>
+    <sheet name="Freshman Profile_SAT sub range " sheetId="3" r:id="rId17"/>
+    <sheet name="Freshman Profile_ACT comp range" sheetId="15" r:id="rId18"/>
+    <sheet name="Freshman Profile_ACT sub range" sheetId="11" r:id="rId19"/>
+    <sheet name="Freshman Profile_Submit" sheetId="34" r:id="rId20"/>
+    <sheet name="Freshman Profile_Percentile" sheetId="2" r:id="rId21"/>
+    <sheet name="Freshman Profile_GPA" sheetId="4" r:id="rId22"/>
+    <sheet name="Freshman Profile_Class Rank" sheetId="18" r:id="rId23"/>
+    <sheet name="Transfer Admission_Statistic" sheetId="17" r:id="rId24"/>
+    <sheet name="Transfer Admission_General" sheetId="5" r:id="rId25"/>
+    <sheet name="Academic Offering and Policy" sheetId="27" r:id="rId26"/>
+    <sheet name="Student Life_CategoryFreshman" sheetId="7" r:id="rId27"/>
+    <sheet name="Student Life_CategoryUndergrad" sheetId="44" r:id="rId28"/>
+    <sheet name="Student Life_Offered" sheetId="8" r:id="rId29"/>
+    <sheet name="Annual Expense_General" sheetId="35" r:id="rId30"/>
+    <sheet name="Annual Expense_CommuterResident" sheetId="43" r:id="rId31"/>
+    <sheet name="Annual Expense_Policy" sheetId="42" r:id="rId32"/>
+    <sheet name="Financial Aid_Awarded" sheetId="19" r:id="rId33"/>
+    <sheet name="Financial Aid_Awarded Freshman" sheetId="20" r:id="rId34"/>
+    <sheet name="Financial Aid_Awarded Undergrad" sheetId="21" r:id="rId35"/>
+    <sheet name="Financial Aid_Awarded Part-Time" sheetId="22" r:id="rId36"/>
+    <sheet name="Financial Aid_Type" sheetId="36" r:id="rId37"/>
+    <sheet name="Faculty And Class Size_Gender" sheetId="24" r:id="rId38"/>
+    <sheet name="Faculty And Class Size_Degree" sheetId="25" r:id="rId39"/>
+    <sheet name="Faculty And Class Size_Ra" sheetId="30" r:id="rId40"/>
+    <sheet name="Faculty And Class Size_Other" sheetId="26" r:id="rId41"/>
+    <sheet name="Faculty And Class Size_Section" sheetId="31" r:id="rId42"/>
+    <sheet name="Faculty And Class Size_Subsec" sheetId="32" r:id="rId43"/>
+    <sheet name="Degree Conferred" sheetId="33" r:id="rId44"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -78,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="741">
   <si>
     <t>Answer</t>
   </si>
@@ -1702,9 +1703,6 @@
     <t xml:space="preserve">Priority date for filing required financial aid forms: March 10. </t>
   </si>
   <si>
-    <t>what is the notificationdate for first-year students apply for financial-aid ?</t>
-  </si>
-  <si>
     <t>Students notified on or about (date): January 15 (early action) - March 15 (regular decision). Students notified on a rolling basis: No</t>
   </si>
   <si>
@@ -2238,6 +2236,79 @@
   </si>
   <si>
     <t>Percentage of full-time and part-time first-year freshman students who are from out of state, who joined fraternities, or sororities, live in college-owned housing, live off campus, or are 25 years or older. The average age of full-time and part-time freshman students</t>
+  </si>
+  <si>
+    <t>Same as the previous description, but for part-time degree-seeking undergraduate students.</t>
+  </si>
+  <si>
+    <t>Same as the previous description, but for full-time degree-seeking undergraduate students.</t>
+  </si>
+  <si>
+    <t>what is the notification date for first-year students apply for financial-aid ?</t>
+  </si>
+  <si>
+    <t>Rose-Hulman's policy regarding institutional scholarship and grant aid for undergraduate degree-seeking nonresident
+aliens. Financial aid forms required to be submitted by domestic or non-resident alien financial aid applicants. Deadline for financial applications. Priority date, Reply date and notification date for financial aid. The type of financial aid loan and scholarship or grants available to undergraduate students. The criteria used in awarding institutional aid.</t>
+  </si>
+  <si>
+    <t>The total number of full-time instructional faculty in general, or by gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The total number of full-time or part-time(or both) instructional faculty whose highest degree is a doctorate, or master's or bachelor, or whose highest degree is unknown. </t>
+  </si>
+  <si>
+    <t>the total number of full-time or part-time(or both) instructional faculty who are members of minority groups, or nonresident aliens.</t>
+  </si>
+  <si>
+    <t>The total number of full-time and part-time instructional faculty in stand-alone graduate/professional programs in which faculty teach only graduate level students.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Majors offered by Rose-Hulman. The percentage of degrees conferred/awarded for the following disciplinary areas: engineering, biological/life sciences, mathematics and statistics, interdisciplinary studies, physical sciences, and social sciences. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of class subsections with number of students (xor {between [^number] and [^number]} {[^range] [^number]}) is &lt;value&gt; </t>
+  </si>
+  <si>
+    <t>Number of class subsections with a number of students within an arbitrary number or more than that number or in an arbitrary range.</t>
+  </si>
+  <si>
+    <t>The average class size at Rose-Hulman. The number of class sections with a number of students more than or within a arbitrary number or in a arbitrary range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of class sections with number of students (xor {between [^number] and [^number]} {[^range] [^number]}) is &lt;value&gt; </t>
+  </si>
+  <si>
+    <t>Does Rose-Hulman make use of ACT and SAT or ACT and SAT subject test in admission decisions for first-time first-year degree-seeking applicants? If yes, please state how the tests will be used.</t>
+  </si>
+  <si>
+    <t>Does Rose-Hulman use ACT or SAT test scores for academic advising?</t>
+  </si>
+  <si>
+    <t>What date by which SAT or ACT scores must be received for fall term admission?</t>
+  </si>
+  <si>
+    <t>Does Rose-Hulman use the following tests for placement: SAT, ACT, SAT subject test, AP test, CLEP test, and institutional exam?</t>
+  </si>
+  <si>
+    <t>Rose-Hulman does not use SAT or ACT test scores for academic advising.</t>
+  </si>
+  <si>
+    <t>ACT and SAT scores are considered in admission decisions if submitted. ACT and SAT scores without essay component are accepted.</t>
+  </si>
+  <si>
+    <t>The latest date by which SAT and ACT score must be received for fall term admission is February 1st</t>
+  </si>
+  <si>
+    <t>Test scores are optional this year due to COVID-19</t>
+  </si>
+  <si>
+    <t>Rose-Hulman uses AP and institutional exams for placement.</t>
+  </si>
+  <si>
+    <t>Rose-Hulman's SAT and ACT policies. If Rose-Hulman makes use of ACT and SAT or ACT and SAT subject test in admission decisions for first-time first-year degree-seeking applicants. If Rose-Hulman uses ACT or SAT test scores for academic advising. The latest date SAT and ACT scores must be received for fall term admission. ACT and SAT test policies -  if tests are optional are not. The tests Rose-Hulman uses for placement.</t>
+  </si>
+  <si>
+    <t>What are Rose-Hulman's SAT and ACT test policies – Are tests recommended for some students, or if tests are not required to be submitted for some students or are they optional?</t>
   </si>
 </sst>
 </file>
@@ -2796,7 +2867,7 @@
         <v>236</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -2837,122 +2908,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7A8EC24-050E-45A2-BA78-4310BE4389C1}">
-  <dimension ref="A1:B12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="78.88671875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="60.33203125" style="5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>633</v>
-      </c>
-      <c r="B2" s="5">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>634</v>
-      </c>
-      <c r="B3" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>635</v>
-      </c>
-      <c r="B4" s="5">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>636</v>
-      </c>
-      <c r="B5" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3551768-8BC9-4E69-8C86-830DF8B3DA69}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -2980,10 +2935,10 @@
     </row>
     <row r="2" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C2" t="s">
         <v>165</v>
@@ -2991,10 +2946,10 @@
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C3" t="s">
         <v>165</v>
@@ -3002,10 +2957,10 @@
     </row>
     <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
+        <v>569</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>570</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>571</v>
       </c>
       <c r="C4" t="s">
         <v>165</v>
@@ -3013,10 +2968,10 @@
     </row>
     <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>572</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>573</v>
       </c>
       <c r="C5" t="s">
         <v>165</v>
@@ -3027,7 +2982,7 @@
         <v>241</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
@@ -3035,7 +2990,7 @@
         <v>236</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
   </sheetData>
@@ -3043,7 +2998,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5DC138E-AAA1-4452-BC05-6992F74BED09}">
   <dimension ref="A1:C20"/>
   <sheetViews>
@@ -3214,7 +3169,7 @@
         <v>236</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -3222,7 +3177,7 @@
         <v>235</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -3263,7 +3218,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B50A1A77-FCFF-4BA2-80DC-49E66C3D11B3}">
   <dimension ref="A1:B19"/>
   <sheetViews>
@@ -3386,7 +3341,7 @@
         <v>236</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -3394,7 +3349,7 @@
         <v>235</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -3434,12 +3389,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0908D19-61E8-460E-9695-3943D19E115C}">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScale="105" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A13" sqref="A13:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="58.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3592,7 +3547,211 @@
         <v>236</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>662</v>
+        <v>661</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" zoomScale="88" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="81.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.5546875" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="116.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>412</v>
       </c>
     </row>
   </sheetData>
@@ -3602,11 +3761,95 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99A416E3-1A6E-44C4-BE5C-83B841156A96}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="61" style="5" customWidth="1"/>
+    <col min="2" max="2" width="40.44140625" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>730</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>731</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>732</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>740</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>733</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>739</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CF2A7F2-CEC5-4907-876C-DED9EAEEDD17}">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3684,7 +3927,7 @@
         <v>236</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -3732,12 +3975,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C307D05E-B833-4D75-9855-8E27A1B5E2C9}">
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView zoomScale="84" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3863,7 +4106,7 @@
         <v>236</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -3915,12 +4158,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3682DD5-C270-454D-A655-BE30A9BBE78A}">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3998,7 +4241,7 @@
         <v>236</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -4046,7 +4289,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20057133-7837-4203-86B9-F46D32350538}">
   <dimension ref="A1:D20"/>
   <sheetViews>
@@ -4177,7 +4420,7 @@
         <v>236</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -4220,122 +4463,6 @@
         <v>240</v>
       </c>
       <c r="B20" t="s">
-        <v>203</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{998E6B56-71DD-4A78-89DB-D3F23672C01B}">
-  <dimension ref="A1:B12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="44.33203125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="33.33203125" style="5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>415</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>416</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>413</v>
-      </c>
-      <c r="B4" s="6">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>414</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
-        <v>237</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="B12" s="5" t="s">
         <v>203</v>
       </c>
     </row>
@@ -4369,7 +4496,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B2" s="5">
         <v>387</v>
@@ -4377,7 +4504,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B3" s="5">
         <v>143</v>
@@ -4385,7 +4512,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B4" s="5">
         <v>1</v>
@@ -4393,7 +4520,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>
@@ -4401,7 +4528,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B6" s="5">
         <v>9</v>
@@ -4409,7 +4536,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B7" s="5">
         <v>2</v>
@@ -4417,7 +4544,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -4425,7 +4552,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B9" s="5">
         <v>0</v>
@@ -4433,7 +4560,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B10" s="5">
         <v>1082</v>
@@ -4441,7 +4568,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B11" s="5">
         <v>329</v>
@@ -4449,7 +4576,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B12" s="5">
         <v>15</v>
@@ -4457,7 +4584,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B13" s="5">
         <v>1</v>
@@ -4604,7 +4731,7 @@
         <v>236</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -4612,7 +4739,7 @@
         <v>235</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -4654,6 +4781,122 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{998E6B56-71DD-4A78-89DB-D3F23672C01B}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="44.33203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>413</v>
+      </c>
+      <c r="B4" s="6">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3892E9F-E7EA-42B9-AE4C-1275BBD6A387}">
   <dimension ref="A1:B40"/>
   <sheetViews>
@@ -4946,7 +5189,7 @@
         <v>236</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -4995,7 +5238,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB852AE-A4C7-4284-9FBD-1CEEB9311916}">
   <dimension ref="A1:C22"/>
   <sheetViews>
@@ -5155,7 +5398,7 @@
         <v>236</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -5207,7 +5450,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDBBFCBD-BE53-4EBE-BC28-AF1024B4BD2D}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -5290,7 +5533,7 @@
         <v>236</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -5338,7 +5581,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{869E4568-D908-477D-923D-F4116B90EDC7}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -5363,7 +5606,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B2" s="6">
         <v>59</v>
@@ -5371,7 +5614,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B3" s="6">
         <v>30</v>
@@ -5379,7 +5622,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B4" s="6">
         <v>9</v>
@@ -5387,7 +5630,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B5" s="6">
         <v>23</v>
@@ -5395,7 +5638,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B6" s="6">
         <v>13</v>
@@ -5403,7 +5646,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B7" s="6">
         <v>2</v>
@@ -5422,7 +5665,7 @@
         <v>236</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -5470,7 +5713,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75CD6236-1D5E-43C4-8447-268AAEF1A0C5}">
   <dimension ref="A1:C28"/>
   <sheetViews>
@@ -5520,7 +5763,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>130</v>
@@ -5539,10 +5782,10 @@
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
+        <v>693</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>694</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>695</v>
       </c>
       <c r="C6" t="s">
         <v>165</v>
@@ -5550,10 +5793,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C7" t="s">
         <v>165</v>
@@ -5561,10 +5804,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C8" t="s">
         <v>165</v>
@@ -5572,10 +5815,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C9" t="s">
         <v>165</v>
@@ -5583,7 +5826,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>132</v>
@@ -5594,7 +5837,7 @@
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>133</v>
@@ -5605,10 +5848,10 @@
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C12" t="s">
         <v>165</v>
@@ -5616,7 +5859,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>266</v>
@@ -5649,7 +5892,7 @@
     </row>
     <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>136</v>
@@ -5737,7 +5980,7 @@
         <v>236</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -5777,7 +6020,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40ABA4F2-212D-4CBD-893A-EB2683BB9A32}">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -5838,7 +6081,7 @@
         <v>236</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -5882,7 +6125,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AECD6F-4371-4391-B58E-E510CF964736}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -5913,7 +6156,7 @@
         <v>143</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C2" t="s">
         <v>165</v>
@@ -5924,7 +6167,7 @@
         <v>146</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="C3" t="s">
         <v>165</v>
@@ -5935,7 +6178,7 @@
         <v>147</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="C4" t="s">
         <v>165</v>
@@ -6009,7 +6252,7 @@
         <v>236</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -6049,12 +6292,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD1BC2B9-A383-49AB-870B-3568000F0DBB}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6077,7 +6320,7 @@
         <v>144</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -6085,7 +6328,7 @@
         <v>145</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -6093,7 +6336,7 @@
         <v>148</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
@@ -6149,7 +6392,7 @@
         <v>236</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -6190,7 +6433,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD4CE82-100F-475B-B66F-A9CBAA32385B}">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -6284,7 +6527,7 @@
         <v>236</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -6321,149 +6564,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD284E4D-E296-45CE-8E65-A3C009D67DE2}">
-  <dimension ref="A1:C12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="40.21875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="27.5546875" style="6" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>505</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>506</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>555</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>690</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>556</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>508</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>557</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>673</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>509</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>510</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>511</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>512</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>513</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>514</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>515</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>516</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
-        <v>517</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>554</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="B11" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>678</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6491,7 +6591,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B2" s="5">
         <v>226</v>
@@ -6499,7 +6599,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B3" s="5">
         <v>104</v>
@@ -6507,7 +6607,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B4" s="5">
         <v>93</v>
@@ -6515,7 +6615,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B5" s="5">
         <v>1295</v>
@@ -6523,7 +6623,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B6" s="5">
         <v>3</v>
@@ -6531,7 +6631,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B7" s="5">
         <v>127</v>
@@ -6539,7 +6639,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -6574,7 +6674,7 @@
         <v>236</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -6582,7 +6682,7 @@
         <v>235</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -6632,6 +6732,149 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD284E4D-E296-45CE-8E65-A3C009D67DE2}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="40.21875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="27.5546875" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>505</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>506</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>554</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>689</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>555</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>508</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>556</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>672</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>510</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>512</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>514</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>515</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>516</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>517</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>553</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="B11" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>677</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C81AE8E2-FE18-482C-A19C-560E4F8CFDBF}">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -6656,10 +6899,10 @@
     </row>
     <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>507</v>
@@ -6670,7 +6913,7 @@
         <v>521</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>507</v>
@@ -6681,7 +6924,7 @@
         <v>522</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>507</v>
@@ -6692,7 +6935,7 @@
         <v>523</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>507</v>
@@ -6700,10 +6943,10 @@
     </row>
     <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>507</v>
@@ -6711,10 +6954,10 @@
     </row>
     <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>507</v>
@@ -6725,7 +6968,7 @@
         <v>524</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>507</v>
@@ -6744,7 +6987,7 @@
         <v>236</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
   </sheetData>
@@ -6752,7 +6995,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04C0EB70-B1AD-40A9-9CC0-12B91CFD2E06}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -6780,7 +7023,7 @@
         <v>518</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>507</v>
@@ -6791,7 +7034,7 @@
         <v>519</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>507</v>
@@ -6802,7 +7045,7 @@
         <v>520</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>507</v>
@@ -6821,7 +7064,7 @@
         <v>236</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
   </sheetData>
@@ -6829,12 +7072,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E00C0EE-B5EA-4C5D-A3F6-0409760A68CF}">
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7032,7 +7275,7 @@
         <v>236</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -7040,7 +7283,7 @@
         <v>235</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -7081,12 +7324,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BD85EB1-BDB8-4AEB-99D1-57DF875DFEB5}">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7230,7 +7473,7 @@
     </row>
     <row r="13" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>349</v>
@@ -7296,7 +7539,7 @@
         <v>236</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -7336,12 +7579,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE4F375-28FB-4634-A90F-E29F4CD5ADA1}">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7546,11 +7789,13 @@
         <v>239</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="B19" s="6"/>
+      <c r="B19" s="6" t="s">
+        <v>718</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
@@ -7589,12 +7834,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46EA6128-27F4-4911-A1F0-865B26420EEF}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7799,11 +8044,13 @@
         <v>239</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="B19" s="6"/>
+      <c r="B19" s="6" t="s">
+        <v>717</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
@@ -7842,12 +8089,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B311E26-48F5-445F-A976-490D3902A0D5}">
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7884,7 +8131,7 @@
         <v>536</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C3" t="s">
         <v>165</v>
@@ -7895,7 +8142,7 @@
         <v>537</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C4" t="s">
         <v>165</v>
@@ -7903,7 +8150,7 @@
     </row>
     <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>538</v>
@@ -7914,10 +8161,10 @@
     </row>
     <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
+        <v>547</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>548</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>549</v>
       </c>
       <c r="C6" t="s">
         <v>165</v>
@@ -7925,10 +8172,10 @@
     </row>
     <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
+        <v>719</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>539</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>540</v>
       </c>
       <c r="C7" t="s">
         <v>488</v>
@@ -7936,10 +8183,10 @@
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C8" t="s">
         <v>488</v>
@@ -7947,10 +8194,10 @@
     </row>
     <row r="9" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C9" t="s">
         <v>488</v>
@@ -7958,10 +8205,10 @@
     </row>
     <row r="10" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C10" t="s">
         <v>488</v>
@@ -7969,10 +8216,10 @@
     </row>
     <row r="11" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C11" t="s">
         <v>488</v>
@@ -7986,23 +8233,25 @@
         <v>239</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="B13" s="6"/>
+      <c r="B13" s="6" t="s">
+        <v>720</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C2A9967-94EA-41CF-ACB5-C81483AD239D}">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8059,18 +8308,20 @@
         <v>239</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="B7" s="6"/>
+      <c r="B7" s="6" t="s">
+        <v>721</v>
+      </c>
     </row>
     <row r="8" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>235</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -8110,11 +8361,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2758D6-F888-4498-88A0-7DFBF7091CA2}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -8204,11 +8455,13 @@
         <v>239</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="B11" s="6"/>
+      <c r="B11" s="6" t="s">
+        <v>722</v>
+      </c>
     </row>
     <row r="12" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
@@ -8252,120 +8505,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{680EF845-E97A-4774-A116-33BCEE8AAAAA}">
-  <dimension ref="A1:B12"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="35.44140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="26.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>437</v>
-      </c>
-      <c r="B2">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>438</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>439</v>
-      </c>
-      <c r="B4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>440</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="B6" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="B7" s="6"/>
-    </row>
-    <row r="8" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="B9" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="B10" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="B11" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="B12" t="s">
-        <v>203</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8394,7 +8533,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B2">
         <v>36</v>
@@ -8402,7 +8541,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B3">
         <v>34</v>
@@ -8410,7 +8549,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B4">
         <v>31</v>
@@ -8426,7 +8565,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -8434,7 +8573,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B7">
         <v>36</v>
@@ -8442,7 +8581,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -8477,7 +8616,7 @@
         <v>236</v>
       </c>
       <c r="B12" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -8485,7 +8624,7 @@
         <v>235</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -8534,11 +8673,127 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{680EF845-E97A-4774-A116-33BCEE8AAAAA}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="35.44140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="B2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>438</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>440</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="B6" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B11" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B12" t="s">
+        <v>203</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61ED34DA-E2CB-4859-9A96-48DF7AE0B7A7}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K16:K17"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8592,11 +8847,13 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="B5" s="6"/>
+      <c r="B5" s="6" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -8611,7 +8868,7 @@
         <v>238</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>165</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -8635,12 +8892,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F6BE80-AC56-42ED-87D6-9266FD24F810}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8729,31 +8986,33 @@
         <v>239</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="B11" s="6"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>237</v>
+      <c r="B11" s="6" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>235</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>203</v>
+        <v>729</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>203</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>203</v>
@@ -8761,9 +9020,17 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B16" s="5" t="s">
         <v>203</v>
       </c>
     </row>
@@ -8772,12 +9039,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA74624B-4AE3-43E9-9C9C-696C43DB0CE5}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8851,34 +9118,58 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>237</v>
+      <c r="A9" s="7" t="s">
+        <v>241</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>235</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>203</v>
+        <v>726</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>203</v>
       </c>
     </row>
@@ -8887,12 +9178,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A321CDB-4432-42F8-8542-C3389F944EAE}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8915,10 +9206,10 @@
     </row>
     <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>488</v>
@@ -8929,7 +9220,7 @@
         <v>489</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>488</v>
@@ -8940,7 +9231,7 @@
         <v>490</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>488</v>
@@ -8951,7 +9242,7 @@
         <v>491</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>488</v>
@@ -8962,7 +9253,7 @@
         <v>492</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>488</v>
@@ -8973,7 +9264,7 @@
         <v>493</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>488</v>
@@ -8984,7 +9275,7 @@
         <v>494</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>488</v>
@@ -8992,13 +9283,29 @@
     </row>
     <row r="9" spans="1:3" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>488</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>725</v>
       </c>
     </row>
   </sheetData>
@@ -9185,7 +9492,7 @@
         <v>236</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -9193,7 +9500,7 @@
         <v>235</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -9258,10 +9565,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>638</v>
+      </c>
+      <c r="B2" t="s">
         <v>639</v>
-      </c>
-      <c r="B2" t="s">
-        <v>640</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -9277,7 +9584,7 @@
         <v>236</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
   </sheetData>
@@ -9287,210 +9594,6 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B23"/>
-  <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="88" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="81.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.5546875" style="5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="388.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>412</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44F6232-9681-4454-AEAB-44094C0C14CF}">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -9514,7 +9617,7 @@
     </row>
     <row r="2" spans="1:2" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B2" s="5">
         <v>3338</v>
@@ -9522,7 +9625,7 @@
     </row>
     <row r="3" spans="1:2" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B3" s="13">
         <v>1038</v>
@@ -9533,7 +9636,7 @@
         <v>241</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -9541,7 +9644,7 @@
         <v>236</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -9549,7 +9652,7 @@
         <v>235</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -9589,7 +9692,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13DAF86C-B225-4BA6-A035-2334E730C14A}">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -9613,7 +9716,7 @@
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B2" s="13">
         <v>2502</v>
@@ -9621,7 +9724,7 @@
     </row>
     <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B3" s="5">
         <v>851</v>
@@ -9632,7 +9735,7 @@
         <v>241</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -9640,7 +9743,7 @@
         <v>236</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -9648,7 +9751,7 @@
         <v>235</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -9686,4 +9789,120 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7A8EC24-050E-45A2-BA78-4310BE4389C1}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="78.88671875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="60.33203125" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>632</v>
+      </c>
+      <c r="B2" s="5">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>633</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>634</v>
+      </c>
+      <c r="B4" s="5">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>635</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed bug with unanswered questions
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDS_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDS_2020_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\RHIT_IRPA_@\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA677A6-3874-419A-BDA3-8C965DF12A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9271012-F191-4195-95CB-94520EE491D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="11" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="38" activeTab="41" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="23" r:id="rId1"/>
@@ -1444,9 +1444,6 @@
     <t>What is the number of class sections with 100 or more students?</t>
   </si>
   <si>
-    <t>The average class size at Rose-Hulman Is 16</t>
-  </si>
-  <si>
     <t>What is the number of class subsections with 2 - 9 students?</t>
   </si>
   <si>
@@ -2251,9 +2248,6 @@
     <t>The average class size at Rose-Hulman. The number of class sections with a number of students more than or within a arbitrary number or in a arbitrary range</t>
   </si>
   <si>
-    <t xml:space="preserve">The number of class sections with number of students (xor {between [^number] and [^number]} {[^range] [^number]}) is &lt;value&gt; </t>
-  </si>
-  <si>
     <t>Does Rose-Hulman make use of ACT and SAT or ACT and SAT subject test in admission decisions for first-time first-year degree-seeking applicants? If yes, please state how the tests will be used.</t>
   </si>
   <si>
@@ -2309,6 +2303,12 @@
   </si>
   <si>
     <t>Does Rose-Hulman use the following tests for placement : SAT, ACT, SAT subject test, AP test, CLEP test, and institutional exam?</t>
+  </si>
+  <si>
+    <t>The average class size from CDS at Rose-Hulman Is 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From CDS, the number of class sections with number of students (xor {between [^number] and [^number]} {[^range] [^number]}) is &lt;value&gt;  </t>
   </si>
 </sst>
 </file>
@@ -2867,7 +2867,7 @@
         <v>236</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -2935,10 +2935,10 @@
     </row>
     <row r="2" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C2" t="s">
         <v>165</v>
@@ -2946,10 +2946,10 @@
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C3" t="s">
         <v>165</v>
@@ -2957,10 +2957,10 @@
     </row>
     <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
+        <v>562</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>563</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>564</v>
       </c>
       <c r="C4" t="s">
         <v>165</v>
@@ -2968,10 +2968,10 @@
     </row>
     <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
+        <v>564</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>565</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>566</v>
       </c>
       <c r="C5" t="s">
         <v>165</v>
@@ -2982,7 +2982,7 @@
         <v>241</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
@@ -2990,7 +2990,7 @@
         <v>236</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
   </sheetData>
@@ -3026,7 +3026,7 @@
     </row>
     <row r="2" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B2" s="5">
         <v>4</v>
@@ -3037,7 +3037,7 @@
     </row>
     <row r="3" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B3" s="5">
         <v>4</v>
@@ -3048,7 +3048,7 @@
     </row>
     <row r="4" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B4" s="5">
         <v>3</v>
@@ -3059,7 +3059,7 @@
     </row>
     <row r="5" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B5" s="5">
         <v>3</v>
@@ -3070,7 +3070,7 @@
     </row>
     <row r="6" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B6" s="5">
         <v>0</v>
@@ -3081,7 +3081,7 @@
     </row>
     <row r="7" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B7" s="5">
         <v>2</v>
@@ -3092,7 +3092,7 @@
     </row>
     <row r="8" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -3103,7 +3103,7 @@
     </row>
     <row r="9" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B9" s="5">
         <v>0</v>
@@ -3114,7 +3114,7 @@
     </row>
     <row r="10" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B10" s="5">
         <v>0</v>
@@ -3125,7 +3125,7 @@
     </row>
     <row r="11" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B11" s="5">
         <v>0</v>
@@ -3136,7 +3136,7 @@
     </row>
     <row r="12" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B12" s="5">
         <v>0</v>
@@ -3147,10 +3147,10 @@
     </row>
     <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
+        <v>495</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>496</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>497</v>
       </c>
       <c r="C13" t="s">
         <v>165</v>
@@ -3169,7 +3169,7 @@
         <v>236</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -3177,7 +3177,7 @@
         <v>235</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -3242,7 +3242,7 @@
     </row>
     <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3250,7 +3250,7 @@
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -3258,7 +3258,7 @@
     </row>
     <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -3266,7 +3266,7 @@
     </row>
     <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -3274,7 +3274,7 @@
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -3282,7 +3282,7 @@
     </row>
     <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -3290,7 +3290,7 @@
     </row>
     <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -3298,7 +3298,7 @@
     </row>
     <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -3306,7 +3306,7 @@
     </row>
     <row r="10" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -3314,7 +3314,7 @@
     </row>
     <row r="11" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -3322,7 +3322,7 @@
     </row>
     <row r="12" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -3341,7 +3341,7 @@
         <v>236</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -3349,7 +3349,7 @@
         <v>235</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -3547,7 +3547,7 @@
         <v>236</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -3583,7 +3583,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -3591,7 +3591,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -3599,7 +3599,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3607,7 +3607,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -3615,7 +3615,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3623,7 +3623,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -3631,7 +3631,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3639,7 +3639,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3647,7 +3647,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3655,7 +3655,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3663,7 +3663,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -3671,7 +3671,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3679,7 +3679,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -3687,7 +3687,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3695,7 +3695,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -3703,7 +3703,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -3711,7 +3711,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -3719,7 +3719,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3727,7 +3727,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3743,7 +3743,7 @@
         <v>236</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3764,8 +3764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99A416E3-1A6E-44C4-BE5C-83B841156A96}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3784,42 +3784,42 @@
     </row>
     <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
+        <v>721</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>723</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>725</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -3835,7 +3835,7 @@
         <v>236</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
     </row>
   </sheetData>
@@ -3927,7 +3927,7 @@
         <v>236</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -3935,7 +3935,7 @@
         <v>235</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -4106,7 +4106,7 @@
         <v>236</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -4114,7 +4114,7 @@
         <v>235</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -4241,7 +4241,7 @@
         <v>236</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -4249,7 +4249,7 @@
         <v>235</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -4420,7 +4420,7 @@
         <v>236</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -4428,7 +4428,7 @@
         <v>235</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -4439,7 +4439,7 @@
         <v>165</v>
       </c>
       <c r="D17" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -4496,7 +4496,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B2" s="5">
         <v>387</v>
@@ -4504,7 +4504,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B3" s="5">
         <v>143</v>
@@ -4512,7 +4512,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B4" s="5">
         <v>1</v>
@@ -4520,7 +4520,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>
@@ -4528,7 +4528,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B6" s="5">
         <v>9</v>
@@ -4536,7 +4536,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B7" s="5">
         <v>2</v>
@@ -4544,7 +4544,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -4552,7 +4552,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B9" s="5">
         <v>0</v>
@@ -4560,7 +4560,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B10" s="5">
         <v>1082</v>
@@ -4568,7 +4568,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B11" s="5">
         <v>329</v>
@@ -4576,7 +4576,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B12" s="5">
         <v>15</v>
@@ -4584,7 +4584,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B13" s="5">
         <v>1</v>
@@ -4731,7 +4731,7 @@
         <v>236</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -4739,7 +4739,7 @@
         <v>235</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -4831,7 +4831,7 @@
         <v>414</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -4847,7 +4847,7 @@
         <v>236</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -4855,7 +4855,7 @@
         <v>235</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -5061,7 +5061,7 @@
         <v>24</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -5189,7 +5189,7 @@
         <v>236</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -5197,7 +5197,7 @@
         <v>235</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -5266,7 +5266,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>91</v>
@@ -5398,7 +5398,7 @@
         <v>236</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -5406,7 +5406,7 @@
         <v>235</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -5533,7 +5533,7 @@
         <v>236</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -5541,7 +5541,7 @@
         <v>235</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -5606,7 +5606,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B2" s="6">
         <v>59</v>
@@ -5614,7 +5614,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B3" s="6">
         <v>30</v>
@@ -5622,7 +5622,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B4" s="6">
         <v>9</v>
@@ -5630,7 +5630,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B5" s="6">
         <v>23</v>
@@ -5638,7 +5638,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B6" s="6">
         <v>13</v>
@@ -5646,7 +5646,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B7" s="6">
         <v>2</v>
@@ -5665,7 +5665,7 @@
         <v>236</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -5763,7 +5763,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>130</v>
@@ -5782,10 +5782,10 @@
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
+        <v>684</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>685</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>686</v>
       </c>
       <c r="C6" t="s">
         <v>165</v>
@@ -5793,10 +5793,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C7" t="s">
         <v>165</v>
@@ -5804,10 +5804,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C8" t="s">
         <v>165</v>
@@ -5815,10 +5815,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C9" t="s">
         <v>165</v>
@@ -5826,7 +5826,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>132</v>
@@ -5837,7 +5837,7 @@
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>133</v>
@@ -5848,10 +5848,10 @@
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C12" t="s">
         <v>165</v>
@@ -5859,7 +5859,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>266</v>
@@ -5892,7 +5892,7 @@
     </row>
     <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>136</v>
@@ -5980,7 +5980,7 @@
         <v>236</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -6081,7 +6081,7 @@
         <v>236</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -6156,7 +6156,7 @@
         <v>143</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C2" t="s">
         <v>165</v>
@@ -6167,7 +6167,7 @@
         <v>146</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C3" t="s">
         <v>165</v>
@@ -6178,7 +6178,7 @@
         <v>147</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C4" t="s">
         <v>165</v>
@@ -6252,7 +6252,7 @@
         <v>236</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -6320,7 +6320,7 @@
         <v>144</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -6328,7 +6328,7 @@
         <v>145</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -6336,7 +6336,7 @@
         <v>148</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
@@ -6392,7 +6392,7 @@
         <v>236</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -6527,7 +6527,7 @@
         <v>236</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -6591,7 +6591,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B2" s="5">
         <v>226</v>
@@ -6599,7 +6599,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B3" s="5">
         <v>104</v>
@@ -6607,7 +6607,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B4" s="5">
         <v>93</v>
@@ -6615,7 +6615,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B5" s="5">
         <v>1295</v>
@@ -6623,7 +6623,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B6" s="5">
         <v>3</v>
@@ -6631,7 +6631,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B7" s="5">
         <v>127</v>
@@ -6639,7 +6639,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -6674,7 +6674,7 @@
         <v>236</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -6682,7 +6682,7 @@
         <v>235</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -6722,7 +6722,7 @@
         <v>262</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
   </sheetData>
@@ -6755,101 +6755,101 @@
     </row>
     <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>504</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>505</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>506</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -6865,7 +6865,7 @@
         <v>236</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
   </sheetData>
@@ -6899,79 +6899,79 @@
     </row>
     <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -6987,7 +6987,7 @@
         <v>236</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
   </sheetData>
@@ -7020,35 +7020,35 @@
     </row>
     <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -7064,7 +7064,7 @@
         <v>236</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
   </sheetData>
@@ -7168,7 +7168,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>334</v>
@@ -7176,7 +7176,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>335</v>
@@ -7184,7 +7184,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>336</v>
@@ -7192,7 +7192,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>328</v>
@@ -7200,7 +7200,7 @@
     </row>
     <row r="15" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>328</v>
@@ -7208,7 +7208,7 @@
     </row>
     <row r="16" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>328</v>
@@ -7275,7 +7275,7 @@
         <v>236</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -7283,7 +7283,7 @@
         <v>235</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -7473,7 +7473,7 @@
     </row>
     <row r="13" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>349</v>
@@ -7539,7 +7539,7 @@
         <v>236</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -7794,7 +7794,7 @@
         <v>236</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -8049,7 +8049,7 @@
         <v>236</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -8117,10 +8117,10 @@
     </row>
     <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>528</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>529</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>530</v>
       </c>
       <c r="C2" t="s">
         <v>165</v>
@@ -8128,10 +8128,10 @@
     </row>
     <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C3" t="s">
         <v>165</v>
@@ -8139,10 +8139,10 @@
     </row>
     <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C4" t="s">
         <v>165</v>
@@ -8150,10 +8150,10 @@
     </row>
     <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C5" t="s">
         <v>165</v>
@@ -8161,10 +8161,10 @@
     </row>
     <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
+        <v>541</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>542</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>543</v>
       </c>
       <c r="C6" t="s">
         <v>165</v>
@@ -8172,57 +8172,57 @@
     </row>
     <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C7" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C8" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C9" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C10" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C11" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -8238,7 +8238,7 @@
         <v>236</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
   </sheetData>
@@ -8313,7 +8313,7 @@
         <v>236</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -8321,7 +8321,7 @@
         <v>235</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -8460,7 +8460,7 @@
         <v>236</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -8533,7 +8533,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B2">
         <v>36</v>
@@ -8541,7 +8541,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B3">
         <v>34</v>
@@ -8549,7 +8549,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B4">
         <v>31</v>
@@ -8557,7 +8557,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B5">
         <v>356</v>
@@ -8565,7 +8565,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -8573,7 +8573,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B7">
         <v>36</v>
@@ -8581,7 +8581,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -8589,7 +8589,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B9">
         <v>31</v>
@@ -8597,7 +8597,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -8616,7 +8616,7 @@
         <v>236</v>
       </c>
       <c r="B12" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -8624,7 +8624,7 @@
         <v>235</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -8676,8 +8676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{680EF845-E97A-4774-A116-33BCEE8AAAAA}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8739,7 +8739,7 @@
         <v>236</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -8852,7 +8852,7 @@
         <v>236</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -8896,14 +8896,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F6BE80-AC56-42ED-87D6-9266FD24F810}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="61.88671875" customWidth="1"/>
-    <col min="2" max="2" width="37.88671875" customWidth="1"/>
+    <col min="2" max="2" width="48.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -8919,7 +8919,7 @@
         <v>445</v>
       </c>
       <c r="B2" t="s">
-        <v>453</v>
+        <v>739</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -8986,12 +8986,12 @@
         <v>239</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>236</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -8999,7 +8999,7 @@
         <v>235</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>721</v>
+        <v>740</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -9063,7 +9063,7 @@
     </row>
     <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -9071,7 +9071,7 @@
     </row>
     <row r="3" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B3">
         <v>33</v>
@@ -9079,7 +9079,7 @@
     </row>
     <row r="4" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B4">
         <v>31</v>
@@ -9087,7 +9087,7 @@
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -9095,7 +9095,7 @@
     </row>
     <row r="6" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -9103,7 +9103,7 @@
     </row>
     <row r="7" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -9111,7 +9111,7 @@
     </row>
     <row r="8" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -9130,7 +9130,7 @@
         <v>236</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -9138,7 +9138,7 @@
         <v>235</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -9206,90 +9206,90 @@
     </row>
     <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -9305,7 +9305,7 @@
         <v>236</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
   </sheetData>
@@ -9492,7 +9492,7 @@
         <v>236</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -9500,7 +9500,7 @@
         <v>235</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -9565,10 +9565,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>631</v>
+      </c>
+      <c r="B2" t="s">
         <v>632</v>
-      </c>
-      <c r="B2" t="s">
-        <v>633</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -9584,7 +9584,7 @@
         <v>236</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
   </sheetData>
@@ -9617,7 +9617,7 @@
     </row>
     <row r="2" spans="1:2" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B2" s="5">
         <v>3338</v>
@@ -9625,7 +9625,7 @@
     </row>
     <row r="3" spans="1:2" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B3" s="13">
         <v>1038</v>
@@ -9636,7 +9636,7 @@
         <v>241</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -9644,7 +9644,7 @@
         <v>236</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -9652,7 +9652,7 @@
         <v>235</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -9716,7 +9716,7 @@
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B2" s="13">
         <v>2502</v>
@@ -9724,7 +9724,7 @@
     </row>
     <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B3" s="5">
         <v>851</v>
@@ -9735,7 +9735,7 @@
         <v>241</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -9743,7 +9743,7 @@
         <v>236</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -9751,7 +9751,7 @@
         <v>235</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -9815,7 +9815,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B2" s="5">
         <v>401</v>
@@ -9823,7 +9823,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
@@ -9831,7 +9831,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B4" s="5">
         <v>145</v>
@@ -9839,7 +9839,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>
@@ -9850,7 +9850,7 @@
         <v>241</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -9858,7 +9858,7 @@
         <v>236</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -9866,7 +9866,7 @@
         <v>235</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
finalized cds data for client, updated training data
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDS_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDS_2020_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\RHIT_IRPA_@\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9271012-F191-4195-95CB-94520EE491D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A89606-D486-4A14-9A3B-2FFDA8FCFF01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="38" activeTab="41" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="32" activeTab="35" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="23" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Admission_Applied" sheetId="40" r:id="rId7"/>
     <sheet name="Admission_Admitted" sheetId="39" r:id="rId8"/>
     <sheet name="Admission_Enrolled" sheetId="37" r:id="rId9"/>
-    <sheet name="Admission_Condition" sheetId="38" r:id="rId10"/>
+    <sheet name="Admission_Waitlist" sheetId="38" r:id="rId10"/>
     <sheet name="Admission_High School Required" sheetId="29" r:id="rId11"/>
     <sheet name="Admission_High School Recommend" sheetId="28" r:id="rId12"/>
     <sheet name="Admission_Policies" sheetId="9" r:id="rId13"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="741">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1517" uniqueCount="768">
   <si>
     <t>Answer</t>
   </si>
@@ -952,9 +952,6 @@
     <t>What is the average financial aid package for degree-seeking first-time full-time freshman students who were awarded any financial aid?</t>
   </si>
   <si>
-    <t>What is the average need-based scholarship or grant awarded to degree-seeking first-time full-time freshman students?</t>
-  </si>
-  <si>
     <t>What is the average need-based self-help awarded to degree-seeking first-time full-time freshman students ?</t>
   </si>
   <si>
@@ -1060,9 +1057,6 @@
     <t>What is the number of degree-seeking part-time undergraduate students who were awarded an institutional non-need-based athletic scholarship or grant?</t>
   </si>
   <si>
-    <t>What is the average amount of institutional non-need-based athletic scholarship and grant to degree-seeking part-time undergraduate students?</t>
-  </si>
-  <si>
     <t>$1355304</t>
   </si>
   <si>
@@ -1084,12 +1078,6 @@
     <t>$738685</t>
   </si>
   <si>
-    <t>$10691241</t>
-  </si>
-  <si>
-    <t>$979015</t>
-  </si>
-  <si>
     <t>$771042</t>
   </si>
   <si>
@@ -1105,81 +1093,15 @@
     <t>What is the amount of non-based athletic award awarded to students?</t>
   </si>
   <si>
-    <t>$4938549</t>
-  </si>
-  <si>
-    <t>$375919</t>
-  </si>
-  <si>
     <t>Rose-Hulman uses federal methology in awarding institutional aid.</t>
   </si>
   <si>
     <t>n/a</t>
   </si>
   <si>
-    <t>73.5%</t>
-  </si>
-  <si>
-    <t>$39903</t>
-  </si>
-  <si>
-    <t>$38185</t>
-  </si>
-  <si>
-    <t>$3840</t>
-  </si>
-  <si>
-    <t>$3327</t>
-  </si>
-  <si>
-    <t>170</t>
-  </si>
-  <si>
-    <t>$21671</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>1394</t>
-  </si>
-  <si>
-    <t>$35451</t>
-  </si>
-  <si>
-    <t>$33608</t>
-  </si>
-  <si>
-    <t>$4679</t>
-  </si>
-  <si>
-    <t>$4351</t>
-  </si>
-  <si>
-    <t>794</t>
-  </si>
-  <si>
-    <t>$16643</t>
-  </si>
-  <si>
-    <t>64.7%</t>
-  </si>
-  <si>
-    <t>$26732</t>
-  </si>
-  <si>
-    <t>$24932</t>
-  </si>
-  <si>
-    <t>$4500</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>$14293</t>
-  </si>
-  <si>
     <t>What is Rose-Hulman's mailing address?</t>
   </si>
   <si>
@@ -1250,9 +1172,6 @@
   </si>
   <si>
     <t>What is the student to faculty ratio at Rose-Hulman?</t>
-  </si>
-  <si>
-    <t>What is the number of degree-seeking full-time full-time freshman students who applied for need-based financial aid</t>
   </si>
   <si>
     <t>What special study programs are offered at Rose-Hulman?</t>
@@ -1404,9 +1323,6 @@
   </si>
   <si>
     <t>What is the total number of part-time instructional faculty who are nonresident aliens?</t>
-  </si>
-  <si>
-    <t>The total number of [enrollment_status] instructional faculty who are (xor {member of [*minority] group} {nonresident alien})   is &lt;value&gt;</t>
   </si>
   <si>
     <t>The student to faculty ratio at Rose-Hulman is 10 to 1</t>
@@ -1736,9 +1652,6 @@
     <t>What is Rose-Hulman's tuition for undergraduate students?</t>
   </si>
   <si>
-    <t>The amount of [need_non_need_base_aid] (xor [self-help_aid] {[financial_aid_type] scholarship or grants} (xor {tuition [*waiver]} (xor [*parent] [*student]) loan)))</t>
-  </si>
-  <si>
     <t>15.7% bachelor's degrees conferred are Computer and information science</t>
   </si>
   <si>
@@ -2010,9 +1923,6 @@
     <t>How many degree-seeking undergraduate caucasian students are enrolled?</t>
   </si>
   <si>
-    <t>The number of undergraduate degree-seeking students enrolled by race and immigration status. This includes students enrolled who are either Hispanics, African American, Caucasian, or Pacific Islander, have two or more races or whose race is unknown.</t>
-  </si>
-  <si>
     <t>The (xor [*percent] number) of students {who graduated (xor {[range] [number] years and [number] years} {[range] [number] years}) in the [initial_final] [year] cohort is &lt;value&gt;</t>
   </si>
   <si>
@@ -2022,9 +1932,6 @@
     <t>The  (xor [*percent] number) of degree-seeking undergraduate students enrolled    (xor {of [^*unknown] race} (xor {who are [^race]} {nonresidence alien})) is  &lt;value&gt;</t>
   </si>
   <si>
-    <t>Enrollment by race for first-time first-year students.</t>
-  </si>
-  <si>
     <t>The cohort of students who enrolled at Rose-Hulman in 2014, and graduated within four, five, or six year and graduation rate for those years. You can also ask all of the things paired with financial aid in terms of student who received pell-grant, student who received stafford loan but not pell grant and student who received neither.</t>
   </si>
   <si>
@@ -2134,9 +2041,6 @@
   </si>
   <si>
     <t>What is the average need-based loan awarded to degree-seeking first-time full-time freshman students who were awarded any need-based self-help aid?</t>
-  </si>
-  <si>
-    <t>Various statistics on financial aid, including the number of degree-seeking, full-time freshman students who applied for need-based financial aid. The number of freshmen who were determined to have financial aid. The number of freshmen who were awarded any need-based or non-need-based scholarship or grants and need-based self-help aid. The number of freshmen whose financial need was fully met. The average amount of financial aid package, or need-based scholarships or grants, and need-based self-help, or loans, awarded to freshman students. The average amount of non-need-based institutional scholarships or grants awarded o freshman students who had no financial need. The number of freshman students who were awarded a non-needed-based institutional athletic scholarship or grant and the average amount of such aid awarded. All information is for full-time freshman students.</t>
   </si>
   <si>
     <t>Does Rose-Hulman require high school transcript to apply for transfer applicants?</t>
@@ -2309,13 +2213,190 @@
   </si>
   <si>
     <t xml:space="preserve">From CDS, the number of class sections with number of students (xor {between [^number] and [^number]} {[^range] [^number]}) is &lt;value&gt;  </t>
+  </si>
+  <si>
+    <t>The number of undergraduate degree-seeking students enrolled by race and nonresident-alien(immigration status). This includes students enrolled who are either Hispanics, African American, Caucasian, or Pacific Islander, have two or more races or whose race is unknown.</t>
+  </si>
+  <si>
+    <t>Enrollment by race and nonresident-alien(immigration status) for first-time first-year students.</t>
+  </si>
+  <si>
+    <t>The total number of [^enrollment_status] instructional faculty who are (xor {member of [*minority] group} {nonresident alien})   is &lt;value&gt;</t>
+  </si>
+  <si>
+    <t>Various statistics on financial aid, including the number of degree-seeking, full-time freshman students who applied for need-based financial aid. The number of freshmen who were determined to have financial aid. The number of freshmen who were awarded any need-based or non-need-based scholarship or grants and need-based self-help aid. The number of freshmen whose financial need was fully met. The average amount of financial aid package, need-based scholarships or grants, need-based self-help, or loans, awarded to freshman students. The average amount of non-need-based institutional scholarships or grants awarded o freshman students who had no financial need. The number of freshman students who were awarded a non-needed-based institutional athletic scholarship or grant and the average amount of such aid awarded. All information is for full-time freshman students.</t>
+  </si>
+  <si>
+    <t>The amount of need-based parent loan awarded to students is $4938549.</t>
+  </si>
+  <si>
+    <t>The amount of non-need-based parent loan awarded to students is $375919.</t>
+  </si>
+  <si>
+    <t>The amount of need-need-based student loan borrowed by undergraduate students is $1,250,122.</t>
+  </si>
+  <si>
+    <t>The amount of non-need-based student loan borrowed by undergraduate students is $10691241.</t>
+  </si>
+  <si>
+    <t>The amount of [^need_non_need_base_aid] (xor [self-help_aid] {[^financial_aid_type] scholarship or grants} {tuition [^*waiver]})  awarded to students is &lt;value&gt;</t>
+  </si>
+  <si>
+    <t>What is the number of degree-seeking first-time full-time freshman students who applied for need-based financial aid</t>
+  </si>
+  <si>
+    <t>The number of degree-seeking full-time full-time freshman students who applied for need-based financial aid is 466</t>
+  </si>
+  <si>
+    <t>The number of degree-seeking first-time full-time freshman students that applied for need-based aid and were determined to have financial need is 360</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The number of degree-seeking first-time full-time freshman students who were determined to have financial need and were awarded any financial aid is 360</t>
+  </si>
+  <si>
+    <t>The number of degree-seeking first-time full-time freshman students who were awarded any need-based scholarship or grant aid is 357</t>
+  </si>
+  <si>
+    <t>The number of degree-seeking first-time full-time freshman students who were awarded any need-based self-help aid is 236</t>
+  </si>
+  <si>
+    <t>The number of degree-seeking first-time full-time freshman students who were awarded any non-need-based scholarship or grant aid is 168</t>
+  </si>
+  <si>
+    <t>The number of degree-seeking first-time full-time freshman students whose financial need was fully met is 124</t>
+  </si>
+  <si>
+    <t>On average, the percentage of financial need that was met for degree-seeking first-time full-time freshman who were awarded any need-based aid is 73.5%</t>
+  </si>
+  <si>
+    <t>The average financial aid package for degree-seeking first time full-time freshman students who were awarded any financial aid is $39903</t>
+  </si>
+  <si>
+    <t>The average amount  of need-based scholarship or grant awarded to degree-seeking first-time full-time freshman is $38185</t>
+  </si>
+  <si>
+    <t>What is the average amount of need-based scholarship or grant awarded to degree-seeking first-time full-time freshman students?</t>
+  </si>
+  <si>
+    <t>The average need-based self-help awarded to degree-seeking first-time full-time freshman students is $3840</t>
+  </si>
+  <si>
+    <t>The average need-based loan awarded to degree-seeing first-time full-time freshman students who were awarded any need-based self-help aid is $3327</t>
+  </si>
+  <si>
+    <t>The number of degree-seeking first-time full-time freshman students who had no financial need and who were awarded institutional non-need-based scholarship or grant aid is 170</t>
+  </si>
+  <si>
+    <t>The average amount of institutional non-need-based scholarship and grant aid awarded to degree-seeking full-time freshman students who had no financial need and who were awarded institutional non-need-based scholarship or grant aid is $21,671.</t>
+  </si>
+  <si>
+    <t>There is no available information on the number of degree-seeking first-time full-time freshman students who were awarded an institutional non-need-based athletic scholarship or grant.</t>
+  </si>
+  <si>
+    <t>There is no available information on the average amount of institutional non-need-based athletic scholarship and grant aid awarded to degree-seeking first-time full-time freshman students.</t>
+  </si>
+  <si>
+    <t>The number of degree-seeking full-time undergraduate students who applied for need-based financial aid is 1,394.</t>
+  </si>
+  <si>
+    <t>Out of the total number of students who applied for need-based financial aid, 1,151 were determined to have financial need.</t>
+  </si>
+  <si>
+    <t>Among those who had financial need, 1,150 were awarded some form of financial aid.</t>
+  </si>
+  <si>
+    <t>The number of degree-seeking full-time undergraduate students who were awarded any need-based scholarship or grant aid is 1,144.</t>
+  </si>
+  <si>
+    <t>A total of 829 degree-seeking full-time undergraduate students were awarded any need-based self-help aid.</t>
+  </si>
+  <si>
+    <t>The number of degree-seeking full-time undergraduate students who were awarded any non-need-based scholarship or grant aid is 1,009.</t>
+  </si>
+  <si>
+    <t>284 degree-seeking full-time undergraduate students had their financial need fully met.</t>
+  </si>
+  <si>
+    <t>On average, the percentage of financial need that was met for degree-seeking full-time undergraduate students who were awarded any need-based aid is 65.9%.</t>
+  </si>
+  <si>
+    <t>The average financial aid package for degree-seeking full-time undergraduate students who were awarded any financial aid is $35,451.</t>
+  </si>
+  <si>
+    <t>The average need-based scholarship or grant awarded to degree-seeking full-time undergraduate students is $33,608.</t>
+  </si>
+  <si>
+    <t>Degree-seeking full-time undergraduate students who were awarded any need-based self-help aid received an average of $4,679.</t>
+  </si>
+  <si>
+    <t>Among those who were awarded any need-based self-help aid, the average need-based loan amount was $4,351.</t>
+  </si>
+  <si>
+    <t>The number of degree-seeking full-time undergraduate students who had no financial need and were awarded institutional non-need-based scholarship or grant aid is 794.</t>
+  </si>
+  <si>
+    <t>The average amount of institutional non-need-based scholarship and grant aid awarded to degree-seeking full-time students who had no financial need and who were awarded institutional non-need-based scholarship or grant aid is $16,643.</t>
+  </si>
+  <si>
+    <t>There is no available information on the number of degree-seeking full-time undergraduate students who were awarded an institutional non-need-based athletic scholarship or grant, or the average amount of such aid.</t>
+  </si>
+  <si>
+    <t>There were 6 degree-seeking part-time undergraduate students who applied for need-based financial aid.</t>
+  </si>
+  <si>
+    <t>Out of the degree-seeking part-time undergraduate students who applied for need-based financial aid, 5 were determined to have financial need.</t>
+  </si>
+  <si>
+    <t>Among the degree-seeking part-time undergraduate students who were determined to have financial need, 5 were awarded some form of financial aid.</t>
+  </si>
+  <si>
+    <t>A total of 5 degree-seeking part-time undergraduate students were awarded need-based scholarship or grant aid.</t>
+  </si>
+  <si>
+    <t>Only 2 degree-seeking part-time undergraduate students were awarded need-based self-help aid.</t>
+  </si>
+  <si>
+    <t>The number of degree-seeking part-time undergraduate students whose financial need was fully met was 1.</t>
+  </si>
+  <si>
+    <t>On average, 64.7% of financial need was met for degree-seeking part-time undergraduate students who were awarded any need-based aid.</t>
+  </si>
+  <si>
+    <t>The average financial aid package awarded to degree-seeking part-time undergraduate students who were awarded any financial aid was $26732.</t>
+  </si>
+  <si>
+    <t>The average need-based scholarship or grant awarded to degree-seeking part-time undergraduate students was $24932.</t>
+  </si>
+  <si>
+    <t>The average need-based self-help awarded to degree-seeking part-time undergraduate students was $4500.</t>
+  </si>
+  <si>
+    <t>The average need-based loan awarded to students who were awarded any need-based self-help aid was $4500.</t>
+  </si>
+  <si>
+    <t>A total of 10 degree-seeking part-time undergraduate students who had no financial need were awarded institutional non-need-based scholarship or grant aid.</t>
+  </si>
+  <si>
+    <t>The average amount of institutional non-need-based scholarship and grant aid awarded to degree-seeking part-time students who had no financial need was $14293.</t>
+  </si>
+  <si>
+    <t>There is no information available regarding the number of degree-seeking part-time undergraduate students who were awarded an institutional non-need-based athletic scholarship or grant.</t>
+  </si>
+  <si>
+    <t>There is no information available regarding the average amount of institutional non-need-based athletic scholarship and grant awarded to degree-seeking part-time undergraduate students.</t>
+  </si>
+  <si>
+    <t>What is the average amount of institutional non-need-based athletic scholarship and grants awarded to degree-seeking part-time undergraduate students?</t>
+  </si>
+  <si>
+    <t>There is no available information on the average amount of institutional non-need-based athletic scholarships and grants awarded to degree-seeking part-time undergraduate students.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2349,6 +2430,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2371,7 +2463,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -2404,6 +2496,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2713,10 +2817,10 @@
     </row>
     <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>366</v>
+        <v>340</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>397</v>
+        <v>370</v>
       </c>
       <c r="C2" t="s">
         <v>165</v>
@@ -2724,10 +2828,10 @@
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>398</v>
+        <v>371</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>399</v>
+        <v>372</v>
       </c>
       <c r="C3" t="s">
         <v>165</v>
@@ -2735,10 +2839,10 @@
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>368</v>
+        <v>342</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>400</v>
+        <v>373</v>
       </c>
       <c r="C4" t="s">
         <v>165</v>
@@ -2746,10 +2850,10 @@
     </row>
     <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>367</v>
+        <v>341</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>401</v>
+        <v>374</v>
       </c>
       <c r="C5" t="s">
         <v>165</v>
@@ -2757,10 +2861,10 @@
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>369</v>
+        <v>343</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>402</v>
+        <v>375</v>
       </c>
       <c r="C6" t="s">
         <v>165</v>
@@ -2768,10 +2872,10 @@
     </row>
     <row r="7" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>370</v>
+        <v>344</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>403</v>
+        <v>376</v>
       </c>
       <c r="C7" t="s">
         <v>165</v>
@@ -2779,10 +2883,10 @@
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>371</v>
+        <v>345</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>404</v>
+        <v>377</v>
       </c>
       <c r="C8" t="s">
         <v>165</v>
@@ -2790,10 +2894,10 @@
     </row>
     <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>405</v>
+        <v>378</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>406</v>
+        <v>379</v>
       </c>
       <c r="C9" t="s">
         <v>165</v>
@@ -2801,10 +2905,10 @@
     </row>
     <row r="10" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>372</v>
+        <v>346</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>407</v>
+        <v>380</v>
       </c>
       <c r="C10" t="s">
         <v>165</v>
@@ -2812,10 +2916,10 @@
     </row>
     <row r="11" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>373</v>
+        <v>347</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>408</v>
+        <v>381</v>
       </c>
       <c r="C11" t="s">
         <v>165</v>
@@ -2823,10 +2927,10 @@
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>374</v>
+        <v>348</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>409</v>
+        <v>382</v>
       </c>
       <c r="C12" t="s">
         <v>165</v>
@@ -2834,10 +2938,10 @@
     </row>
     <row r="13" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>375</v>
+        <v>349</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>410</v>
+        <v>383</v>
       </c>
       <c r="C13" t="s">
         <v>165</v>
@@ -2845,10 +2949,10 @@
     </row>
     <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>376</v>
+        <v>350</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>411</v>
+        <v>384</v>
       </c>
       <c r="C14" t="s">
         <v>165</v>
@@ -2867,7 +2971,7 @@
         <v>236</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>634</v>
+        <v>605</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -2912,7 +3016,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2935,10 +3039,10 @@
     </row>
     <row r="2" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>560</v>
+        <v>531</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>630</v>
+        <v>601</v>
       </c>
       <c r="C2" t="s">
         <v>165</v>
@@ -2946,10 +3050,10 @@
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>561</v>
+        <v>532</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>566</v>
+        <v>537</v>
       </c>
       <c r="C3" t="s">
         <v>165</v>
@@ -2957,10 +3061,10 @@
     </row>
     <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>562</v>
+        <v>533</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>563</v>
+        <v>534</v>
       </c>
       <c r="C4" t="s">
         <v>165</v>
@@ -2968,10 +3072,10 @@
     </row>
     <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>564</v>
+        <v>535</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>565</v>
+        <v>536</v>
       </c>
       <c r="C5" t="s">
         <v>165</v>
@@ -2982,7 +3086,7 @@
         <v>241</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>567</v>
+        <v>538</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
@@ -2990,7 +3094,7 @@
         <v>236</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>651</v>
+        <v>620</v>
       </c>
     </row>
   </sheetData>
@@ -3026,7 +3130,7 @@
     </row>
     <row r="2" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>473</v>
+        <v>445</v>
       </c>
       <c r="B2" s="5">
         <v>4</v>
@@ -3037,7 +3141,7 @@
     </row>
     <row r="3" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>474</v>
+        <v>446</v>
       </c>
       <c r="B3" s="5">
         <v>4</v>
@@ -3048,7 +3152,7 @@
     </row>
     <row r="4" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>475</v>
+        <v>447</v>
       </c>
       <c r="B4" s="5">
         <v>3</v>
@@ -3059,7 +3163,7 @@
     </row>
     <row r="5" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>476</v>
+        <v>448</v>
       </c>
       <c r="B5" s="5">
         <v>3</v>
@@ -3070,7 +3174,7 @@
     </row>
     <row r="6" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>466</v>
+        <v>438</v>
       </c>
       <c r="B6" s="5">
         <v>0</v>
@@ -3081,7 +3185,7 @@
     </row>
     <row r="7" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>467</v>
+        <v>439</v>
       </c>
       <c r="B7" s="5">
         <v>2</v>
@@ -3092,7 +3196,7 @@
     </row>
     <row r="8" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>468</v>
+        <v>440</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -3103,7 +3207,7 @@
     </row>
     <row r="9" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>469</v>
+        <v>441</v>
       </c>
       <c r="B9" s="5">
         <v>0</v>
@@ -3114,7 +3218,7 @@
     </row>
     <row r="10" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>470</v>
+        <v>442</v>
       </c>
       <c r="B10" s="5">
         <v>0</v>
@@ -3125,7 +3229,7 @@
     </row>
     <row r="11" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>471</v>
+        <v>443</v>
       </c>
       <c r="B11" s="5">
         <v>0</v>
@@ -3136,7 +3240,7 @@
     </row>
     <row r="12" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>472</v>
+        <v>444</v>
       </c>
       <c r="B12" s="5">
         <v>0</v>
@@ -3147,10 +3251,10 @@
     </row>
     <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>495</v>
+        <v>467</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>496</v>
+        <v>468</v>
       </c>
       <c r="C13" t="s">
         <v>165</v>
@@ -3169,7 +3273,7 @@
         <v>236</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>652</v>
+        <v>621</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -3177,7 +3281,7 @@
         <v>235</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>572</v>
+        <v>543</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -3242,7 +3346,7 @@
     </row>
     <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>477</v>
+        <v>449</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3250,7 +3354,7 @@
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>478</v>
+        <v>450</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -3258,7 +3362,7 @@
     </row>
     <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>479</v>
+        <v>451</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -3266,7 +3370,7 @@
     </row>
     <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>494</v>
+        <v>466</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -3274,7 +3378,7 @@
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>480</v>
+        <v>452</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -3282,7 +3386,7 @@
     </row>
     <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>481</v>
+        <v>453</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -3290,7 +3394,7 @@
     </row>
     <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>482</v>
+        <v>454</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -3298,7 +3402,7 @@
     </row>
     <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>483</v>
+        <v>455</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -3306,7 +3410,7 @@
     </row>
     <row r="10" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>484</v>
+        <v>456</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -3314,7 +3418,7 @@
     </row>
     <row r="11" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>485</v>
+        <v>457</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -3322,7 +3426,7 @@
     </row>
     <row r="12" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>486</v>
+        <v>458</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -3341,7 +3445,7 @@
         <v>236</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>653</v>
+        <v>622</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -3349,7 +3453,7 @@
         <v>235</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>571</v>
+        <v>542</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -3547,7 +3651,7 @@
         <v>236</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>654</v>
+        <v>623</v>
       </c>
     </row>
   </sheetData>
@@ -3583,7 +3687,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>573</v>
+        <v>544</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -3591,7 +3695,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>574</v>
+        <v>545</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -3599,7 +3703,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>575</v>
+        <v>546</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3607,7 +3711,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>576</v>
+        <v>547</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -3615,7 +3719,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>578</v>
+        <v>549</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3623,7 +3727,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>577</v>
+        <v>548</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -3631,7 +3735,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>579</v>
+        <v>550</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3639,7 +3743,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>580</v>
+        <v>551</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3647,7 +3751,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>581</v>
+        <v>552</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3655,7 +3759,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>582</v>
+        <v>553</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3663,7 +3767,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>583</v>
+        <v>554</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -3671,7 +3775,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>584</v>
+        <v>555</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3679,7 +3783,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>585</v>
+        <v>556</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -3687,7 +3791,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>586</v>
+        <v>557</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3695,7 +3799,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>587</v>
+        <v>558</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -3703,7 +3807,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>588</v>
+        <v>559</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -3711,7 +3815,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>589</v>
+        <v>560</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -3719,7 +3823,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>590</v>
+        <v>561</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3727,7 +3831,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>591</v>
+        <v>562</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3743,7 +3847,7 @@
         <v>236</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>647</v>
+        <v>616</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3751,7 +3855,7 @@
         <v>235</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>412</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -3784,42 +3888,42 @@
     </row>
     <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>720</v>
+        <v>688</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>724</v>
+        <v>692</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>721</v>
+        <v>689</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>723</v>
+        <v>691</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>722</v>
+        <v>690</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>725</v>
+        <v>693</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>729</v>
+        <v>697</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>726</v>
+        <v>694</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>738</v>
+        <v>706</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>727</v>
+        <v>695</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -3835,7 +3939,7 @@
         <v>236</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>728</v>
+        <v>696</v>
       </c>
     </row>
   </sheetData>
@@ -3927,7 +4031,7 @@
         <v>236</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>656</v>
+        <v>625</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -3935,7 +4039,7 @@
         <v>235</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>527</v>
+        <v>499</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -4106,7 +4210,7 @@
         <v>236</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>655</v>
+        <v>624</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -4114,7 +4218,7 @@
         <v>235</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>526</v>
+        <v>498</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -4241,7 +4345,7 @@
         <v>236</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>657</v>
+        <v>626</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -4249,7 +4353,7 @@
         <v>235</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>525</v>
+        <v>497</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -4420,7 +4524,7 @@
         <v>236</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>658</v>
+        <v>627</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -4428,7 +4532,7 @@
         <v>235</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>520</v>
+        <v>492</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -4439,7 +4543,7 @@
         <v>165</v>
       </c>
       <c r="D17" t="s">
-        <v>501</v>
+        <v>473</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -4496,7 +4600,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>595</v>
+        <v>566</v>
       </c>
       <c r="B2" s="5">
         <v>387</v>
@@ -4504,7 +4608,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>594</v>
+        <v>565</v>
       </c>
       <c r="B3" s="5">
         <v>143</v>
@@ -4512,7 +4616,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>593</v>
+        <v>564</v>
       </c>
       <c r="B4" s="5">
         <v>1</v>
@@ -4520,7 +4624,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>600</v>
+        <v>571</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>
@@ -4528,7 +4632,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>638</v>
+        <v>609</v>
       </c>
       <c r="B6" s="5">
         <v>9</v>
@@ -4536,7 +4640,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>637</v>
+        <v>608</v>
       </c>
       <c r="B7" s="5">
         <v>2</v>
@@ -4544,7 +4648,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>636</v>
+        <v>607</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -4552,7 +4656,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>635</v>
+        <v>606</v>
       </c>
       <c r="B9" s="5">
         <v>0</v>
@@ -4560,7 +4664,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>596</v>
+        <v>567</v>
       </c>
       <c r="B10" s="5">
         <v>1082</v>
@@ -4568,7 +4672,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>597</v>
+        <v>568</v>
       </c>
       <c r="B11" s="5">
         <v>329</v>
@@ -4576,7 +4680,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>598</v>
+        <v>569</v>
       </c>
       <c r="B12" s="5">
         <v>15</v>
@@ -4584,7 +4688,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>599</v>
+        <v>570</v>
       </c>
       <c r="B13" s="5">
         <v>1</v>
@@ -4731,7 +4835,7 @@
         <v>236</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>639</v>
+        <v>610</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -4739,7 +4843,7 @@
         <v>235</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>620</v>
+        <v>591</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -4804,7 +4908,7 @@
     </row>
     <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>415</v>
+        <v>388</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>53</v>
@@ -4812,7 +4916,7 @@
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>416</v>
+        <v>389</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>54</v>
@@ -4820,7 +4924,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>413</v>
+        <v>386</v>
       </c>
       <c r="B4" s="6">
         <v>350</v>
@@ -4828,10 +4932,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>414</v>
+        <v>387</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>502</v>
+        <v>474</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -4847,7 +4951,7 @@
         <v>236</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>659</v>
+        <v>628</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -4855,7 +4959,7 @@
         <v>235</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>519</v>
+        <v>491</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -5061,7 +5165,7 @@
         <v>24</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>503</v>
+        <v>475</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -5189,7 +5293,7 @@
         <v>236</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>660</v>
+        <v>629</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -5197,7 +5301,7 @@
         <v>235</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>521</v>
+        <v>493</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -5266,7 +5370,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>524</v>
+        <v>496</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>91</v>
@@ -5277,7 +5381,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>417</v>
+        <v>390</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>92</v>
@@ -5288,7 +5392,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>418</v>
+        <v>391</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>93</v>
@@ -5299,7 +5403,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>419</v>
+        <v>392</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>94</v>
@@ -5310,7 +5414,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>420</v>
+        <v>393</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>95</v>
@@ -5321,7 +5425,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>421</v>
+        <v>394</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>96</v>
@@ -5332,7 +5436,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>422</v>
+        <v>395</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>102</v>
@@ -5343,7 +5447,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>423</v>
+        <v>396</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>102</v>
@@ -5354,7 +5458,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>424</v>
+        <v>397</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>102</v>
@@ -5365,10 +5469,10 @@
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>425</v>
+        <v>398</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>433</v>
+        <v>406</v>
       </c>
       <c r="C11" t="s">
         <v>165</v>
@@ -5376,10 +5480,10 @@
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>426</v>
+        <v>399</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>434</v>
+        <v>407</v>
       </c>
       <c r="C12" t="s">
         <v>165</v>
@@ -5398,7 +5502,7 @@
         <v>236</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>661</v>
+        <v>630</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -5406,7 +5510,7 @@
         <v>235</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>522</v>
+        <v>494</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -5474,7 +5578,7 @@
     </row>
     <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>427</v>
+        <v>400</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>115</v>
@@ -5482,7 +5586,7 @@
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>428</v>
+        <v>401</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>116</v>
@@ -5490,7 +5594,7 @@
     </row>
     <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>429</v>
+        <v>402</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>117</v>
@@ -5498,7 +5602,7 @@
     </row>
     <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>430</v>
+        <v>403</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>118</v>
@@ -5506,7 +5610,7 @@
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>431</v>
+        <v>404</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>102</v>
@@ -5514,7 +5618,7 @@
     </row>
     <row r="7" spans="1:2" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>432</v>
+        <v>405</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>119</v>
@@ -5533,7 +5637,7 @@
         <v>236</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>662</v>
+        <v>631</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -5541,7 +5645,7 @@
         <v>235</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>523</v>
+        <v>495</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -5606,7 +5710,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>616</v>
+        <v>587</v>
       </c>
       <c r="B2" s="6">
         <v>59</v>
@@ -5614,7 +5718,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>617</v>
+        <v>588</v>
       </c>
       <c r="B3" s="6">
         <v>30</v>
@@ -5622,7 +5726,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>618</v>
+        <v>589</v>
       </c>
       <c r="B4" s="6">
         <v>9</v>
@@ -5630,7 +5734,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>613</v>
+        <v>584</v>
       </c>
       <c r="B5" s="6">
         <v>23</v>
@@ -5638,7 +5742,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>614</v>
+        <v>585</v>
       </c>
       <c r="B6" s="6">
         <v>13</v>
@@ -5646,7 +5750,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>615</v>
+        <v>586</v>
       </c>
       <c r="B7" s="6">
         <v>2</v>
@@ -5665,7 +5769,7 @@
         <v>236</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>663</v>
+        <v>632</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -5673,7 +5777,7 @@
         <v>235</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>396</v>
+        <v>369</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -5763,7 +5867,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>694</v>
+        <v>662</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>130</v>
@@ -5782,10 +5886,10 @@
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>684</v>
+        <v>652</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>685</v>
+        <v>653</v>
       </c>
       <c r="C6" t="s">
         <v>165</v>
@@ -5793,10 +5897,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>695</v>
+        <v>663</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>686</v>
+        <v>654</v>
       </c>
       <c r="C7" t="s">
         <v>165</v>
@@ -5804,10 +5908,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>687</v>
+        <v>655</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>690</v>
+        <v>658</v>
       </c>
       <c r="C8" t="s">
         <v>165</v>
@@ -5815,10 +5919,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>696</v>
+        <v>664</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>691</v>
+        <v>659</v>
       </c>
       <c r="C9" t="s">
         <v>165</v>
@@ -5826,7 +5930,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>697</v>
+        <v>665</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>132</v>
@@ -5837,7 +5941,7 @@
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>698</v>
+        <v>666</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>133</v>
@@ -5848,10 +5952,10 @@
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>688</v>
+        <v>656</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>692</v>
+        <v>660</v>
       </c>
       <c r="C12" t="s">
         <v>165</v>
@@ -5859,7 +5963,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>689</v>
+        <v>657</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>266</v>
@@ -5892,7 +5996,7 @@
     </row>
     <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>699</v>
+        <v>667</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>136</v>
@@ -5980,7 +6084,7 @@
         <v>236</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>693</v>
+        <v>661</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -6043,15 +6147,15 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>391</v>
+        <v>364</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>393</v>
+        <v>366</v>
       </c>
       <c r="C2" t="s">
         <v>165</v>
@@ -6059,10 +6163,10 @@
     </row>
     <row r="3" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>392</v>
+        <v>365</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>395</v>
+        <v>368</v>
       </c>
       <c r="C3" t="s">
         <v>165</v>
@@ -6081,7 +6185,7 @@
         <v>236</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>629</v>
+        <v>600</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -6156,7 +6260,7 @@
         <v>143</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>700</v>
+        <v>668</v>
       </c>
       <c r="C2" t="s">
         <v>165</v>
@@ -6167,7 +6271,7 @@
         <v>146</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>703</v>
+        <v>671</v>
       </c>
       <c r="C3" t="s">
         <v>165</v>
@@ -6178,7 +6282,7 @@
         <v>147</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>704</v>
+        <v>672</v>
       </c>
       <c r="C4" t="s">
         <v>165</v>
@@ -6252,7 +6356,7 @@
         <v>236</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>707</v>
+        <v>675</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -6320,7 +6424,7 @@
         <v>144</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>701</v>
+        <v>669</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -6328,7 +6432,7 @@
         <v>145</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>702</v>
+        <v>670</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -6336,7 +6440,7 @@
         <v>148</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>705</v>
+        <v>673</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
@@ -6392,7 +6496,7 @@
         <v>236</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>706</v>
+        <v>674</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -6527,7 +6631,7 @@
         <v>236</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>664</v>
+        <v>633</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -6572,7 +6676,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6591,7 +6695,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>606</v>
+        <v>577</v>
       </c>
       <c r="B2" s="5">
         <v>226</v>
@@ -6599,7 +6703,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>605</v>
+        <v>576</v>
       </c>
       <c r="B3" s="5">
         <v>104</v>
@@ -6607,7 +6711,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>601</v>
+        <v>572</v>
       </c>
       <c r="B4" s="5">
         <v>93</v>
@@ -6615,7 +6719,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>640</v>
+        <v>611</v>
       </c>
       <c r="B5" s="5">
         <v>1295</v>
@@ -6623,7 +6727,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>602</v>
+        <v>573</v>
       </c>
       <c r="B6" s="5">
         <v>3</v>
@@ -6631,7 +6735,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>603</v>
+        <v>574</v>
       </c>
       <c r="B7" s="5">
         <v>127</v>
@@ -6639,7 +6743,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>604</v>
+        <v>575</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -6669,12 +6773,12 @@
         <v>239</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>236</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>641</v>
+        <v>709</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -6682,7 +6786,7 @@
         <v>235</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>644</v>
+        <v>614</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -6722,7 +6826,7 @@
         <v>262</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>497</v>
+        <v>469</v>
       </c>
     </row>
   </sheetData>
@@ -6755,101 +6859,101 @@
     </row>
     <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>504</v>
+        <v>476</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>505</v>
+        <v>477</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>506</v>
+        <v>478</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>730</v>
+        <v>698</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>731</v>
+        <v>699</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>506</v>
+        <v>478</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>548</v>
+        <v>520</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>732</v>
+        <v>700</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>506</v>
+        <v>478</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>549</v>
+        <v>521</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>733</v>
+        <v>701</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>506</v>
+        <v>478</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>507</v>
+        <v>479</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>734</v>
+        <v>702</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>506</v>
+        <v>478</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>508</v>
+        <v>480</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>735</v>
+        <v>703</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>506</v>
+        <v>478</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>509</v>
+        <v>481</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>737</v>
+        <v>705</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>506</v>
+        <v>478</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>510</v>
+        <v>482</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>736</v>
+        <v>704</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>506</v>
+        <v>478</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>511</v>
+        <v>483</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>547</v>
+        <v>519</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>506</v>
+        <v>478</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -6865,7 +6969,7 @@
         <v>236</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>669</v>
+        <v>638</v>
       </c>
     </row>
   </sheetData>
@@ -6899,79 +7003,79 @@
     </row>
     <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>670</v>
+        <v>639</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>673</v>
+        <v>642</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>506</v>
+        <v>478</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>515</v>
+        <v>487</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>672</v>
+        <v>641</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>506</v>
+        <v>478</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>516</v>
+        <v>488</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>671</v>
+        <v>640</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>506</v>
+        <v>478</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>517</v>
+        <v>489</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>665</v>
+        <v>634</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>506</v>
+        <v>478</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>667</v>
+        <v>636</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>675</v>
+        <v>644</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>506</v>
+        <v>478</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>674</v>
+        <v>643</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>677</v>
+        <v>646</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>506</v>
+        <v>478</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>518</v>
+        <v>490</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>666</v>
+        <v>635</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>506</v>
+        <v>478</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -6987,7 +7091,7 @@
         <v>236</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>676</v>
+        <v>645</v>
       </c>
     </row>
   </sheetData>
@@ -7020,35 +7124,35 @@
     </row>
     <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>512</v>
+        <v>484</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>678</v>
+        <v>647</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>506</v>
+        <v>478</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>513</v>
+        <v>485</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>679</v>
+        <v>648</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>506</v>
+        <v>478</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>514</v>
+        <v>486</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>680</v>
+        <v>649</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>506</v>
+        <v>478</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -7064,7 +7168,7 @@
         <v>236</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>668</v>
+        <v>637</v>
       </c>
     </row>
   </sheetData>
@@ -7074,195 +7178,262 @@
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E00C0EE-B5EA-4C5D-A3F6-0409760A68CF}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="83.6640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="62.109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="64.88671875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>271</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>272</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+      <c r="C3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>273</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+      <c r="C4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>274</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>327</v>
+      </c>
+      <c r="C5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>275</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>328</v>
+      </c>
+      <c r="C6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>276</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+        <v>329</v>
+      </c>
+      <c r="C7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>277</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+        <v>330</v>
+      </c>
+      <c r="C8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>278</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+      <c r="C9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>279</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>331</v>
+      </c>
+      <c r="C10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>460</v>
+        <v>432</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+        <v>716</v>
+      </c>
+      <c r="C11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>461</v>
+        <v>433</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <v>715</v>
+      </c>
+      <c r="C12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>462</v>
+        <v>434</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+        <v>332</v>
+      </c>
+      <c r="C13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
-        <v>463</v>
+        <v>435</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+      <c r="C14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>464</v>
+        <v>436</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+      <c r="C15" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
-        <v>465</v>
+        <v>437</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+      <c r="C16" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>280</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+        <v>713</v>
+      </c>
+      <c r="C17" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>281</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+        <v>714</v>
+      </c>
+      <c r="C18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+        <v>338</v>
+      </c>
+      <c r="C19" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+        <v>338</v>
+      </c>
+      <c r="C21" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+        <v>338</v>
+      </c>
+      <c r="C22" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>241</v>
       </c>
@@ -7270,23 +7441,23 @@
         <v>239</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>236</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>235</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>237</v>
       </c>
@@ -7294,7 +7465,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>238</v>
       </c>
@@ -7302,7 +7473,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>242</v>
       </c>
@@ -7310,7 +7481,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>240</v>
       </c>
@@ -7328,8 +7499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BD85EB1-BDB8-4AEB-99D1-57DF875DFEB5}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7350,177 +7521,177 @@
         <v>265</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>390</v>
-      </c>
-      <c r="B2" s="6">
-        <v>466</v>
+        <v>718</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>719</v>
       </c>
       <c r="C2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="B3" s="6">
-        <v>360</v>
+      <c r="B3" s="6" t="s">
+        <v>720</v>
       </c>
       <c r="C3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="B4" s="6">
-        <v>360</v>
+      <c r="B4" s="6" t="s">
+        <v>721</v>
       </c>
       <c r="C4" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="B5" s="6">
-        <v>357</v>
+      <c r="B5" s="6" t="s">
+        <v>722</v>
       </c>
       <c r="C5" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="B6" s="6">
-        <v>236</v>
+      <c r="B6" s="6" t="s">
+        <v>723</v>
       </c>
       <c r="C6" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="B7" s="6">
-        <v>168</v>
+      <c r="B7" s="6" t="s">
+        <v>724</v>
       </c>
       <c r="C7" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="B8" s="6">
-        <v>124</v>
+      <c r="B8" s="6" t="s">
+        <v>725</v>
       </c>
       <c r="C8" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>288</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>345</v>
+        <v>726</v>
       </c>
       <c r="C9" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>289</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>346</v>
+        <v>727</v>
       </c>
       <c r="C10" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
+        <v>729</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>728</v>
+      </c>
+      <c r="C11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>347</v>
-      </c>
-      <c r="C11" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>291</v>
-      </c>
       <c r="B12" s="6" t="s">
-        <v>348</v>
+        <v>730</v>
       </c>
       <c r="C12" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>682</v>
+        <v>651</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>349</v>
+        <v>731</v>
       </c>
       <c r="C13" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>732</v>
+      </c>
+      <c r="C14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>733</v>
+      </c>
+      <c r="C15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="C14" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>351</v>
-      </c>
-      <c r="C15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+      <c r="B16" s="14" t="s">
+        <v>734</v>
+      </c>
+      <c r="C16" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>352</v>
-      </c>
-      <c r="C16" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>352</v>
+      <c r="B17" s="14" t="s">
+        <v>735</v>
       </c>
       <c r="C17" t="s">
         <v>165</v>
@@ -7530,7 +7701,7 @@
       <c r="A18" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="5" t="s">
         <v>239</v>
       </c>
     </row>
@@ -7539,14 +7710,14 @@
         <v>236</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>683</v>
+        <v>712</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="5" t="s">
         <v>203</v>
       </c>
     </row>
@@ -7554,7 +7725,7 @@
       <c r="A21" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="5" t="s">
         <v>203</v>
       </c>
     </row>
@@ -7562,7 +7733,7 @@
       <c r="A22" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="5" t="s">
         <v>203</v>
       </c>
     </row>
@@ -7570,12 +7741,13 @@
       <c r="A23" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="5" t="s">
         <v>203</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7583,14 +7755,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE4F375-28FB-4634-A90F-E29F4CD5ADA1}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="85.88671875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="49.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="49.33203125" style="15" customWidth="1"/>
     <col min="3" max="3" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7598,173 +7770,173 @@
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>736</v>
+      </c>
+      <c r="C2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="C2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="B3" s="16" t="s">
+        <v>737</v>
+      </c>
+      <c r="C3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="B3" s="4">
-        <v>1151</v>
-      </c>
-      <c r="C3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="B4" s="16" t="s">
+        <v>738</v>
+      </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="B4" s="4">
-        <v>1150</v>
-      </c>
-      <c r="C4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="B5" s="16" t="s">
+        <v>739</v>
+      </c>
+      <c r="C5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="B5" s="4">
-        <v>1144</v>
-      </c>
-      <c r="C5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="B6" s="16" t="s">
+        <v>740</v>
+      </c>
+      <c r="C6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="B6" s="4">
-        <v>829</v>
-      </c>
-      <c r="C6" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="B7" s="16" t="s">
+        <v>741</v>
+      </c>
+      <c r="C7" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="B7" s="4">
-        <v>1009</v>
-      </c>
-      <c r="C7" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="B8" s="16" t="s">
+        <v>742</v>
+      </c>
+      <c r="C8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="B8" s="4">
-        <v>284</v>
-      </c>
-      <c r="C8" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="B9" s="16" t="s">
+        <v>743</v>
+      </c>
+      <c r="C9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="B10" s="16" t="s">
+        <v>744</v>
+      </c>
+      <c r="C10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>354</v>
-      </c>
-      <c r="C10" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="B11" s="16" t="s">
+        <v>745</v>
+      </c>
+      <c r="C11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="C11" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="B12" s="16" t="s">
+        <v>746</v>
+      </c>
+      <c r="C12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>747</v>
+      </c>
+      <c r="C13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>356</v>
-      </c>
-      <c r="C12" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>435</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="C13" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="B14" s="16" t="s">
+        <v>748</v>
+      </c>
+      <c r="C14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="75" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
         <v>308</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>358</v>
-      </c>
-      <c r="C14" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="B15" s="16" t="s">
+        <v>749</v>
+      </c>
+      <c r="C15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="75" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>359</v>
-      </c>
-      <c r="C15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>352</v>
+      <c r="B16" s="16" t="s">
+        <v>750</v>
       </c>
       <c r="C16" t="s">
         <v>165</v>
@@ -7772,10 +7944,10 @@
     </row>
     <row r="17" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>352</v>
+        <v>310</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>339</v>
       </c>
       <c r="C17" t="s">
         <v>165</v>
@@ -7785,7 +7957,7 @@
       <c r="A18" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="17" t="s">
         <v>239</v>
       </c>
     </row>
@@ -7793,15 +7965,15 @@
       <c r="A19" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>709</v>
+      <c r="B19" s="15" t="s">
+        <v>677</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="17" t="s">
         <v>203</v>
       </c>
     </row>
@@ -7809,7 +7981,7 @@
       <c r="A21" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="17" t="s">
         <v>203</v>
       </c>
     </row>
@@ -7817,7 +7989,7 @@
       <c r="A22" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="17" t="s">
         <v>203</v>
       </c>
     </row>
@@ -7825,7 +7997,7 @@
       <c r="A23" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="17" t="s">
         <v>203</v>
       </c>
     </row>
@@ -7838,14 +8010,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46EA6128-27F4-4911-A1F0-865B26420EEF}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="78.88671875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="40.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="40.33203125" style="6" customWidth="1"/>
     <col min="3" max="3" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7853,52 +8025,52 @@
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>751</v>
+      </c>
+      <c r="C2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
         <v>312</v>
       </c>
-      <c r="B2" s="4">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="B3" s="14" t="s">
+        <v>752</v>
+      </c>
+      <c r="C3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="B3" s="4">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="B4" s="14" t="s">
+        <v>753</v>
+      </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="C4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>232</v>
+      <c r="B5" s="14" t="s">
+        <v>754</v>
       </c>
       <c r="C5" t="s">
         <v>165</v>
@@ -7906,131 +8078,131 @@
     </row>
     <row r="6" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>755</v>
+      </c>
+      <c r="C6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
         <v>316</v>
       </c>
-      <c r="B6" s="4">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="B7" s="14" t="s">
+        <v>756</v>
+      </c>
+      <c r="C7" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
         <v>317</v>
       </c>
-      <c r="B7" s="4">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="B8" s="14" t="s">
+        <v>757</v>
+      </c>
+      <c r="C8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
         <v>318</v>
       </c>
-      <c r="B8" s="4">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="B9" s="14" t="s">
+        <v>758</v>
+      </c>
+      <c r="C9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
         <v>319</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>360</v>
-      </c>
-      <c r="C9" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="B10" s="14" t="s">
+        <v>759</v>
+      </c>
+      <c r="C10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
         <v>320</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>361</v>
-      </c>
-      <c r="C10" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="B11" s="14" t="s">
+        <v>760</v>
+      </c>
+      <c r="C11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
         <v>321</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>362</v>
-      </c>
-      <c r="C11" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="B12" s="14" t="s">
+        <v>761</v>
+      </c>
+      <c r="C12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>762</v>
+      </c>
+      <c r="C13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
         <v>322</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>363</v>
-      </c>
-      <c r="C12" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>292</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>363</v>
-      </c>
-      <c r="C13" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="B14" s="14" t="s">
+        <v>763</v>
+      </c>
+      <c r="C14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="69" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>364</v>
-      </c>
-      <c r="C14" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="B15" s="14" t="s">
+        <v>764</v>
+      </c>
+      <c r="C15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
         <v>324</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>365</v>
-      </c>
-      <c r="C15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>325</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>352</v>
+      <c r="B16" s="14" t="s">
+        <v>765</v>
       </c>
       <c r="C16" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>326</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>352</v>
+        <v>766</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>767</v>
       </c>
       <c r="C17" t="s">
         <v>165</v>
@@ -8040,7 +8212,7 @@
       <c r="A18" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="5" t="s">
         <v>239</v>
       </c>
     </row>
@@ -8049,14 +8221,14 @@
         <v>236</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>708</v>
+        <v>676</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="5" t="s">
         <v>203</v>
       </c>
     </row>
@@ -8064,7 +8236,7 @@
       <c r="A21" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="5" t="s">
         <v>203</v>
       </c>
     </row>
@@ -8072,7 +8244,7 @@
       <c r="A22" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="5" t="s">
         <v>203</v>
       </c>
     </row>
@@ -8080,7 +8252,7 @@
       <c r="A23" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="5" t="s">
         <v>203</v>
       </c>
     </row>
@@ -8093,7 +8265,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B311E26-48F5-445F-A976-490D3902A0D5}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -8117,10 +8289,10 @@
     </row>
     <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>528</v>
+        <v>500</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>529</v>
+        <v>501</v>
       </c>
       <c r="C2" t="s">
         <v>165</v>
@@ -8128,10 +8300,10 @@
     </row>
     <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>530</v>
+        <v>502</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>538</v>
+        <v>510</v>
       </c>
       <c r="C3" t="s">
         <v>165</v>
@@ -8139,10 +8311,10 @@
     </row>
     <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>531</v>
+        <v>503</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>539</v>
+        <v>511</v>
       </c>
       <c r="C4" t="s">
         <v>165</v>
@@ -8150,10 +8322,10 @@
     </row>
     <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>540</v>
+        <v>512</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>532</v>
+        <v>504</v>
       </c>
       <c r="C5" t="s">
         <v>165</v>
@@ -8161,10 +8333,10 @@
     </row>
     <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>541</v>
+        <v>513</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>542</v>
+        <v>514</v>
       </c>
       <c r="C6" t="s">
         <v>165</v>
@@ -8172,57 +8344,57 @@
     </row>
     <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>710</v>
+        <v>678</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>533</v>
+        <v>505</v>
       </c>
       <c r="C7" t="s">
-        <v>487</v>
+        <v>459</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>534</v>
+        <v>506</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>543</v>
+        <v>515</v>
       </c>
       <c r="C8" t="s">
-        <v>487</v>
+        <v>459</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>535</v>
+        <v>507</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>546</v>
+        <v>518</v>
       </c>
       <c r="C9" t="s">
-        <v>487</v>
+        <v>459</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>536</v>
+        <v>508</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>545</v>
+        <v>517</v>
       </c>
       <c r="C10" t="s">
-        <v>487</v>
+        <v>459</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>537</v>
+        <v>509</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>544</v>
+        <v>516</v>
       </c>
       <c r="C11" t="s">
-        <v>487</v>
+        <v>459</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -8238,7 +8410,7 @@
         <v>236</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>711</v>
+        <v>679</v>
       </c>
     </row>
   </sheetData>
@@ -8270,7 +8442,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>377</v>
+        <v>351</v>
       </c>
       <c r="B2">
         <v>50</v>
@@ -8278,7 +8450,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>378</v>
+        <v>352</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -8286,7 +8458,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>379</v>
+        <v>353</v>
       </c>
       <c r="B4">
         <v>137</v>
@@ -8294,7 +8466,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>380</v>
+        <v>354</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -8313,7 +8485,7 @@
         <v>236</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>712</v>
+        <v>680</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -8321,7 +8493,7 @@
         <v>235</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>559</v>
+        <v>530</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -8385,7 +8557,7 @@
     </row>
     <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>381</v>
+        <v>355</v>
       </c>
       <c r="B2">
         <v>182</v>
@@ -8393,7 +8565,7 @@
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>382</v>
+        <v>356</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -8401,7 +8573,7 @@
     </row>
     <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>383</v>
+        <v>357</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -8409,7 +8581,7 @@
     </row>
     <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>384</v>
+        <v>358</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -8417,7 +8589,7 @@
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>385</v>
+        <v>359</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -8425,7 +8597,7 @@
     </row>
     <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>386</v>
+        <v>360</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -8433,7 +8605,7 @@
     </row>
     <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>387</v>
+        <v>361</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -8441,7 +8613,7 @@
     </row>
     <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>388</v>
+        <v>362</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -8460,7 +8632,7 @@
         <v>236</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>713</v>
+        <v>681</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -8468,7 +8640,7 @@
         <v>235</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>436</v>
+        <v>409</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -8512,7 +8684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8ED044F-2B62-42B7-A288-F87892E20B00}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -8533,7 +8705,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>608</v>
+        <v>579</v>
       </c>
       <c r="B2">
         <v>36</v>
@@ -8541,7 +8713,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>607</v>
+        <v>578</v>
       </c>
       <c r="B3">
         <v>34</v>
@@ -8549,7 +8721,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>609</v>
+        <v>580</v>
       </c>
       <c r="B4">
         <v>31</v>
@@ -8557,7 +8729,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>498</v>
+        <v>470</v>
       </c>
       <c r="B5">
         <v>356</v>
@@ -8565,7 +8737,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>610</v>
+        <v>581</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -8573,7 +8745,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>611</v>
+        <v>582</v>
       </c>
       <c r="B7">
         <v>36</v>
@@ -8581,7 +8753,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>612</v>
+        <v>583</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -8589,7 +8761,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>499</v>
+        <v>471</v>
       </c>
       <c r="B9">
         <v>31</v>
@@ -8597,7 +8769,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>500</v>
+        <v>472</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -8616,7 +8788,7 @@
         <v>236</v>
       </c>
       <c r="B12" t="s">
-        <v>645</v>
+        <v>710</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -8624,7 +8796,7 @@
         <v>235</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>643</v>
+        <v>613</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -8677,7 +8849,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8696,7 +8868,7 @@
     </row>
     <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>437</v>
+        <v>410</v>
       </c>
       <c r="B2">
         <v>33</v>
@@ -8704,7 +8876,7 @@
     </row>
     <row r="3" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>438</v>
+        <v>411</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -8712,7 +8884,7 @@
     </row>
     <row r="4" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>439</v>
+        <v>412</v>
       </c>
       <c r="B4">
         <v>8</v>
@@ -8720,7 +8892,7 @@
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -8739,7 +8911,7 @@
         <v>236</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>714</v>
+        <v>682</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -8747,7 +8919,7 @@
         <v>235</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>441</v>
+        <v>711</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -8816,10 +8988,10 @@
     </row>
     <row r="2" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>443</v>
+        <v>415</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>444</v>
+        <v>416</v>
       </c>
       <c r="C2" t="s">
         <v>165</v>
@@ -8827,10 +8999,10 @@
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>389</v>
+        <v>363</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>442</v>
+        <v>414</v>
       </c>
       <c r="C3" t="s">
         <v>165</v>
@@ -8852,7 +9024,7 @@
         <v>236</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>715</v>
+        <v>683</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -8896,8 +9068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F6BE80-AC56-42ED-87D6-9266FD24F810}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8916,15 +9088,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>445</v>
+        <v>417</v>
       </c>
       <c r="B2" t="s">
-        <v>739</v>
+        <v>707</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>446</v>
+        <v>418</v>
       </c>
       <c r="B3">
         <v>76</v>
@@ -8932,7 +9104,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>447</v>
+        <v>419</v>
       </c>
       <c r="B4">
         <v>216</v>
@@ -8940,7 +9112,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>448</v>
+        <v>420</v>
       </c>
       <c r="B5">
         <v>129</v>
@@ -8948,7 +9120,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>449</v>
+        <v>421</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -8956,7 +9128,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>450</v>
+        <v>422</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -8964,7 +9136,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>451</v>
+        <v>423</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -8972,7 +9144,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>452</v>
+        <v>424</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -8991,7 +9163,7 @@
         <v>236</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>719</v>
+        <v>687</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -8999,7 +9171,7 @@
         <v>235</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>740</v>
+        <v>708</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -9043,8 +9215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA74624B-4AE3-43E9-9C9C-696C43DB0CE5}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9063,7 +9235,7 @@
     </row>
     <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -9071,7 +9243,7 @@
     </row>
     <row r="3" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
       <c r="B3">
         <v>33</v>
@@ -9079,7 +9251,7 @@
     </row>
     <row r="4" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>455</v>
+        <v>427</v>
       </c>
       <c r="B4">
         <v>31</v>
@@ -9087,7 +9259,7 @@
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>456</v>
+        <v>428</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -9095,7 +9267,7 @@
     </row>
     <row r="6" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>457</v>
+        <v>429</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -9103,7 +9275,7 @@
     </row>
     <row r="7" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>458</v>
+        <v>430</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -9111,7 +9283,7 @@
     </row>
     <row r="8" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>459</v>
+        <v>431</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -9130,7 +9302,7 @@
         <v>236</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>718</v>
+        <v>686</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -9138,7 +9310,7 @@
         <v>235</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>717</v>
+        <v>685</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -9206,90 +9378,90 @@
     </row>
     <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>558</v>
+        <v>529</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>551</v>
+        <v>522</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>487</v>
+        <v>459</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>488</v>
+        <v>460</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>552</v>
+        <v>523</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>487</v>
+        <v>459</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>489</v>
+        <v>461</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>553</v>
+        <v>524</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>487</v>
+        <v>459</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>490</v>
+        <v>462</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>554</v>
+        <v>525</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>487</v>
+        <v>459</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>491</v>
+        <v>463</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>555</v>
+        <v>526</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>487</v>
+        <v>459</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>492</v>
+        <v>464</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>556</v>
+        <v>527</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>487</v>
+        <v>459</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>493</v>
+        <v>465</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>557</v>
+        <v>528</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>487</v>
+        <v>459</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>619</v>
+        <v>590</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>592</v>
+        <v>563</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>487</v>
+        <v>459</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -9305,7 +9477,7 @@
         <v>236</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>716</v>
+        <v>684</v>
       </c>
     </row>
   </sheetData>
@@ -9492,7 +9664,7 @@
         <v>236</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>646</v>
+        <v>615</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -9500,7 +9672,7 @@
         <v>235</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>642</v>
+        <v>612</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -9546,7 +9718,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9565,10 +9737,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>631</v>
+        <v>602</v>
       </c>
       <c r="B2" t="s">
-        <v>632</v>
+        <v>603</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -9584,7 +9756,7 @@
         <v>236</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>633</v>
+        <v>604</v>
       </c>
     </row>
   </sheetData>
@@ -9617,7 +9789,7 @@
     </row>
     <row r="2" spans="1:2" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>622</v>
+        <v>593</v>
       </c>
       <c r="B2" s="5">
         <v>3338</v>
@@ -9625,7 +9797,7 @@
     </row>
     <row r="3" spans="1:2" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>621</v>
+        <v>592</v>
       </c>
       <c r="B3" s="13">
         <v>1038</v>
@@ -9636,7 +9808,7 @@
         <v>241</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>567</v>
+        <v>538</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -9644,7 +9816,7 @@
         <v>236</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>649</v>
+        <v>618</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -9652,7 +9824,7 @@
         <v>235</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>570</v>
+        <v>541</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -9716,7 +9888,7 @@
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>623</v>
+        <v>594</v>
       </c>
       <c r="B2" s="13">
         <v>2502</v>
@@ -9724,7 +9896,7 @@
     </row>
     <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>624</v>
+        <v>595</v>
       </c>
       <c r="B3" s="5">
         <v>851</v>
@@ -9735,7 +9907,7 @@
         <v>241</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>567</v>
+        <v>538</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -9743,7 +9915,7 @@
         <v>236</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>648</v>
+        <v>617</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -9751,7 +9923,7 @@
         <v>235</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>569</v>
+        <v>540</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -9815,7 +9987,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>625</v>
+        <v>596</v>
       </c>
       <c r="B2" s="5">
         <v>401</v>
@@ -9823,7 +9995,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>626</v>
+        <v>597</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
@@ -9831,7 +10003,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>627</v>
+        <v>598</v>
       </c>
       <c r="B4" s="5">
         <v>145</v>
@@ -9839,7 +10011,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>628</v>
+        <v>599</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>
@@ -9850,7 +10022,7 @@
         <v>241</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>567</v>
+        <v>538</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -9858,7 +10030,7 @@
         <v>236</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>650</v>
+        <v>619</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -9866,7 +10038,7 @@
         <v>235</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>568</v>
+        <v>539</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fixed bug for unanswered questions
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDS_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDS_2020_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\RHIT_IRPA_@\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE45F6C9-9486-4558-B247-69631781E44A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1187F9-6DD9-4605-8D01-E27C53FC2B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="19" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="23" r:id="rId1"/>
@@ -1189,9 +1189,6 @@
     <t>The areas in which all or most students are requried to complete some course work prior to graduation are the following: computer literacy, English(including composition), Humanities, Mathematics, Sciences(biological or physical) and Social science</t>
   </si>
   <si>
-    <t>The number of [gender] transfer applicants that are [action] is &lt;value&gt;</t>
-  </si>
-  <si>
     <t>Rose-Hulman's mailing address is 5500 Wabash Ave, Terre Haute, IN 47803</t>
   </si>
   <si>
@@ -2390,6 +2387,9 @@
   </si>
   <si>
     <t>There is no available information on the average amount of institutional non-need-based athletic scholarships and grants awarded to degree-seeking part-time undergraduate students.</t>
+  </si>
+  <si>
+    <t>The number of [gender] transfer applicants that are [^action] is &lt;value&gt;</t>
   </si>
 </sst>
 </file>
@@ -2793,7 +2793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E422E2F-D9FA-411F-968E-DE340F994DF5}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -2820,7 +2820,7 @@
         <v>340</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C2" t="s">
         <v>165</v>
@@ -2828,10 +2828,10 @@
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>371</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>372</v>
       </c>
       <c r="C3" t="s">
         <v>165</v>
@@ -2842,7 +2842,7 @@
         <v>342</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C4" t="s">
         <v>165</v>
@@ -2853,7 +2853,7 @@
         <v>341</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C5" t="s">
         <v>165</v>
@@ -2864,7 +2864,7 @@
         <v>343</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C6" t="s">
         <v>165</v>
@@ -2875,7 +2875,7 @@
         <v>344</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C7" t="s">
         <v>165</v>
@@ -2886,7 +2886,7 @@
         <v>345</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C8" t="s">
         <v>165</v>
@@ -2894,10 +2894,10 @@
     </row>
     <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>378</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>379</v>
       </c>
       <c r="C9" t="s">
         <v>165</v>
@@ -2908,7 +2908,7 @@
         <v>346</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C10" t="s">
         <v>165</v>
@@ -2919,7 +2919,7 @@
         <v>347</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C11" t="s">
         <v>165</v>
@@ -2930,7 +2930,7 @@
         <v>348</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C12" t="s">
         <v>165</v>
@@ -2941,7 +2941,7 @@
         <v>349</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C13" t="s">
         <v>165</v>
@@ -2952,7 +2952,7 @@
         <v>350</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C14" t="s">
         <v>165</v>
@@ -2971,7 +2971,7 @@
         <v>236</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -3039,10 +3039,10 @@
     </row>
     <row r="2" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C2" t="s">
         <v>165</v>
@@ -3050,10 +3050,10 @@
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C3" t="s">
         <v>165</v>
@@ -3061,10 +3061,10 @@
     </row>
     <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
+        <v>532</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>533</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>534</v>
       </c>
       <c r="C4" t="s">
         <v>165</v>
@@ -3072,10 +3072,10 @@
     </row>
     <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
+        <v>534</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>535</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>536</v>
       </c>
       <c r="C5" t="s">
         <v>165</v>
@@ -3086,7 +3086,7 @@
         <v>241</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
@@ -3094,7 +3094,7 @@
         <v>236</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
   </sheetData>
@@ -3130,7 +3130,7 @@
     </row>
     <row r="2" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B2" s="5">
         <v>4</v>
@@ -3141,7 +3141,7 @@
     </row>
     <row r="3" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B3" s="5">
         <v>4</v>
@@ -3152,7 +3152,7 @@
     </row>
     <row r="4" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B4" s="5">
         <v>3</v>
@@ -3163,7 +3163,7 @@
     </row>
     <row r="5" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B5" s="5">
         <v>3</v>
@@ -3174,7 +3174,7 @@
     </row>
     <row r="6" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B6" s="5">
         <v>0</v>
@@ -3185,7 +3185,7 @@
     </row>
     <row r="7" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B7" s="5">
         <v>2</v>
@@ -3196,7 +3196,7 @@
     </row>
     <row r="8" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -3207,7 +3207,7 @@
     </row>
     <row r="9" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B9" s="5">
         <v>0</v>
@@ -3218,7 +3218,7 @@
     </row>
     <row r="10" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B10" s="5">
         <v>0</v>
@@ -3229,7 +3229,7 @@
     </row>
     <row r="11" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B11" s="5">
         <v>0</v>
@@ -3240,7 +3240,7 @@
     </row>
     <row r="12" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B12" s="5">
         <v>0</v>
@@ -3251,10 +3251,10 @@
     </row>
     <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
+        <v>466</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>467</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>468</v>
       </c>
       <c r="C13" t="s">
         <v>165</v>
@@ -3273,7 +3273,7 @@
         <v>236</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -3281,7 +3281,7 @@
         <v>235</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -3346,7 +3346,7 @@
     </row>
     <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3354,7 +3354,7 @@
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -3362,7 +3362,7 @@
     </row>
     <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -3370,7 +3370,7 @@
     </row>
     <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -3378,7 +3378,7 @@
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -3386,7 +3386,7 @@
     </row>
     <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -3394,7 +3394,7 @@
     </row>
     <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -3402,7 +3402,7 @@
     </row>
     <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -3410,7 +3410,7 @@
     </row>
     <row r="10" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -3418,7 +3418,7 @@
     </row>
     <row r="11" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -3426,7 +3426,7 @@
     </row>
     <row r="12" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -3445,7 +3445,7 @@
         <v>236</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -3453,7 +3453,7 @@
         <v>235</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -3651,7 +3651,7 @@
         <v>236</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
   </sheetData>
@@ -3687,7 +3687,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -3695,7 +3695,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -3703,7 +3703,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3711,7 +3711,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -3719,7 +3719,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3727,7 +3727,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -3735,7 +3735,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3743,7 +3743,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3751,7 +3751,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3759,7 +3759,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3767,7 +3767,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -3775,7 +3775,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3783,7 +3783,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -3791,7 +3791,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3799,7 +3799,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -3807,7 +3807,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -3815,7 +3815,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -3823,7 +3823,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3831,7 +3831,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3847,7 +3847,7 @@
         <v>236</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3855,7 +3855,7 @@
         <v>235</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -3888,42 +3888,42 @@
     </row>
     <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -3939,7 +3939,7 @@
         <v>236</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
   </sheetData>
@@ -4031,7 +4031,7 @@
         <v>236</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -4039,7 +4039,7 @@
         <v>235</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -4210,7 +4210,7 @@
         <v>236</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -4218,7 +4218,7 @@
         <v>235</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -4345,7 +4345,7 @@
         <v>236</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -4353,7 +4353,7 @@
         <v>235</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -4524,7 +4524,7 @@
         <v>236</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -4532,7 +4532,7 @@
         <v>235</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -4543,7 +4543,7 @@
         <v>165</v>
       </c>
       <c r="D17" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -4600,7 +4600,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B2" s="5">
         <v>387</v>
@@ -4608,7 +4608,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B3" s="5">
         <v>143</v>
@@ -4616,7 +4616,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B4" s="5">
         <v>1</v>
@@ -4624,7 +4624,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>
@@ -4632,7 +4632,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B6" s="5">
         <v>9</v>
@@ -4640,7 +4640,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B7" s="5">
         <v>2</v>
@@ -4648,7 +4648,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -4656,7 +4656,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B9" s="5">
         <v>0</v>
@@ -4664,7 +4664,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B10" s="5">
         <v>1082</v>
@@ -4672,7 +4672,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B11" s="5">
         <v>329</v>
@@ -4680,7 +4680,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B12" s="5">
         <v>15</v>
@@ -4688,7 +4688,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B13" s="5">
         <v>1</v>
@@ -4835,7 +4835,7 @@
         <v>236</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -4843,7 +4843,7 @@
         <v>235</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -4908,7 +4908,7 @@
     </row>
     <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>53</v>
@@ -4916,7 +4916,7 @@
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>54</v>
@@ -4924,7 +4924,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B4" s="6">
         <v>350</v>
@@ -4932,10 +4932,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -4951,7 +4951,7 @@
         <v>236</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -4959,7 +4959,7 @@
         <v>235</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -5165,7 +5165,7 @@
         <v>24</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -5293,7 +5293,7 @@
         <v>236</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -5301,7 +5301,7 @@
         <v>235</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -5370,7 +5370,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>91</v>
@@ -5381,7 +5381,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>92</v>
@@ -5392,7 +5392,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>93</v>
@@ -5403,7 +5403,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>94</v>
@@ -5414,7 +5414,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>95</v>
@@ -5425,7 +5425,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>96</v>
@@ -5436,7 +5436,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>102</v>
@@ -5447,7 +5447,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>102</v>
@@ -5458,7 +5458,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>102</v>
@@ -5469,10 +5469,10 @@
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C11" t="s">
         <v>165</v>
@@ -5480,10 +5480,10 @@
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C12" t="s">
         <v>165</v>
@@ -5502,7 +5502,7 @@
         <v>236</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -5510,7 +5510,7 @@
         <v>235</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -5578,7 +5578,7 @@
     </row>
     <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>115</v>
@@ -5586,7 +5586,7 @@
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>116</v>
@@ -5594,7 +5594,7 @@
     </row>
     <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>117</v>
@@ -5602,7 +5602,7 @@
     </row>
     <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>118</v>
@@ -5610,7 +5610,7 @@
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>102</v>
@@ -5618,7 +5618,7 @@
     </row>
     <row r="7" spans="1:2" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>119</v>
@@ -5637,7 +5637,7 @@
         <v>236</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -5645,7 +5645,7 @@
         <v>235</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -5689,8 +5689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{869E4568-D908-477D-923D-F4116B90EDC7}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5710,7 +5710,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B2" s="6">
         <v>59</v>
@@ -5718,7 +5718,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B3" s="6">
         <v>30</v>
@@ -5726,7 +5726,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B4" s="6">
         <v>9</v>
@@ -5734,7 +5734,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B5" s="6">
         <v>23</v>
@@ -5742,7 +5742,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B6" s="6">
         <v>13</v>
@@ -5750,7 +5750,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B7" s="6">
         <v>2</v>
@@ -5769,7 +5769,7 @@
         <v>236</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -5777,7 +5777,7 @@
         <v>235</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>369</v>
+        <v>767</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -5867,7 +5867,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>130</v>
@@ -5886,10 +5886,10 @@
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
+        <v>651</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>652</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>653</v>
       </c>
       <c r="C6" t="s">
         <v>165</v>
@@ -5897,10 +5897,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C7" t="s">
         <v>165</v>
@@ -5908,10 +5908,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C8" t="s">
         <v>165</v>
@@ -5919,10 +5919,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C9" t="s">
         <v>165</v>
@@ -5930,7 +5930,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>132</v>
@@ -5941,7 +5941,7 @@
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>133</v>
@@ -5952,10 +5952,10 @@
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C12" t="s">
         <v>165</v>
@@ -5963,7 +5963,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>266</v>
@@ -5996,7 +5996,7 @@
     </row>
     <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>136</v>
@@ -6084,7 +6084,7 @@
         <v>236</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -6185,7 +6185,7 @@
         <v>236</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -6260,7 +6260,7 @@
         <v>143</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C2" t="s">
         <v>165</v>
@@ -6271,7 +6271,7 @@
         <v>146</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C3" t="s">
         <v>165</v>
@@ -6282,7 +6282,7 @@
         <v>147</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C4" t="s">
         <v>165</v>
@@ -6356,7 +6356,7 @@
         <v>236</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -6424,7 +6424,7 @@
         <v>144</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -6432,7 +6432,7 @@
         <v>145</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -6440,7 +6440,7 @@
         <v>148</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
@@ -6496,7 +6496,7 @@
         <v>236</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -6631,7 +6631,7 @@
         <v>236</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -6695,7 +6695,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B2" s="5">
         <v>226</v>
@@ -6703,7 +6703,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B3" s="5">
         <v>104</v>
@@ -6711,7 +6711,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B4" s="5">
         <v>93</v>
@@ -6719,7 +6719,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B5" s="5">
         <v>1295</v>
@@ -6727,7 +6727,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B6" s="5">
         <v>3</v>
@@ -6735,7 +6735,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B7" s="5">
         <v>127</v>
@@ -6743,7 +6743,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -6778,7 +6778,7 @@
         <v>236</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -6786,7 +6786,7 @@
         <v>235</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -6826,7 +6826,7 @@
         <v>262</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
   </sheetData>
@@ -6859,101 +6859,101 @@
     </row>
     <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>476</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>477</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
+        <v>697</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>698</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>699</v>
-      </c>
       <c r="C3" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -6969,7 +6969,7 @@
         <v>236</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
   </sheetData>
@@ -7003,79 +7003,79 @@
     </row>
     <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -7091,7 +7091,7 @@
         <v>236</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
   </sheetData>
@@ -7124,35 +7124,35 @@
     </row>
     <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -7168,7 +7168,7 @@
         <v>236</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
   </sheetData>
@@ -7303,10 +7303,10 @@
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C11" t="s">
         <v>165</v>
@@ -7314,10 +7314,10 @@
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C12" t="s">
         <v>165</v>
@@ -7325,7 +7325,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>332</v>
@@ -7336,7 +7336,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>326</v>
@@ -7347,7 +7347,7 @@
     </row>
     <row r="15" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>326</v>
@@ -7358,7 +7358,7 @@
     </row>
     <row r="16" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>326</v>
@@ -7372,7 +7372,7 @@
         <v>280</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="C17" t="s">
         <v>165</v>
@@ -7383,7 +7383,7 @@
         <v>281</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="C18" t="s">
         <v>165</v>
@@ -7446,7 +7446,7 @@
         <v>236</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -7454,7 +7454,7 @@
         <v>235</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -7523,10 +7523,10 @@
     </row>
     <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>718</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>719</v>
       </c>
       <c r="C2" t="s">
         <v>165</v>
@@ -7537,7 +7537,7 @@
         <v>282</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C3" t="s">
         <v>165</v>
@@ -7548,7 +7548,7 @@
         <v>283</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C4" t="s">
         <v>165</v>
@@ -7559,7 +7559,7 @@
         <v>284</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="C5" t="s">
         <v>165</v>
@@ -7570,7 +7570,7 @@
         <v>285</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="C6" t="s">
         <v>165</v>
@@ -7581,7 +7581,7 @@
         <v>286</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C7" t="s">
         <v>165</v>
@@ -7592,7 +7592,7 @@
         <v>287</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C8" t="s">
         <v>165</v>
@@ -7603,7 +7603,7 @@
         <v>288</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C9" t="s">
         <v>165</v>
@@ -7614,7 +7614,7 @@
         <v>289</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C10" t="s">
         <v>165</v>
@@ -7622,10 +7622,10 @@
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="C11" t="s">
         <v>165</v>
@@ -7636,7 +7636,7 @@
         <v>290</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C12" t="s">
         <v>165</v>
@@ -7644,10 +7644,10 @@
     </row>
     <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C13" t="s">
         <v>165</v>
@@ -7658,7 +7658,7 @@
         <v>292</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C14" t="s">
         <v>165</v>
@@ -7669,7 +7669,7 @@
         <v>295</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="C15" t="s">
         <v>165</v>
@@ -7680,7 +7680,7 @@
         <v>293</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C16" t="s">
         <v>165</v>
@@ -7691,7 +7691,7 @@
         <v>294</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C17" t="s">
         <v>165</v>
@@ -7710,7 +7710,7 @@
         <v>236</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -7782,7 +7782,7 @@
         <v>296</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C2" t="s">
         <v>165</v>
@@ -7793,7 +7793,7 @@
         <v>297</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="C3" t="s">
         <v>165</v>
@@ -7804,7 +7804,7 @@
         <v>298</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="C4" t="s">
         <v>165</v>
@@ -7815,7 +7815,7 @@
         <v>299</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="C5" t="s">
         <v>165</v>
@@ -7826,7 +7826,7 @@
         <v>300</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="C6" t="s">
         <v>165</v>
@@ -7837,7 +7837,7 @@
         <v>301</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="C7" t="s">
         <v>165</v>
@@ -7848,7 +7848,7 @@
         <v>302</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C8" t="s">
         <v>165</v>
@@ -7859,7 +7859,7 @@
         <v>303</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="C9" t="s">
         <v>165</v>
@@ -7870,7 +7870,7 @@
         <v>304</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C10" t="s">
         <v>165</v>
@@ -7881,7 +7881,7 @@
         <v>305</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C11" t="s">
         <v>165</v>
@@ -7892,7 +7892,7 @@
         <v>306</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="C12" t="s">
         <v>165</v>
@@ -7900,10 +7900,10 @@
     </row>
     <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C13" t="s">
         <v>165</v>
@@ -7914,7 +7914,7 @@
         <v>307</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C14" t="s">
         <v>165</v>
@@ -7925,7 +7925,7 @@
         <v>308</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="C15" t="s">
         <v>165</v>
@@ -7936,7 +7936,7 @@
         <v>309</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C16" t="s">
         <v>165</v>
@@ -7966,7 +7966,7 @@
         <v>236</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -8037,7 +8037,7 @@
         <v>311</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="C2" t="s">
         <v>165</v>
@@ -8048,7 +8048,7 @@
         <v>312</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="C3" t="s">
         <v>165</v>
@@ -8059,7 +8059,7 @@
         <v>313</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="C4" t="s">
         <v>165</v>
@@ -8070,7 +8070,7 @@
         <v>314</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="C5" t="s">
         <v>165</v>
@@ -8081,7 +8081,7 @@
         <v>315</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C6" t="s">
         <v>165</v>
@@ -8092,7 +8092,7 @@
         <v>316</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="C7" t="s">
         <v>165</v>
@@ -8103,7 +8103,7 @@
         <v>317</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="C8" t="s">
         <v>165</v>
@@ -8114,7 +8114,7 @@
         <v>318</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="C9" t="s">
         <v>165</v>
@@ -8125,7 +8125,7 @@
         <v>319</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="C10" t="s">
         <v>165</v>
@@ -8136,7 +8136,7 @@
         <v>320</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C11" t="s">
         <v>165</v>
@@ -8147,7 +8147,7 @@
         <v>321</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C12" t="s">
         <v>165</v>
@@ -8158,7 +8158,7 @@
         <v>291</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C13" t="s">
         <v>165</v>
@@ -8169,7 +8169,7 @@
         <v>322</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="C14" t="s">
         <v>165</v>
@@ -8180,7 +8180,7 @@
         <v>323</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C15" t="s">
         <v>165</v>
@@ -8191,7 +8191,7 @@
         <v>324</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C16" t="s">
         <v>165</v>
@@ -8199,10 +8199,10 @@
     </row>
     <row r="17" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
+        <v>765</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>766</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>767</v>
       </c>
       <c r="C17" t="s">
         <v>165</v>
@@ -8221,7 +8221,7 @@
         <v>236</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -8289,10 +8289,10 @@
     </row>
     <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>499</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>500</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>501</v>
       </c>
       <c r="C2" t="s">
         <v>165</v>
@@ -8300,10 +8300,10 @@
     </row>
     <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C3" t="s">
         <v>165</v>
@@ -8311,10 +8311,10 @@
     </row>
     <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C4" t="s">
         <v>165</v>
@@ -8322,10 +8322,10 @@
     </row>
     <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C5" t="s">
         <v>165</v>
@@ -8333,10 +8333,10 @@
     </row>
     <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
+        <v>512</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>513</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>514</v>
       </c>
       <c r="C6" t="s">
         <v>165</v>
@@ -8344,57 +8344,57 @@
     </row>
     <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C7" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C8" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C9" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C10" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C11" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -8410,7 +8410,7 @@
         <v>236</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
   </sheetData>
@@ -8485,7 +8485,7 @@
         <v>236</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -8493,7 +8493,7 @@
         <v>235</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -8632,7 +8632,7 @@
         <v>236</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -8640,7 +8640,7 @@
         <v>235</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -8705,7 +8705,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B2">
         <v>36</v>
@@ -8713,7 +8713,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B3">
         <v>34</v>
@@ -8721,7 +8721,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B4">
         <v>31</v>
@@ -8729,7 +8729,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B5">
         <v>356</v>
@@ -8737,7 +8737,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -8745,7 +8745,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B7">
         <v>36</v>
@@ -8753,7 +8753,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -8761,7 +8761,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B9">
         <v>31</v>
@@ -8769,7 +8769,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -8788,7 +8788,7 @@
         <v>236</v>
       </c>
       <c r="B12" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -8796,7 +8796,7 @@
         <v>235</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -8868,7 +8868,7 @@
     </row>
     <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B2">
         <v>33</v>
@@ -8876,7 +8876,7 @@
     </row>
     <row r="3" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -8884,7 +8884,7 @@
     </row>
     <row r="4" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B4">
         <v>8</v>
@@ -8892,7 +8892,7 @@
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -8911,7 +8911,7 @@
         <v>236</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -8919,7 +8919,7 @@
         <v>235</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -8988,10 +8988,10 @@
     </row>
     <row r="2" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>415</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>416</v>
       </c>
       <c r="C2" t="s">
         <v>165</v>
@@ -9002,7 +9002,7 @@
         <v>363</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C3" t="s">
         <v>165</v>
@@ -9024,7 +9024,7 @@
         <v>236</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -9088,15 +9088,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B2" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B3">
         <v>76</v>
@@ -9104,7 +9104,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B4">
         <v>216</v>
@@ -9112,7 +9112,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B5">
         <v>129</v>
@@ -9120,7 +9120,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -9128,7 +9128,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -9136,7 +9136,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -9144,7 +9144,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -9163,7 +9163,7 @@
         <v>236</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -9171,7 +9171,7 @@
         <v>235</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -9235,7 +9235,7 @@
     </row>
     <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -9243,7 +9243,7 @@
     </row>
     <row r="3" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B3">
         <v>33</v>
@@ -9251,7 +9251,7 @@
     </row>
     <row r="4" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B4">
         <v>31</v>
@@ -9259,7 +9259,7 @@
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -9267,7 +9267,7 @@
     </row>
     <row r="6" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -9275,7 +9275,7 @@
     </row>
     <row r="7" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -9283,7 +9283,7 @@
     </row>
     <row r="8" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -9302,7 +9302,7 @@
         <v>236</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -9310,7 +9310,7 @@
         <v>235</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -9378,90 +9378,90 @@
     </row>
     <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -9477,7 +9477,7 @@
         <v>236</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
   </sheetData>
@@ -9664,7 +9664,7 @@
         <v>236</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -9672,7 +9672,7 @@
         <v>235</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -9737,10 +9737,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>601</v>
+      </c>
+      <c r="B2" t="s">
         <v>602</v>
-      </c>
-      <c r="B2" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -9756,7 +9756,7 @@
         <v>236</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
   </sheetData>
@@ -9789,7 +9789,7 @@
     </row>
     <row r="2" spans="1:2" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B2" s="5">
         <v>3338</v>
@@ -9797,7 +9797,7 @@
     </row>
     <row r="3" spans="1:2" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B3" s="13">
         <v>1038</v>
@@ -9808,7 +9808,7 @@
         <v>241</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -9816,7 +9816,7 @@
         <v>236</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -9824,7 +9824,7 @@
         <v>235</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -9888,7 +9888,7 @@
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B2" s="13">
         <v>2502</v>
@@ -9896,7 +9896,7 @@
     </row>
     <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B3" s="5">
         <v>851</v>
@@ -9907,7 +9907,7 @@
         <v>241</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -9915,7 +9915,7 @@
         <v>236</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -9923,7 +9923,7 @@
         <v>235</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -9987,7 +9987,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B2" s="5">
         <v>401</v>
@@ -9995,7 +9995,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
@@ -10003,7 +10003,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B4" s="5">
         <v>145</v>
@@ -10011,7 +10011,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>
@@ -10022,7 +10022,7 @@
         <v>241</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -10030,7 +10030,7 @@
         <v>236</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -10038,7 +10038,7 @@
         <v>235</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updated cohort training data
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDS_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDS_2020_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\RHIT_IRPA_@\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02E57B1-5D28-47BA-AB7F-629E044DFF58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47913BAB-6FA2-423F-83ED-AB11A756DBA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="30" activeTab="32" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="23" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1517" uniqueCount="769">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="769">
   <si>
     <t>Answer</t>
   </si>
@@ -1318,9 +1318,6 @@
     <t>How many visual/performing art units are required for admission?</t>
   </si>
   <si>
-    <t>What other units are required for admission?</t>
-  </si>
-  <si>
     <t>How many English units are required for admission?</t>
   </si>
   <si>
@@ -1358,9 +1355,6 @@
   </si>
   <si>
     <t>How many visual/performing art units are recommended for admission?</t>
-  </si>
-  <si>
-    <t>What other units are recommended for admission?</t>
   </si>
   <si>
     <t>yes</t>
@@ -2393,6 +2387,12 @@
   </si>
   <si>
     <t>The (xor [^aggregation] [^percentile])  [^standarized_test] [^test_component] score for incoming freshmen is &lt;value&gt;</t>
+  </si>
+  <si>
+    <t>No other additional units are recommended for admission</t>
+  </si>
+  <si>
+    <t>What other units are recommended for admission? (please specify)</t>
   </si>
 </sst>
 </file>
@@ -2974,7 +2974,7 @@
         <v>204</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -3042,10 +3042,10 @@
     </row>
     <row r="2" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="C2" t="s">
         <v>133</v>
@@ -3053,10 +3053,10 @@
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C3" t="s">
         <v>133</v>
@@ -3064,10 +3064,10 @@
     </row>
     <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C4" t="s">
         <v>133</v>
@@ -3075,10 +3075,10 @@
     </row>
     <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C5" t="s">
         <v>133</v>
@@ -3089,7 +3089,7 @@
         <v>209</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
@@ -3097,7 +3097,7 @@
         <v>204</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
   </sheetData>
@@ -3107,10 +3107,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5DC138E-AAA1-4452-BC05-6992F74BED09}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="74" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView zoomScale="74" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3133,46 +3133,46 @@
     </row>
     <row r="2" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B2" s="5">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>133</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B3" s="5">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>133</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B4" s="5">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>133</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B5" s="5">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>133</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
@@ -3183,7 +3183,7 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>133</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
@@ -3194,7 +3194,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>133</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
@@ -3205,7 +3205,7 @@
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>133</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
@@ -3216,7 +3216,7 @@
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>133</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
@@ -3227,7 +3227,7 @@
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>133</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
@@ -3238,58 +3238,55 @@
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>411</v>
-      </c>
-      <c r="B12" s="5">
-        <v>0</v>
+        <v>432</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>433</v>
       </c>
       <c r="C12" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>434</v>
+        <v>209</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>435</v>
-      </c>
-      <c r="C13" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>204</v>
+        <v>581</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>203</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>505</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>171</v>
@@ -3297,7 +3294,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>171</v>
@@ -3305,17 +3302,9 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="B20" s="5" t="s">
         <v>171</v>
       </c>
     </row>
@@ -3327,115 +3316,152 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B50A1A77-FCFF-4BA2-80DC-49E66C3D11B3}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37.88671875" style="5" customWidth="1"/>
     <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="3" max="3" width="21.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>425</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <v>768</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>767</v>
+      </c>
+      <c r="C12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>209</v>
       </c>
@@ -3443,23 +3469,23 @@
         <v>207</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>204</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>203</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>205</v>
       </c>
@@ -3654,7 +3680,7 @@
         <v>204</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
   </sheetData>
@@ -3690,7 +3716,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -3698,7 +3724,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -3706,7 +3732,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3714,7 +3740,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -3722,7 +3748,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3730,7 +3756,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -3738,7 +3764,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3746,7 +3772,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3754,7 +3780,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3762,7 +3788,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3770,7 +3796,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -3778,7 +3804,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3786,7 +3812,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -3794,7 +3820,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3802,7 +3828,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -3810,7 +3836,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -3818,7 +3844,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -3826,7 +3852,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3834,7 +3860,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3850,7 +3876,7 @@
         <v>204</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3872,7 +3898,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3891,42 +3917,42 @@
     </row>
     <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
+        <v>649</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>651</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>653</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -3942,7 +3968,7 @@
         <v>204</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
     </row>
   </sheetData>
@@ -4034,7 +4060,7 @@
         <v>204</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -4042,7 +4068,7 @@
         <v>203</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -4213,7 +4239,7 @@
         <v>204</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -4221,7 +4247,7 @@
         <v>203</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -4270,7 +4296,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4348,7 +4374,7 @@
         <v>204</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -4356,7 +4382,7 @@
         <v>203</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -4527,7 +4553,7 @@
         <v>204</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -4535,7 +4561,7 @@
         <v>203</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -4546,7 +4572,7 @@
         <v>133</v>
       </c>
       <c r="D17" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -4603,7 +4629,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B2" s="5">
         <v>387</v>
@@ -4611,7 +4637,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B3" s="5">
         <v>143</v>
@@ -4619,7 +4645,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B4" s="5">
         <v>1</v>
@@ -4627,7 +4653,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>
@@ -4635,7 +4661,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B6" s="5">
         <v>9</v>
@@ -4643,7 +4669,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B7" s="5">
         <v>2</v>
@@ -4651,7 +4677,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -4659,7 +4685,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B9" s="5">
         <v>0</v>
@@ -4667,7 +4693,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B10" s="5">
         <v>1082</v>
@@ -4675,7 +4701,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B11" s="5">
         <v>329</v>
@@ -4683,7 +4709,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B12" s="5">
         <v>15</v>
@@ -4691,7 +4717,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B13" s="5">
         <v>1</v>
@@ -4838,7 +4864,7 @@
         <v>204</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -4846,7 +4872,7 @@
         <v>203</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -4938,7 +4964,7 @@
         <v>354</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -4954,7 +4980,7 @@
         <v>204</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -4962,7 +4988,7 @@
         <v>203</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -5008,7 +5034,7 @@
   <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView topLeftCell="A12" zoomScale="80" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5029,7 +5055,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="B2" s="6">
         <v>1270</v>
@@ -5037,7 +5063,7 @@
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B3" s="6">
         <v>610</v>
@@ -5045,7 +5071,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="B4" s="6">
         <v>650</v>
@@ -5053,7 +5079,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>232</v>
@@ -5061,7 +5087,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="B6" s="6">
         <v>1355</v>
@@ -5069,7 +5095,7 @@
     </row>
     <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="B7" s="6">
         <v>650</v>
@@ -5077,7 +5103,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="B8" s="6">
         <v>700</v>
@@ -5085,7 +5111,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>23</v>
@@ -5093,7 +5119,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="B10" s="6">
         <v>1440</v>
@@ -5101,7 +5127,7 @@
     </row>
     <row r="11" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="B11" s="6">
         <v>700</v>
@@ -5109,7 +5135,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="B12" s="6">
         <v>760</v>
@@ -5117,7 +5143,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="B13" s="6">
         <v>1352</v>
@@ -5125,7 +5151,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="B14" s="6">
         <v>1352</v>
@@ -5133,7 +5159,7 @@
     </row>
     <row r="15" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="B15" s="6">
         <v>652</v>
@@ -5141,7 +5167,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="B16" s="6">
         <v>700</v>
@@ -5149,7 +5175,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>306</v>
@@ -5157,7 +5183,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="B18" s="6">
         <v>27</v>
@@ -5165,15 +5191,15 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B20" s="6">
         <v>26</v>
@@ -5181,15 +5207,15 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B22" s="6">
         <v>31</v>
@@ -5197,7 +5223,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="B23" s="6">
         <v>31</v>
@@ -5205,7 +5231,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="B24" s="6">
         <v>31.5</v>
@@ -5213,7 +5239,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>306</v>
@@ -5221,7 +5247,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="B26" s="6">
         <v>33</v>
@@ -5229,7 +5255,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="B27" s="6">
         <v>34</v>
@@ -5237,7 +5263,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="B28" s="6">
         <v>35</v>
@@ -5245,7 +5271,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>306</v>
@@ -5253,7 +5279,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="B30" s="6">
         <v>30</v>
@@ -5261,7 +5287,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="B31" s="6">
         <v>30</v>
@@ -5269,7 +5295,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="B32" s="6">
         <v>30</v>
@@ -5277,7 +5303,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>306</v>
@@ -5296,7 +5322,7 @@
         <v>204</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -5304,7 +5330,7 @@
         <v>203</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -5373,7 +5399,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>59</v>
@@ -5505,7 +5531,7 @@
         <v>204</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -5513,7 +5539,7 @@
         <v>203</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -5640,7 +5666,7 @@
         <v>204</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -5648,7 +5674,7 @@
         <v>203</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -5713,7 +5739,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B2" s="6">
         <v>59</v>
@@ -5721,7 +5747,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B3" s="6">
         <v>30</v>
@@ -5729,7 +5755,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B4" s="6">
         <v>9</v>
@@ -5737,7 +5763,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B5" s="6">
         <v>23</v>
@@ -5745,7 +5771,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B6" s="6">
         <v>13</v>
@@ -5753,7 +5779,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B7" s="6">
         <v>2</v>
@@ -5772,7 +5798,7 @@
         <v>204</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -5780,7 +5806,7 @@
         <v>203</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -5870,7 +5896,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>98</v>
@@ -5889,10 +5915,10 @@
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="C6" t="s">
         <v>133</v>
@@ -5900,10 +5926,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C7" t="s">
         <v>133</v>
@@ -5911,10 +5937,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="C8" t="s">
         <v>133</v>
@@ -5922,10 +5948,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="C9" t="s">
         <v>133</v>
@@ -5933,7 +5959,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>100</v>
@@ -5944,7 +5970,7 @@
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>101</v>
@@ -5955,10 +5981,10 @@
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="C12" t="s">
         <v>133</v>
@@ -5966,7 +5992,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>234</v>
@@ -5999,7 +6025,7 @@
     </row>
     <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>104</v>
@@ -6087,7 +6113,7 @@
         <v>204</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -6188,7 +6214,7 @@
         <v>204</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -6263,7 +6289,7 @@
         <v>111</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C2" t="s">
         <v>133</v>
@@ -6274,7 +6300,7 @@
         <v>114</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="C3" t="s">
         <v>133</v>
@@ -6285,7 +6311,7 @@
         <v>115</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="C4" t="s">
         <v>133</v>
@@ -6359,7 +6385,7 @@
         <v>204</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -6403,8 +6429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD1BC2B9-A383-49AB-870B-3568000F0DBB}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6427,7 +6453,7 @@
         <v>112</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -6435,7 +6461,7 @@
         <v>113</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -6443,7 +6469,7 @@
         <v>116</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
@@ -6499,7 +6525,7 @@
         <v>204</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -6634,7 +6660,7 @@
         <v>204</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -6698,7 +6724,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B2" s="5">
         <v>226</v>
@@ -6706,7 +6732,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B3" s="5">
         <v>104</v>
@@ -6714,7 +6740,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B4" s="5">
         <v>93</v>
@@ -6722,7 +6748,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B5" s="5">
         <v>1295</v>
@@ -6730,7 +6756,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B6" s="5">
         <v>3</v>
@@ -6738,7 +6764,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B7" s="5">
         <v>127</v>
@@ -6746,7 +6772,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -6781,7 +6807,7 @@
         <v>204</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -6789,7 +6815,7 @@
         <v>203</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -6829,7 +6855,7 @@
         <v>230</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
   </sheetData>
@@ -6862,101 +6888,101 @@
     </row>
     <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>443</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>444</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -6972,7 +6998,7 @@
         <v>204</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
   </sheetData>
@@ -7006,79 +7032,79 @@
     </row>
     <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -7094,7 +7120,7 @@
         <v>204</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
   </sheetData>
@@ -7127,35 +7153,35 @@
     </row>
     <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -7171,7 +7197,7 @@
         <v>204</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
   </sheetData>
@@ -7183,8 +7209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B311E26-48F5-445F-A976-490D3902A0D5}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7207,10 +7233,10 @@
     </row>
     <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C2" t="s">
         <v>133</v>
@@ -7218,10 +7244,10 @@
     </row>
     <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C3" t="s">
         <v>133</v>
@@ -7229,10 +7255,10 @@
     </row>
     <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C4" t="s">
         <v>133</v>
@@ -7240,10 +7266,10 @@
     </row>
     <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C5" t="s">
         <v>133</v>
@@ -7251,10 +7277,10 @@
     </row>
     <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C6" t="s">
         <v>133</v>
@@ -7262,57 +7288,57 @@
     </row>
     <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C7" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C8" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C9" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C10" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C11" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -7328,7 +7354,7 @@
         <v>204</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
     </row>
   </sheetData>
@@ -7341,8 +7367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E00C0EE-B5EA-4C5D-A3F6-0409760A68CF}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7467,7 +7493,7 @@
         <v>399</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="C11" t="s">
         <v>133</v>
@@ -7478,7 +7504,7 @@
         <v>400</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="C12" t="s">
         <v>133</v>
@@ -7533,7 +7559,7 @@
         <v>248</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="C17" t="s">
         <v>133</v>
@@ -7544,7 +7570,7 @@
         <v>249</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="C18" t="s">
         <v>133</v>
@@ -7607,7 +7633,7 @@
         <v>204</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -7615,7 +7641,7 @@
         <v>203</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -7661,7 +7687,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7684,10 +7710,10 @@
     </row>
     <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="C2" t="s">
         <v>133</v>
@@ -7698,7 +7724,7 @@
         <v>250</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="C3" t="s">
         <v>133</v>
@@ -7709,7 +7735,7 @@
         <v>251</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="C4" t="s">
         <v>133</v>
@@ -7720,7 +7746,7 @@
         <v>252</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C5" t="s">
         <v>133</v>
@@ -7731,7 +7757,7 @@
         <v>253</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="C6" t="s">
         <v>133</v>
@@ -7742,7 +7768,7 @@
         <v>254</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="C7" t="s">
         <v>133</v>
@@ -7753,7 +7779,7 @@
         <v>255</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="C8" t="s">
         <v>133</v>
@@ -7764,7 +7790,7 @@
         <v>256</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="C9" t="s">
         <v>133</v>
@@ -7775,7 +7801,7 @@
         <v>257</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="C10" t="s">
         <v>133</v>
@@ -7783,10 +7809,10 @@
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="C11" t="s">
         <v>133</v>
@@ -7797,7 +7823,7 @@
         <v>258</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="C12" t="s">
         <v>133</v>
@@ -7805,10 +7831,10 @@
     </row>
     <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="C13" t="s">
         <v>133</v>
@@ -7819,7 +7845,7 @@
         <v>260</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="C14" t="s">
         <v>133</v>
@@ -7830,7 +7856,7 @@
         <v>263</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="C15" t="s">
         <v>133</v>
@@ -7841,7 +7867,7 @@
         <v>261</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="C16" t="s">
         <v>133</v>
@@ -7852,7 +7878,7 @@
         <v>262</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="C17" t="s">
         <v>133</v>
@@ -7871,7 +7897,7 @@
         <v>204</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -7943,7 +7969,7 @@
         <v>264</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C2" t="s">
         <v>133</v>
@@ -7954,7 +7980,7 @@
         <v>265</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="C3" t="s">
         <v>133</v>
@@ -7965,7 +7991,7 @@
         <v>266</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="C4" t="s">
         <v>133</v>
@@ -7976,7 +8002,7 @@
         <v>267</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="C5" t="s">
         <v>133</v>
@@ -7987,7 +8013,7 @@
         <v>268</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="C6" t="s">
         <v>133</v>
@@ -7998,7 +8024,7 @@
         <v>269</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="C7" t="s">
         <v>133</v>
@@ -8009,7 +8035,7 @@
         <v>270</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="C8" t="s">
         <v>133</v>
@@ -8020,7 +8046,7 @@
         <v>271</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="C9" t="s">
         <v>133</v>
@@ -8031,7 +8057,7 @@
         <v>272</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="C10" t="s">
         <v>133</v>
@@ -8042,7 +8068,7 @@
         <v>273</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="C11" t="s">
         <v>133</v>
@@ -8053,7 +8079,7 @@
         <v>274</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="C12" t="s">
         <v>133</v>
@@ -8064,7 +8090,7 @@
         <v>375</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="C13" t="s">
         <v>133</v>
@@ -8075,7 +8101,7 @@
         <v>275</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="C14" t="s">
         <v>133</v>
@@ -8086,7 +8112,7 @@
         <v>276</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="C15" t="s">
         <v>133</v>
@@ -8097,7 +8123,7 @@
         <v>277</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="C16" t="s">
         <v>133</v>
@@ -8127,7 +8153,7 @@
         <v>204</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -8198,7 +8224,7 @@
         <v>279</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="C2" t="s">
         <v>133</v>
@@ -8209,7 +8235,7 @@
         <v>280</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="C3" t="s">
         <v>133</v>
@@ -8220,7 +8246,7 @@
         <v>281</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="C4" t="s">
         <v>133</v>
@@ -8231,7 +8257,7 @@
         <v>282</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="C5" t="s">
         <v>133</v>
@@ -8242,7 +8268,7 @@
         <v>283</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="C6" t="s">
         <v>133</v>
@@ -8253,7 +8279,7 @@
         <v>284</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="C7" t="s">
         <v>133</v>
@@ -8264,7 +8290,7 @@
         <v>285</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="C8" t="s">
         <v>133</v>
@@ -8275,7 +8301,7 @@
         <v>286</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="C9" t="s">
         <v>133</v>
@@ -8286,7 +8312,7 @@
         <v>287</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="C10" t="s">
         <v>133</v>
@@ -8297,7 +8323,7 @@
         <v>288</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="C11" t="s">
         <v>133</v>
@@ -8308,7 +8334,7 @@
         <v>289</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="C12" t="s">
         <v>133</v>
@@ -8319,7 +8345,7 @@
         <v>259</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="C13" t="s">
         <v>133</v>
@@ -8330,7 +8356,7 @@
         <v>290</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="C14" t="s">
         <v>133</v>
@@ -8341,7 +8367,7 @@
         <v>291</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="C15" t="s">
         <v>133</v>
@@ -8352,7 +8378,7 @@
         <v>292</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="C16" t="s">
         <v>133</v>
@@ -8360,10 +8386,10 @@
     </row>
     <row r="17" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="C17" t="s">
         <v>133</v>
@@ -8382,7 +8408,7 @@
         <v>204</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -8489,7 +8515,7 @@
         <v>204</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -8497,7 +8523,7 @@
         <v>203</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -8636,7 +8662,7 @@
         <v>204</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -8709,7 +8735,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B2">
         <v>36</v>
@@ -8717,7 +8743,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B3">
         <v>34</v>
@@ -8725,7 +8751,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B4">
         <v>31</v>
@@ -8733,7 +8759,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B5">
         <v>356</v>
@@ -8741,7 +8767,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -8749,7 +8775,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B7">
         <v>36</v>
@@ -8757,7 +8783,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -8765,7 +8791,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B9">
         <v>31</v>
@@ -8773,7 +8799,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -8792,7 +8818,7 @@
         <v>204</v>
       </c>
       <c r="B12" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -8800,7 +8826,7 @@
         <v>203</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -8915,7 +8941,7 @@
         <v>204</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -8923,7 +8949,7 @@
         <v>203</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -9028,7 +9054,7 @@
         <v>204</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -9095,7 +9121,7 @@
         <v>384</v>
       </c>
       <c r="B2" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -9167,7 +9193,7 @@
         <v>204</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -9175,7 +9201,7 @@
         <v>203</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -9306,7 +9332,7 @@
         <v>204</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -9314,7 +9340,7 @@
         <v>203</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -9382,90 +9408,90 @@
     </row>
     <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -9481,7 +9507,7 @@
         <v>204</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
     </row>
   </sheetData>
@@ -9668,7 +9694,7 @@
         <v>204</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -9676,7 +9702,7 @@
         <v>203</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -9741,10 +9767,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B2" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -9760,7 +9786,7 @@
         <v>204</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
   </sheetData>
@@ -9793,7 +9819,7 @@
     </row>
     <row r="2" spans="1:2" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="B2" s="5">
         <v>3338</v>
@@ -9801,7 +9827,7 @@
     </row>
     <row r="3" spans="1:2" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B3" s="13">
         <v>1038</v>
@@ -9812,7 +9838,7 @@
         <v>209</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -9820,7 +9846,7 @@
         <v>204</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -9828,7 +9854,7 @@
         <v>203</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -9892,7 +9918,7 @@
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B2" s="13">
         <v>2502</v>
@@ -9900,7 +9926,7 @@
     </row>
     <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B3" s="5">
         <v>851</v>
@@ -9911,7 +9937,7 @@
         <v>209</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -9919,7 +9945,7 @@
         <v>204</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -9927,7 +9953,7 @@
         <v>203</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -9991,7 +10017,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="B2" s="5">
         <v>401</v>
@@ -9999,7 +10025,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
@@ -10007,7 +10033,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B4" s="5">
         <v>145</v>
@@ -10015,7 +10041,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>
@@ -10026,7 +10052,7 @@
         <v>209</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -10034,7 +10060,7 @@
         <v>204</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -10042,7 +10068,7 @@
         <v>203</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added documentation of change
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDS_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDS_2020_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\RHIT_IRPA_@\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C75A08-CEED-4417-B0BD-35501BE2AFD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95467F72-8154-4461-8B83-4B032E391E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="16" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="32" activeTab="35" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="23" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1529" uniqueCount="767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1539" uniqueCount="769">
   <si>
     <t>Answer</t>
   </si>
@@ -1760,9 +1760,6 @@
     <t>What is the retention rate for 2019 cohort?</t>
   </si>
   <si>
-    <t>89.7% (445/496)</t>
-  </si>
-  <si>
     <t>The retention rate of full-time bachelor’s (or equivalent) degree-seeking undergraduate students who entered Rose-Hulman as
 freshmen in Fall 2019</t>
   </si>
@@ -2387,6 +2384,15 @@
   </si>
   <si>
     <t xml:space="preserve">The percentage of freshman students with sat (xor [^test_component] [^subject]) score (xor {between [^number] and [^number]} {[^range] [^number]}) is &lt;value&gt; </t>
+  </si>
+  <si>
+    <t>The retention rate for 2019 cohort is 89.7% (445/496)</t>
+  </si>
+  <si>
+    <t>Documentation-Of-Change</t>
+  </si>
+  <si>
+    <t>Aid related to CARES Act or unique to the COVID-19 pandemic are not included in financial aid calculations.</t>
   </si>
 </sst>
 </file>
@@ -2790,8 +2796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E422E2F-D9FA-411F-968E-DE340F994DF5}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2968,7 +2974,7 @@
         <v>201</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -3012,8 +3018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3551768-8BC9-4E69-8C86-830DF8B3DA69}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3091,7 +3097,7 @@
         <v>201</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
   </sheetData>
@@ -3259,7 +3265,7 @@
         <v>201</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -3446,10 +3452,10 @@
     </row>
     <row r="12" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C12" t="s">
         <v>130</v>
@@ -3468,7 +3474,7 @@
         <v>201</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
@@ -3674,7 +3680,7 @@
         <v>201</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
   </sheetData>
@@ -3870,7 +3876,7 @@
         <v>201</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3911,42 +3917,42 @@
     </row>
     <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -3962,7 +3968,7 @@
         <v>201</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
   </sheetData>
@@ -4054,7 +4060,7 @@
         <v>201</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -4233,7 +4239,7 @@
         <v>201</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -4241,7 +4247,7 @@
         <v>200</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -4349,7 +4355,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>67</v>
@@ -4368,7 +4374,7 @@
         <v>201</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -4528,7 +4534,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>67</v>
@@ -4547,7 +4553,7 @@
         <v>201</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -4655,7 +4661,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B6" s="5">
         <v>9</v>
@@ -4663,7 +4669,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B7" s="5">
         <v>2</v>
@@ -4671,7 +4677,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -4679,7 +4685,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B9" s="5">
         <v>0</v>
@@ -4858,7 +4864,7 @@
         <v>201</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -4974,7 +4980,7 @@
         <v>201</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -5027,8 +5033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3892E9F-E7EA-42B9-AE4C-1275BBD6A387}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView topLeftCell="A22" zoomScale="80" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5049,7 +5055,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B2" s="6">
         <v>1270</v>
@@ -5057,7 +5063,7 @@
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B3" s="6">
         <v>610</v>
@@ -5065,7 +5071,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B4" s="6">
         <v>650</v>
@@ -5073,7 +5079,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>302</v>
@@ -5081,7 +5087,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B6" s="6">
         <v>1355</v>
@@ -5089,7 +5095,7 @@
     </row>
     <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B7" s="6">
         <v>650</v>
@@ -5097,7 +5103,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B8" s="6">
         <v>700</v>
@@ -5105,7 +5111,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>302</v>
@@ -5113,7 +5119,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B10" s="6">
         <v>1440</v>
@@ -5121,7 +5127,7 @@
     </row>
     <row r="11" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B11" s="6">
         <v>700</v>
@@ -5129,7 +5135,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B12" s="6">
         <v>760</v>
@@ -5137,7 +5143,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B13" s="6">
         <v>1352</v>
@@ -5145,7 +5151,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B14" s="6">
         <v>1352</v>
@@ -5153,7 +5159,7 @@
     </row>
     <row r="15" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B15" s="6">
         <v>652</v>
@@ -5161,7 +5167,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B16" s="6">
         <v>700</v>
@@ -5169,7 +5175,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>302</v>
@@ -5177,7 +5183,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B18" s="6">
         <v>27</v>
@@ -5185,7 +5191,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>436</v>
@@ -5193,7 +5199,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B20" s="6">
         <v>26</v>
@@ -5201,15 +5207,15 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B22" s="6">
         <v>31</v>
@@ -5217,7 +5223,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B23" s="6">
         <v>31</v>
@@ -5225,7 +5231,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B24" s="6">
         <v>31.5</v>
@@ -5233,7 +5239,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>302</v>
@@ -5241,7 +5247,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B26" s="6">
         <v>33</v>
@@ -5249,7 +5255,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B27" s="6">
         <v>34</v>
@@ -5257,7 +5263,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B28" s="6">
         <v>35</v>
@@ -5265,7 +5271,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>302</v>
@@ -5273,7 +5279,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="B30" s="6">
         <v>30</v>
@@ -5281,7 +5287,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B31" s="6">
         <v>30</v>
@@ -5289,7 +5295,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B32" s="6">
         <v>30</v>
@@ -5297,7 +5303,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>302</v>
@@ -5316,7 +5322,7 @@
         <v>201</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -5324,7 +5330,7 @@
         <v>200</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -5525,7 +5531,7 @@
         <v>201</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -5660,7 +5666,7 @@
         <v>201</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -5792,7 +5798,7 @@
         <v>201</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -5800,7 +5806,7 @@
         <v>200</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -5890,7 +5896,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>95</v>
@@ -5909,10 +5915,10 @@
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
+        <v>605</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>606</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>607</v>
       </c>
       <c r="C6" t="s">
         <v>130</v>
@@ -5920,10 +5926,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C7" t="s">
         <v>130</v>
@@ -5931,10 +5937,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C8" t="s">
         <v>130</v>
@@ -5942,10 +5948,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C9" t="s">
         <v>130</v>
@@ -5953,7 +5959,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>97</v>
@@ -5964,7 +5970,7 @@
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>98</v>
@@ -5975,10 +5981,10 @@
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C12" t="s">
         <v>130</v>
@@ -5986,7 +5992,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>230</v>
@@ -6019,7 +6025,7 @@
     </row>
     <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>101</v>
@@ -6107,7 +6113,7 @@
         <v>201</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -6283,7 +6289,7 @@
         <v>108</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C2" t="s">
         <v>130</v>
@@ -6294,7 +6300,7 @@
         <v>111</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C3" t="s">
         <v>130</v>
@@ -6305,7 +6311,7 @@
         <v>112</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C4" t="s">
         <v>130</v>
@@ -6379,7 +6385,7 @@
         <v>201</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -6447,7 +6453,7 @@
         <v>109</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -6455,7 +6461,7 @@
         <v>110</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -6463,7 +6469,7 @@
         <v>113</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
@@ -6519,7 +6525,7 @@
         <v>201</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -6654,7 +6660,7 @@
         <v>201</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -6742,7 +6748,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B5" s="5">
         <v>1295</v>
@@ -6801,7 +6807,7 @@
         <v>201</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -6809,7 +6815,7 @@
         <v>200</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -6893,10 +6899,10 @@
     </row>
     <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
+        <v>651</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>652</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>653</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>439</v>
@@ -6907,7 +6913,7 @@
         <v>475</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>439</v>
@@ -6918,7 +6924,7 @@
         <v>476</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>439</v>
@@ -6929,7 +6935,7 @@
         <v>440</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>439</v>
@@ -6940,7 +6946,7 @@
         <v>441</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>439</v>
@@ -6951,7 +6957,7 @@
         <v>442</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>439</v>
@@ -6962,7 +6968,7 @@
         <v>443</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>439</v>
@@ -6992,7 +6998,7 @@
         <v>201</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
   </sheetData>
@@ -7026,10 +7032,10 @@
     </row>
     <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>439</v>
@@ -7040,7 +7046,7 @@
         <v>448</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>439</v>
@@ -7051,7 +7057,7 @@
         <v>449</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>439</v>
@@ -7062,7 +7068,7 @@
         <v>450</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>439</v>
@@ -7070,10 +7076,10 @@
     </row>
     <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>439</v>
@@ -7081,10 +7087,10 @@
     </row>
     <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>439</v>
@@ -7095,7 +7101,7 @@
         <v>451</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>439</v>
@@ -7114,7 +7120,7 @@
         <v>201</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
   </sheetData>
@@ -7150,7 +7156,7 @@
         <v>445</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>439</v>
@@ -7161,7 +7167,7 @@
         <v>446</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>439</v>
@@ -7172,7 +7178,7 @@
         <v>447</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>439</v>
@@ -7191,7 +7197,7 @@
         <v>201</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
   </sheetData>
@@ -7203,7 +7209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B311E26-48F5-445F-A976-490D3902A0D5}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -7238,7 +7244,7 @@
     </row>
     <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>467</v>
@@ -7249,7 +7255,7 @@
     </row>
     <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>468</v>
@@ -7260,7 +7266,7 @@
     </row>
     <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>461</v>
@@ -7271,7 +7277,7 @@
     </row>
     <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>469</v>
@@ -7282,7 +7288,7 @@
     </row>
     <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>462</v>
@@ -7348,7 +7354,7 @@
         <v>201</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
   </sheetData>
@@ -7359,10 +7365,10 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E00C0EE-B5EA-4C5D-A3F6-0409760A68CF}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7487,7 +7493,7 @@
         <v>395</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C11" t="s">
         <v>130</v>
@@ -7498,7 +7504,7 @@
         <v>396</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C12" t="s">
         <v>130</v>
@@ -7553,7 +7559,7 @@
         <v>244</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C17" t="s">
         <v>130</v>
@@ -7564,7 +7570,7 @@
         <v>245</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C18" t="s">
         <v>130</v>
@@ -7627,7 +7633,7 @@
         <v>201</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -7635,7 +7641,7 @@
         <v>200</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -7668,6 +7674,14 @@
       </c>
       <c r="B29" s="5" t="s">
         <v>168</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="10" t="s">
+        <v>767</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>768</v>
       </c>
     </row>
   </sheetData>
@@ -7678,10 +7692,10 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BD85EB1-BDB8-4AEB-99D1-57DF875DFEB5}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7704,10 +7718,10 @@
     </row>
     <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>671</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>672</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>673</v>
       </c>
       <c r="C2" t="s">
         <v>130</v>
@@ -7718,7 +7732,7 @@
         <v>246</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C3" t="s">
         <v>130</v>
@@ -7729,7 +7743,7 @@
         <v>247</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="C4" t="s">
         <v>130</v>
@@ -7740,7 +7754,7 @@
         <v>248</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C5" t="s">
         <v>130</v>
@@ -7751,7 +7765,7 @@
         <v>249</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="C6" t="s">
         <v>130</v>
@@ -7762,7 +7776,7 @@
         <v>250</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="C7" t="s">
         <v>130</v>
@@ -7773,7 +7787,7 @@
         <v>251</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C8" t="s">
         <v>130</v>
@@ -7784,7 +7798,7 @@
         <v>252</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="C9" t="s">
         <v>130</v>
@@ -7795,7 +7809,7 @@
         <v>253</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C10" t="s">
         <v>130</v>
@@ -7803,10 +7817,10 @@
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C11" t="s">
         <v>130</v>
@@ -7817,7 +7831,7 @@
         <v>254</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C12" t="s">
         <v>130</v>
@@ -7825,10 +7839,10 @@
     </row>
     <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="C13" t="s">
         <v>130</v>
@@ -7839,7 +7853,7 @@
         <v>256</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="C14" t="s">
         <v>130</v>
@@ -7850,7 +7864,7 @@
         <v>259</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C15" t="s">
         <v>130</v>
@@ -7861,7 +7875,7 @@
         <v>257</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C16" t="s">
         <v>130</v>
@@ -7872,7 +7886,7 @@
         <v>258</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C17" t="s">
         <v>130</v>
@@ -7891,7 +7905,7 @@
         <v>201</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -7924,6 +7938,14 @@
       </c>
       <c r="B23" s="5" t="s">
         <v>168</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
+        <v>767</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>768</v>
       </c>
     </row>
   </sheetData>
@@ -7934,10 +7956,10 @@
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE4F375-28FB-4634-A90F-E29F4CD5ADA1}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7963,7 +7985,7 @@
         <v>260</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C2" t="s">
         <v>130</v>
@@ -7974,7 +7996,7 @@
         <v>261</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C3" t="s">
         <v>130</v>
@@ -7985,7 +8007,7 @@
         <v>262</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C4" t="s">
         <v>130</v>
@@ -7996,7 +8018,7 @@
         <v>263</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C5" t="s">
         <v>130</v>
@@ -8007,7 +8029,7 @@
         <v>264</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="C6" t="s">
         <v>130</v>
@@ -8018,7 +8040,7 @@
         <v>265</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C7" t="s">
         <v>130</v>
@@ -8029,7 +8051,7 @@
         <v>266</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C8" t="s">
         <v>130</v>
@@ -8040,7 +8062,7 @@
         <v>267</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C9" t="s">
         <v>130</v>
@@ -8051,7 +8073,7 @@
         <v>268</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C10" t="s">
         <v>130</v>
@@ -8062,7 +8084,7 @@
         <v>269</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C11" t="s">
         <v>130</v>
@@ -8073,7 +8095,7 @@
         <v>270</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C12" t="s">
         <v>130</v>
@@ -8084,7 +8106,7 @@
         <v>371</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C13" t="s">
         <v>130</v>
@@ -8095,7 +8117,7 @@
         <v>271</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C14" t="s">
         <v>130</v>
@@ -8106,7 +8128,7 @@
         <v>272</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C15" t="s">
         <v>130</v>
@@ -8117,7 +8139,7 @@
         <v>273</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C16" t="s">
         <v>130</v>
@@ -8147,7 +8169,7 @@
         <v>201</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -8180,6 +8202,14 @@
       </c>
       <c r="B23" s="17" t="s">
         <v>168</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
+        <v>767</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>768</v>
       </c>
     </row>
   </sheetData>
@@ -8189,10 +8219,10 @@
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46EA6128-27F4-4911-A1F0-865B26420EEF}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8218,7 +8248,7 @@
         <v>275</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C2" t="s">
         <v>130</v>
@@ -8229,7 +8259,7 @@
         <v>276</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="C3" t="s">
         <v>130</v>
@@ -8240,7 +8270,7 @@
         <v>277</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C4" t="s">
         <v>130</v>
@@ -8251,7 +8281,7 @@
         <v>278</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="C5" t="s">
         <v>130</v>
@@ -8262,7 +8292,7 @@
         <v>279</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C6" t="s">
         <v>130</v>
@@ -8273,7 +8303,7 @@
         <v>280</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C7" t="s">
         <v>130</v>
@@ -8284,7 +8314,7 @@
         <v>281</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="C8" t="s">
         <v>130</v>
@@ -8295,7 +8325,7 @@
         <v>282</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="C9" t="s">
         <v>130</v>
@@ -8306,7 +8336,7 @@
         <v>283</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="C10" t="s">
         <v>130</v>
@@ -8317,7 +8347,7 @@
         <v>284</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="C11" t="s">
         <v>130</v>
@@ -8328,7 +8358,7 @@
         <v>285</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C12" t="s">
         <v>130</v>
@@ -8339,7 +8369,7 @@
         <v>255</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C13" t="s">
         <v>130</v>
@@ -8350,7 +8380,7 @@
         <v>286</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="C14" t="s">
         <v>130</v>
@@ -8361,7 +8391,7 @@
         <v>287</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C15" t="s">
         <v>130</v>
@@ -8372,7 +8402,7 @@
         <v>288</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C16" t="s">
         <v>130</v>
@@ -8380,10 +8410,10 @@
     </row>
     <row r="17" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
+        <v>719</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>720</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>721</v>
       </c>
       <c r="C17" t="s">
         <v>130</v>
@@ -8402,7 +8432,7 @@
         <v>201</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -8435,6 +8465,14 @@
       </c>
       <c r="B23" s="5" t="s">
         <v>168</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
+        <v>767</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>768</v>
       </c>
     </row>
   </sheetData>
@@ -8447,7 +8485,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8509,7 +8547,7 @@
         <v>201</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -8656,7 +8694,7 @@
         <v>201</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -8812,7 +8850,7 @@
         <v>201</v>
       </c>
       <c r="B12" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -8820,7 +8858,7 @@
         <v>200</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -8935,7 +8973,7 @@
         <v>201</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -8943,7 +8981,7 @@
         <v>200</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -9048,7 +9086,7 @@
         <v>201</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -9115,7 +9153,7 @@
         <v>380</v>
       </c>
       <c r="B2" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -9187,7 +9225,7 @@
         <v>201</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -9195,7 +9233,7 @@
         <v>200</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -9326,7 +9364,7 @@
         <v>201</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -9334,7 +9372,7 @@
         <v>200</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -9501,7 +9539,7 @@
         <v>201</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
   </sheetData>
@@ -9513,7 +9551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7606B2B-8397-4A8E-AF38-C293D77D8867}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -9688,7 +9726,7 @@
         <v>201</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -9696,7 +9734,7 @@
         <v>200</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -9745,35 +9783,42 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45AC6AA-908C-41CC-B7C1-A904CC3B6462}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="43.88671875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="28.88671875" customWidth="1"/>
+    <col min="2" max="2" width="28.88671875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>557</v>
       </c>
-      <c r="B2" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B2" s="5" t="s">
+        <v>766</v>
+      </c>
+      <c r="C2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>206</v>
       </c>
@@ -9781,12 +9826,12 @@
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>201</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
   </sheetData>
@@ -9846,7 +9891,7 @@
         <v>201</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -9945,7 +9990,7 @@
         <v>201</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -10060,7 +10105,7 @@
         <v>201</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
working on administator list ui
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDS_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDS_2020_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\RHIT_IRPA_@\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC71F112-48EB-4700-BDC3-6A7DD817EF0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16ABDA7B-D7A5-44F2-A7F4-AF19DE7BCE72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="30" activeTab="35" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="36" activeTab="40" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="23" r:id="rId1"/>
@@ -933,9 +933,6 @@
     <t>What is the total number of full-time instructional faculty who have a doctorate degree?</t>
   </si>
   <si>
-    <t>What is the total number of part-time instructional faculty who have a doctorate degree?</t>
-  </si>
-  <si>
     <t>What is the total number of full-time instructional faculty whose highest degree is a masters </t>
   </si>
   <si>
@@ -949,9 +946,6 @@
   </si>
   <si>
     <t>What is the total number of full-time instructional faculty whose highest degree is unknown</t>
-  </si>
-  <si>
-    <t>What is the total number of part-time instructional faculty whose highest degree is unknown</t>
   </si>
   <si>
     <t>What is the student to faculty ratio at Rose-Hulman?</t>
@@ -2413,6 +2407,12 @@
   </si>
   <si>
     <t>How many students in the initial cohort who graduated in between five and six years did not receive a Pell Grant or a subsidized Stafford Loan?</t>
+  </si>
+  <si>
+    <t>What is the total number of part-time instructional faculty whose highest degree is unknown or other</t>
+  </si>
+  <si>
+    <t>What is the total number of part-time instructional faculty who have a doctorate degree or terminal degrees</t>
   </si>
 </sst>
 </file>
@@ -2862,7 +2862,7 @@
         <v>267</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C2" t="s">
         <v>124</v>
@@ -2870,10 +2870,10 @@
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C3" t="s">
         <v>124</v>
@@ -2884,7 +2884,7 @@
         <v>269</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C4" t="s">
         <v>124</v>
@@ -2895,7 +2895,7 @@
         <v>268</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C5" t="s">
         <v>124</v>
@@ -2906,7 +2906,7 @@
         <v>270</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C6" t="s">
         <v>124</v>
@@ -2917,7 +2917,7 @@
         <v>271</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C7" t="s">
         <v>124</v>
@@ -2928,7 +2928,7 @@
         <v>272</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C8" t="s">
         <v>124</v>
@@ -2936,10 +2936,10 @@
     </row>
     <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C9" t="s">
         <v>124</v>
@@ -2950,7 +2950,7 @@
         <v>273</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C10" t="s">
         <v>124</v>
@@ -2961,7 +2961,7 @@
         <v>274</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C11" t="s">
         <v>124</v>
@@ -2972,7 +2972,7 @@
         <v>275</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C12" t="s">
         <v>124</v>
@@ -2983,7 +2983,7 @@
         <v>276</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C13" t="s">
         <v>124</v>
@@ -2994,7 +2994,7 @@
         <v>277</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C14" t="s">
         <v>124</v>
@@ -3013,7 +3013,7 @@
         <v>165</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -3077,7 +3077,7 @@
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B2" s="13">
         <v>2502</v>
@@ -3085,7 +3085,7 @@
     </row>
     <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B3" s="5">
         <v>851</v>
@@ -3096,7 +3096,7 @@
         <v>170</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -3104,7 +3104,7 @@
         <v>165</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -3112,7 +3112,7 @@
         <v>164</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -3176,7 +3176,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B2" s="5">
         <v>401</v>
@@ -3184,7 +3184,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
@@ -3192,7 +3192,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B4" s="5">
         <v>145</v>
@@ -3200,7 +3200,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>
@@ -3211,7 +3211,7 @@
         <v>170</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -3219,7 +3219,7 @@
         <v>165</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -3227,7 +3227,7 @@
         <v>164</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -3296,10 +3296,10 @@
     </row>
     <row r="2" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="C2" t="s">
         <v>124</v>
@@ -3307,10 +3307,10 @@
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C3" t="s">
         <v>124</v>
@@ -3318,10 +3318,10 @@
     </row>
     <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C4" t="s">
         <v>124</v>
@@ -3329,10 +3329,10 @@
     </row>
     <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C5" t="s">
         <v>124</v>
@@ -3343,7 +3343,7 @@
         <v>170</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
@@ -3351,7 +3351,7 @@
         <v>165</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
   </sheetData>
@@ -3387,7 +3387,7 @@
     </row>
     <row r="2" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B2" s="5">
         <v>4</v>
@@ -3398,7 +3398,7 @@
     </row>
     <row r="3" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B3" s="5">
         <v>4</v>
@@ -3409,7 +3409,7 @@
     </row>
     <row r="4" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B4" s="5">
         <v>3</v>
@@ -3420,7 +3420,7 @@
     </row>
     <row r="5" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B5" s="5">
         <v>3</v>
@@ -3431,7 +3431,7 @@
     </row>
     <row r="6" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B6" s="5">
         <v>0</v>
@@ -3442,7 +3442,7 @@
     </row>
     <row r="7" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B7" s="5">
         <v>2</v>
@@ -3453,7 +3453,7 @@
     </row>
     <row r="8" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -3464,7 +3464,7 @@
     </row>
     <row r="9" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B9" s="5">
         <v>0</v>
@@ -3475,7 +3475,7 @@
     </row>
     <row r="10" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B10" s="5">
         <v>0</v>
@@ -3486,7 +3486,7 @@
     </row>
     <row r="11" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B11" s="5">
         <v>0</v>
@@ -3497,10 +3497,10 @@
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C12" t="s">
         <v>124</v>
@@ -3519,7 +3519,7 @@
         <v>165</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -3527,7 +3527,7 @@
         <v>164</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -3596,7 +3596,7 @@
     </row>
     <row r="2" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3607,7 +3607,7 @@
     </row>
     <row r="3" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -3618,7 +3618,7 @@
     </row>
     <row r="4" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -3629,7 +3629,7 @@
     </row>
     <row r="5" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -3640,7 +3640,7 @@
     </row>
     <row r="6" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -3651,7 +3651,7 @@
     </row>
     <row r="7" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -3662,7 +3662,7 @@
     </row>
     <row r="8" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -3673,7 +3673,7 @@
     </row>
     <row r="9" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -3684,7 +3684,7 @@
     </row>
     <row r="10" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -3695,7 +3695,7 @@
     </row>
     <row r="11" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -3706,10 +3706,10 @@
     </row>
     <row r="12" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="C12" t="s">
         <v>124</v>
@@ -3728,7 +3728,7 @@
         <v>165</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
@@ -3736,7 +3736,7 @@
         <v>164</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -3780,7 +3780,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0908D19-61E8-460E-9695-3943D19E115C}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView zoomScale="105" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="105" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -3934,7 +3934,7 @@
         <v>165</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
   </sheetData>
@@ -3970,7 +3970,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -3978,7 +3978,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -3986,7 +3986,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -3994,7 +3994,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -4002,7 +4002,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -4010,7 +4010,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -4018,7 +4018,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -4026,7 +4026,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -4034,7 +4034,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -4042,7 +4042,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -4050,7 +4050,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -4058,7 +4058,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -4066,7 +4066,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -4074,7 +4074,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -4082,7 +4082,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -4090,7 +4090,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -4098,7 +4098,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -4106,7 +4106,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -4114,7 +4114,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -4130,7 +4130,7 @@
         <v>165</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -4138,7 +4138,7 @@
         <v>164</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -4171,42 +4171,42 @@
     </row>
     <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
+        <v>602</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>604</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -4222,7 +4222,7 @@
         <v>165</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
   </sheetData>
@@ -4314,7 +4314,7 @@
         <v>165</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -4322,7 +4322,7 @@
         <v>164</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -4367,7 +4367,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView zoomScale="84" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4493,7 +4493,7 @@
         <v>165</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -4501,7 +4501,7 @@
         <v>164</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -4569,7 +4569,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B2" s="5">
         <v>387</v>
@@ -4577,7 +4577,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B3" s="5">
         <v>143</v>
@@ -4585,7 +4585,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B4" s="5">
         <v>1</v>
@@ -4593,7 +4593,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>
@@ -4601,7 +4601,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B6" s="5">
         <v>9</v>
@@ -4609,7 +4609,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B7" s="5">
         <v>2</v>
@@ -4617,7 +4617,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -4625,7 +4625,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B9" s="5">
         <v>0</v>
@@ -4633,7 +4633,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B10" s="5">
         <v>1082</v>
@@ -4641,7 +4641,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B11" s="5">
         <v>329</v>
@@ -4649,7 +4649,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B12" s="5">
         <v>15</v>
@@ -4657,7 +4657,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B13" s="5">
         <v>1</v>
@@ -4804,7 +4804,7 @@
         <v>165</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -4812,7 +4812,7 @@
         <v>164</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -4858,7 +4858,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4917,7 +4917,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>67</v>
@@ -4936,7 +4936,7 @@
         <v>165</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -4944,7 +4944,7 @@
         <v>164</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -5096,7 +5096,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>67</v>
@@ -5115,7 +5115,7 @@
         <v>165</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -5123,7 +5123,7 @@
         <v>164</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -5134,7 +5134,7 @@
         <v>124</v>
       </c>
       <c r="D17" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -5191,7 +5191,7 @@
     </row>
     <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>21</v>
@@ -5199,7 +5199,7 @@
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>22</v>
@@ -5207,7 +5207,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B4" s="6">
         <v>350</v>
@@ -5215,10 +5215,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -5234,7 +5234,7 @@
         <v>165</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -5242,7 +5242,7 @@
         <v>164</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -5309,7 +5309,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="B2" s="6">
         <v>1270</v>
@@ -5317,7 +5317,7 @@
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="B3" s="6">
         <v>610</v>
@@ -5325,7 +5325,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="B4" s="6">
         <v>650</v>
@@ -5333,7 +5333,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>265</v>
@@ -5341,7 +5341,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="B6" s="6">
         <v>1355</v>
@@ -5349,7 +5349,7 @@
     </row>
     <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B7" s="6">
         <v>650</v>
@@ -5357,7 +5357,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="B8" s="6">
         <v>700</v>
@@ -5365,7 +5365,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>265</v>
@@ -5373,7 +5373,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B10" s="6">
         <v>1440</v>
@@ -5381,7 +5381,7 @@
     </row>
     <row r="11" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="B11" s="6">
         <v>700</v>
@@ -5389,7 +5389,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="B12" s="6">
         <v>760</v>
@@ -5397,7 +5397,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="B13" s="6">
         <v>1352</v>
@@ -5405,7 +5405,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="B14" s="6">
         <v>1352</v>
@@ -5413,7 +5413,7 @@
     </row>
     <row r="15" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="B15" s="6">
         <v>652</v>
@@ -5421,7 +5421,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="B16" s="6">
         <v>700</v>
@@ -5429,7 +5429,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>265</v>
@@ -5437,7 +5437,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="B18" s="6">
         <v>27</v>
@@ -5445,15 +5445,15 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="B20" s="6">
         <v>26</v>
@@ -5461,15 +5461,15 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="B22" s="6">
         <v>31</v>
@@ -5477,7 +5477,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="B23" s="6">
         <v>31</v>
@@ -5485,7 +5485,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B24" s="6">
         <v>31.5</v>
@@ -5493,7 +5493,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>265</v>
@@ -5501,7 +5501,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B26" s="6">
         <v>33</v>
@@ -5509,7 +5509,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="B27" s="6">
         <v>34</v>
@@ -5517,7 +5517,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="B28" s="6">
         <v>35</v>
@@ -5525,7 +5525,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>265</v>
@@ -5533,7 +5533,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="B30" s="6">
         <v>30</v>
@@ -5541,7 +5541,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="B31" s="6">
         <v>30</v>
@@ -5549,7 +5549,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="B32" s="6">
         <v>30</v>
@@ -5557,7 +5557,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>265</v>
@@ -5576,7 +5576,7 @@
         <v>165</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -5584,7 +5584,7 @@
         <v>164</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -5653,7 +5653,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>56</v>
@@ -5664,7 +5664,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>57</v>
@@ -5675,7 +5675,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>58</v>
@@ -5686,7 +5686,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>59</v>
@@ -5697,7 +5697,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>60</v>
@@ -5708,7 +5708,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>61</v>
@@ -5719,7 +5719,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>67</v>
@@ -5730,7 +5730,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>67</v>
@@ -5741,7 +5741,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>67</v>
@@ -5752,10 +5752,10 @@
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C11" t="s">
         <v>124</v>
@@ -5763,10 +5763,10 @@
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C12" t="s">
         <v>124</v>
@@ -5785,7 +5785,7 @@
         <v>165</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -5793,7 +5793,7 @@
         <v>164</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -5861,7 +5861,7 @@
     </row>
     <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>80</v>
@@ -5869,7 +5869,7 @@
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>81</v>
@@ -5877,7 +5877,7 @@
     </row>
     <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>82</v>
@@ -5885,7 +5885,7 @@
     </row>
     <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>83</v>
@@ -5893,7 +5893,7 @@
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>67</v>
@@ -5901,7 +5901,7 @@
     </row>
     <row r="7" spans="1:2" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>84</v>
@@ -5920,7 +5920,7 @@
         <v>165</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -5928,7 +5928,7 @@
         <v>164</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -5993,7 +5993,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B2" s="6">
         <v>59</v>
@@ -6001,7 +6001,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B3" s="6">
         <v>30</v>
@@ -6009,7 +6009,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B4" s="6">
         <v>9</v>
@@ -6017,7 +6017,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B5" s="6">
         <v>23</v>
@@ -6025,7 +6025,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B6" s="6">
         <v>13</v>
@@ -6033,7 +6033,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B7" s="6">
         <v>2</v>
@@ -6052,7 +6052,7 @@
         <v>165</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -6060,7 +6060,7 @@
         <v>164</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -6150,7 +6150,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>95</v>
@@ -6169,10 +6169,10 @@
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C6" t="s">
         <v>124</v>
@@ -6180,10 +6180,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C7" t="s">
         <v>124</v>
@@ -6191,10 +6191,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="C8" t="s">
         <v>124</v>
@@ -6202,10 +6202,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="C9" t="s">
         <v>124</v>
@@ -6213,7 +6213,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>97</v>
@@ -6224,7 +6224,7 @@
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>98</v>
@@ -6235,10 +6235,10 @@
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C12" t="s">
         <v>124</v>
@@ -6246,7 +6246,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>193</v>
@@ -6279,7 +6279,7 @@
     </row>
     <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>101</v>
@@ -6367,7 +6367,7 @@
         <v>165</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -6430,15 +6430,15 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>291</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>293</v>
       </c>
       <c r="C2" t="s">
         <v>124</v>
@@ -6446,10 +6446,10 @@
     </row>
     <row r="3" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C3" t="s">
         <v>124</v>
@@ -6468,7 +6468,7 @@
         <v>165</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -6543,7 +6543,7 @@
         <v>108</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="C2" t="s">
         <v>124</v>
@@ -6554,7 +6554,7 @@
         <v>111</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="C3" t="s">
         <v>124</v>
@@ -6565,7 +6565,7 @@
         <v>112</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="C4" t="s">
         <v>124</v>
@@ -6576,7 +6576,7 @@
         <v>114</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C5" t="s">
         <v>124</v>
@@ -6587,7 +6587,7 @@
         <v>116</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="C6" t="s">
         <v>124</v>
@@ -6598,7 +6598,7 @@
         <v>118</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="C7" t="s">
         <v>124</v>
@@ -6639,7 +6639,7 @@
         <v>165</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -6704,7 +6704,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B2" s="5">
         <v>226</v>
@@ -6712,7 +6712,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B3" s="5">
         <v>104</v>
@@ -6720,7 +6720,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B4" s="5">
         <v>93</v>
@@ -6728,7 +6728,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B5" s="5">
         <v>1295</v>
@@ -6736,7 +6736,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B6" s="5">
         <v>3</v>
@@ -6744,7 +6744,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B7" s="5">
         <v>127</v>
@@ -6752,7 +6752,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -6787,7 +6787,7 @@
         <v>165</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -6795,7 +6795,7 @@
         <v>164</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -6835,7 +6835,7 @@
         <v>191</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -6876,7 +6876,7 @@
         <v>109</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="C2" t="s">
         <v>124</v>
@@ -6887,7 +6887,7 @@
         <v>110</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C3" t="s">
         <v>124</v>
@@ -6898,7 +6898,7 @@
         <v>113</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="C4" t="s">
         <v>124</v>
@@ -6909,7 +6909,7 @@
         <v>115</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="C5" t="s">
         <v>124</v>
@@ -6920,7 +6920,7 @@
         <v>117</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="C6" t="s">
         <v>124</v>
@@ -6931,7 +6931,7 @@
         <v>120</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="C7" t="s">
         <v>124</v>
@@ -6972,7 +6972,7 @@
         <v>165</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -7107,7 +7107,7 @@
         <v>165</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -7171,101 +7171,101 @@
     </row>
     <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>400</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -7281,7 +7281,7 @@
         <v>165</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
   </sheetData>
@@ -7315,79 +7315,79 @@
     </row>
     <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -7403,7 +7403,7 @@
         <v>165</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
   </sheetData>
@@ -7436,35 +7436,35 @@
     </row>
     <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -7480,7 +7480,7 @@
         <v>165</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
   </sheetData>
@@ -7516,10 +7516,10 @@
     </row>
     <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C2" t="s">
         <v>124</v>
@@ -7527,10 +7527,10 @@
     </row>
     <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C3" t="s">
         <v>124</v>
@@ -7538,10 +7538,10 @@
     </row>
     <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C4" t="s">
         <v>124</v>
@@ -7549,10 +7549,10 @@
     </row>
     <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C5" t="s">
         <v>124</v>
@@ -7560,10 +7560,10 @@
     </row>
     <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C6" t="s">
         <v>124</v>
@@ -7571,57 +7571,57 @@
     </row>
     <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C8" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C9" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C10" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C11" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -7637,7 +7637,7 @@
         <v>165</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
   </sheetData>
@@ -7650,7 +7650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E00C0EE-B5EA-4C5D-A3F6-0409760A68CF}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
@@ -7773,10 +7773,10 @@
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="C11" t="s">
         <v>124</v>
@@ -7784,10 +7784,10 @@
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C12" t="s">
         <v>124</v>
@@ -7795,7 +7795,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>259</v>
@@ -7806,7 +7806,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>253</v>
@@ -7817,7 +7817,7 @@
     </row>
     <row r="15" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>253</v>
@@ -7828,7 +7828,7 @@
     </row>
     <row r="16" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>253</v>
@@ -7842,7 +7842,7 @@
         <v>207</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="C17" t="s">
         <v>124</v>
@@ -7853,7 +7853,7 @@
         <v>208</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="C18" t="s">
         <v>124</v>
@@ -7916,7 +7916,7 @@
         <v>165</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -7924,7 +7924,7 @@
         <v>164</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -7961,10 +7961,10 @@
     </row>
     <row r="30" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
     </row>
   </sheetData>
@@ -8001,10 +8001,10 @@
     </row>
     <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="C2" t="s">
         <v>124</v>
@@ -8015,7 +8015,7 @@
         <v>209</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="C3" t="s">
         <v>124</v>
@@ -8026,7 +8026,7 @@
         <v>210</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="C4" t="s">
         <v>124</v>
@@ -8037,7 +8037,7 @@
         <v>211</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="C5" t="s">
         <v>124</v>
@@ -8048,7 +8048,7 @@
         <v>212</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="C6" t="s">
         <v>124</v>
@@ -8059,7 +8059,7 @@
         <v>213</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="C7" t="s">
         <v>124</v>
@@ -8070,7 +8070,7 @@
         <v>214</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C8" t="s">
         <v>124</v>
@@ -8081,7 +8081,7 @@
         <v>215</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="C9" t="s">
         <v>124</v>
@@ -8092,7 +8092,7 @@
         <v>216</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="C10" t="s">
         <v>124</v>
@@ -8100,10 +8100,10 @@
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C11" t="s">
         <v>124</v>
@@ -8114,7 +8114,7 @@
         <v>217</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C12" t="s">
         <v>124</v>
@@ -8122,10 +8122,10 @@
     </row>
     <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C13" t="s">
         <v>124</v>
@@ -8136,7 +8136,7 @@
         <v>219</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="C14" t="s">
         <v>124</v>
@@ -8147,7 +8147,7 @@
         <v>222</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="C15" t="s">
         <v>124</v>
@@ -8158,7 +8158,7 @@
         <v>220</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="C16" t="s">
         <v>124</v>
@@ -8169,7 +8169,7 @@
         <v>221</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="C17" t="s">
         <v>124</v>
@@ -8188,7 +8188,7 @@
         <v>165</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -8225,10 +8225,10 @@
     </row>
     <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
     </row>
   </sheetData>
@@ -8268,7 +8268,7 @@
         <v>223</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="C2" t="s">
         <v>124</v>
@@ -8279,7 +8279,7 @@
         <v>224</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="C3" t="s">
         <v>124</v>
@@ -8290,7 +8290,7 @@
         <v>225</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="C4" t="s">
         <v>124</v>
@@ -8301,7 +8301,7 @@
         <v>226</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C5" t="s">
         <v>124</v>
@@ -8312,7 +8312,7 @@
         <v>227</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="C6" t="s">
         <v>124</v>
@@ -8323,7 +8323,7 @@
         <v>228</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C7" t="s">
         <v>124</v>
@@ -8334,7 +8334,7 @@
         <v>229</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C8" t="s">
         <v>124</v>
@@ -8345,7 +8345,7 @@
         <v>230</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="C9" t="s">
         <v>124</v>
@@ -8356,7 +8356,7 @@
         <v>231</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="C10" t="s">
         <v>124</v>
@@ -8367,7 +8367,7 @@
         <v>232</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C11" t="s">
         <v>124</v>
@@ -8378,7 +8378,7 @@
         <v>233</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="C12" t="s">
         <v>124</v>
@@ -8386,10 +8386,10 @@
     </row>
     <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="C13" t="s">
         <v>124</v>
@@ -8400,7 +8400,7 @@
         <v>234</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="C14" t="s">
         <v>124</v>
@@ -8411,7 +8411,7 @@
         <v>235</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="C15" t="s">
         <v>124</v>
@@ -8422,7 +8422,7 @@
         <v>236</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="C16" t="s">
         <v>124</v>
@@ -8452,7 +8452,7 @@
         <v>165</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -8489,10 +8489,10 @@
     </row>
     <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
     </row>
   </sheetData>
@@ -8531,7 +8531,7 @@
         <v>238</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C2" t="s">
         <v>124</v>
@@ -8542,7 +8542,7 @@
         <v>239</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="C3" t="s">
         <v>124</v>
@@ -8553,7 +8553,7 @@
         <v>240</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C4" t="s">
         <v>124</v>
@@ -8564,7 +8564,7 @@
         <v>241</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="C5" t="s">
         <v>124</v>
@@ -8575,7 +8575,7 @@
         <v>242</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="C6" t="s">
         <v>124</v>
@@ -8586,7 +8586,7 @@
         <v>243</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="C7" t="s">
         <v>124</v>
@@ -8597,7 +8597,7 @@
         <v>244</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="C8" t="s">
         <v>124</v>
@@ -8608,7 +8608,7 @@
         <v>245</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="C9" t="s">
         <v>124</v>
@@ -8619,7 +8619,7 @@
         <v>246</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="C10" t="s">
         <v>124</v>
@@ -8630,7 +8630,7 @@
         <v>247</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="C11" t="s">
         <v>124</v>
@@ -8641,7 +8641,7 @@
         <v>248</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="C12" t="s">
         <v>124</v>
@@ -8652,7 +8652,7 @@
         <v>218</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="C13" t="s">
         <v>124</v>
@@ -8663,7 +8663,7 @@
         <v>249</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="C14" t="s">
         <v>124</v>
@@ -8674,7 +8674,7 @@
         <v>250</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="C15" t="s">
         <v>124</v>
@@ -8685,7 +8685,7 @@
         <v>251</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="C16" t="s">
         <v>124</v>
@@ -8693,10 +8693,10 @@
     </row>
     <row r="17" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="C17" t="s">
         <v>124</v>
@@ -8715,7 +8715,7 @@
         <v>165</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -8752,10 +8752,10 @@
     </row>
     <row r="24" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
     </row>
   </sheetData>
@@ -8788,7 +8788,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B2">
         <v>36</v>
@@ -8796,7 +8796,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B3">
         <v>34</v>
@@ -8804,7 +8804,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B4">
         <v>31</v>
@@ -8812,7 +8812,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B5">
         <v>356</v>
@@ -8820,7 +8820,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -8828,7 +8828,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B7">
         <v>36</v>
@@ -8836,7 +8836,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -8844,7 +8844,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B9">
         <v>31</v>
@@ -8852,7 +8852,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -8871,7 +8871,7 @@
         <v>165</v>
       </c>
       <c r="B12" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -8879,7 +8879,7 @@
         <v>164</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -8932,7 +8932,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8994,7 +8994,7 @@
         <v>165</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -9002,7 +9002,7 @@
         <v>164</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -9046,8 +9046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2758D6-F888-4498-88A0-7DFBF7091CA2}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9074,7 +9074,7 @@
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>283</v>
+        <v>774</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -9082,7 +9082,7 @@
     </row>
     <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -9090,7 +9090,7 @@
     </row>
     <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -9098,7 +9098,7 @@
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -9106,7 +9106,7 @@
     </row>
     <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -9114,7 +9114,7 @@
     </row>
     <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -9122,7 +9122,7 @@
     </row>
     <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>289</v>
+        <v>773</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -9141,7 +9141,7 @@
         <v>165</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -9149,7 +9149,7 @@
         <v>164</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -9213,7 +9213,7 @@
     </row>
     <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B2">
         <v>33</v>
@@ -9221,7 +9221,7 @@
     </row>
     <row r="3" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -9229,7 +9229,7 @@
     </row>
     <row r="4" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B4">
         <v>8</v>
@@ -9237,7 +9237,7 @@
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -9256,7 +9256,7 @@
         <v>165</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -9264,7 +9264,7 @@
         <v>164</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -9333,10 +9333,10 @@
     </row>
     <row r="2" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C2" t="s">
         <v>124</v>
@@ -9344,10 +9344,10 @@
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C3" t="s">
         <v>124</v>
@@ -9369,7 +9369,7 @@
         <v>165</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -9433,15 +9433,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B2" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B3">
         <v>76</v>
@@ -9449,7 +9449,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B4">
         <v>216</v>
@@ -9457,7 +9457,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B5">
         <v>129</v>
@@ -9465,7 +9465,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -9473,7 +9473,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -9481,7 +9481,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -9489,7 +9489,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -9508,7 +9508,7 @@
         <v>165</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -9516,7 +9516,7 @@
         <v>164</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -9580,7 +9580,7 @@
     </row>
     <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -9588,7 +9588,7 @@
     </row>
     <row r="3" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B3">
         <v>33</v>
@@ -9596,7 +9596,7 @@
     </row>
     <row r="4" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B4">
         <v>31</v>
@@ -9604,7 +9604,7 @@
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -9612,7 +9612,7 @@
     </row>
     <row r="6" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -9620,7 +9620,7 @@
     </row>
     <row r="7" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -9628,7 +9628,7 @@
     </row>
     <row r="8" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -9647,7 +9647,7 @@
         <v>165</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -9655,7 +9655,7 @@
         <v>164</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -9723,90 +9723,90 @@
     </row>
     <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -9822,7 +9822,7 @@
         <v>165</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
   </sheetData>
@@ -9861,7 +9861,7 @@
         <v>163</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="C2" t="s">
         <v>124</v>
@@ -9869,10 +9869,10 @@
     </row>
     <row r="3" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="C3" t="s">
         <v>124</v>
@@ -9880,10 +9880,10 @@
     </row>
     <row r="4" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="C4" t="s">
         <v>124</v>
@@ -9905,7 +9905,7 @@
         <v>165</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C6" t="s">
         <v>124</v>
@@ -9916,7 +9916,7 @@
         <v>164</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="C7" t="s">
         <v>124</v>
@@ -9990,10 +9990,10 @@
     </row>
     <row r="2" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="C2" t="s">
         <v>124</v>
@@ -10001,10 +10001,10 @@
     </row>
     <row r="3" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="C3" t="s">
         <v>124</v>
@@ -10012,10 +10012,10 @@
     </row>
     <row r="4" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="C4" t="s">
         <v>124</v>
@@ -10023,10 +10023,10 @@
     </row>
     <row r="5" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="C5" t="s">
         <v>124</v>
@@ -10034,10 +10034,10 @@
     </row>
     <row r="6" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="C6" t="s">
         <v>124</v>
@@ -10045,10 +10045,10 @@
     </row>
     <row r="7" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="C7" t="s">
         <v>124</v>
@@ -10056,10 +10056,10 @@
     </row>
     <row r="8" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C8" t="s">
         <v>124</v>
@@ -10067,10 +10067,10 @@
     </row>
     <row r="9" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="C9" t="s">
         <v>124</v>
@@ -10078,10 +10078,10 @@
     </row>
     <row r="10" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="C10" t="s">
         <v>124</v>
@@ -10089,10 +10089,10 @@
     </row>
     <row r="11" spans="1:3" ht="66" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="C11" t="s">
         <v>124</v>
@@ -10166,81 +10166,81 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>744</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>755</v>
+      </c>
+      <c r="C2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>744</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>755</v>
+      </c>
+      <c r="C3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>745</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>768</v>
+      </c>
+      <c r="C4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>746</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B5" s="20" t="s">
+        <v>769</v>
+      </c>
+      <c r="C5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>740</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>756</v>
+      </c>
+      <c r="C6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>748</v>
+      </c>
+      <c r="B7" s="19" t="s">
         <v>757</v>
       </c>
-      <c r="C2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>746</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>757</v>
-      </c>
-      <c r="C3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>747</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>770</v>
-      </c>
-      <c r="C4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>748</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>771</v>
-      </c>
-      <c r="C5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>742</v>
-      </c>
-      <c r="B6" s="19" t="s">
+      <c r="C7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>741</v>
+      </c>
+      <c r="B8" s="19" t="s">
         <v>758</v>
-      </c>
-      <c r="C6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>750</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>759</v>
-      </c>
-      <c r="C7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>743</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>760</v>
       </c>
       <c r="C8" t="s">
         <v>124</v>
@@ -10279,10 +10279,10 @@
     </row>
     <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="C2" t="s">
         <v>124</v>
@@ -10301,7 +10301,7 @@
         <v>165</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
   </sheetData>
@@ -10334,7 +10334,7 @@
     </row>
     <row r="2" spans="1:2" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B2" s="5">
         <v>3338</v>
@@ -10342,7 +10342,7 @@
     </row>
     <row r="3" spans="1:2" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B3" s="13">
         <v>1038</v>
@@ -10353,7 +10353,7 @@
         <v>170</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -10361,7 +10361,7 @@
         <v>165</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -10369,7 +10369,7 @@
         <v>164</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
refactored unanswered question code
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDS_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDS_2020_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\RHIT_IRPA_@\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD2686B-49FA-49C7-9CB8-ECFB1E91F2C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5839F305-8EBF-4CB6-8857-BEF006079413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="28" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6533,7 +6533,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
continue working on active learning
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDS_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDS_2020_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\RHIT_IRPA_@\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B31DABB7-D3DD-4BC9-92F4-3F2CDE34909B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8091E5-0498-49C3-BDAA-6331CFDC781A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="18" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="40" activeTab="42" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="23" r:id="rId1"/>
@@ -2599,7 +2599,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -2657,12 +2657,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3390,7 +3384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3551768-8BC9-4E69-8C86-830DF8B3DA69}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -3671,8 +3665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B50A1A77-FCFF-4BA2-80DC-49E66C3D11B3}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3871,8 +3865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0908D19-61E8-460E-9695-3943D19E115C}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView zoomScale="105" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A4" zoomScale="105" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="58.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5372,7 +5366,7 @@
       <c r="A13" s="10" t="s">
         <v>779</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="5" t="s">
         <v>120</v>
       </c>
     </row>
@@ -5386,7 +5380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3892E9F-E7EA-42B9-AE4C-1275BBD6A387}">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="80" workbookViewId="0">
+    <sheetView topLeftCell="A14" zoomScale="80" workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
@@ -7736,7 +7730,7 @@
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
@@ -7744,7 +7738,7 @@
       <c r="A2" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="22" t="s">
         <v>784</v>
       </c>
     </row>
@@ -7752,7 +7746,7 @@
       <c r="A3" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="22" t="s">
         <v>785</v>
       </c>
     </row>
@@ -7760,7 +7754,7 @@
       <c r="A4" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="22" t="s">
         <v>786</v>
       </c>
     </row>
@@ -7768,7 +7762,7 @@
       <c r="A5" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="22" t="s">
         <v>787</v>
       </c>
     </row>
@@ -7776,7 +7770,7 @@
       <c r="A6" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="22" t="s">
         <v>788</v>
       </c>
     </row>
@@ -7784,7 +7778,7 @@
       <c r="A7" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="22" t="s">
         <v>789</v>
       </c>
     </row>
@@ -7792,7 +7786,7 @@
       <c r="A8" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="22" t="s">
         <v>790</v>
       </c>
     </row>
@@ -7800,7 +7794,7 @@
       <c r="A9" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="22" t="s">
         <v>791</v>
       </c>
     </row>
@@ -7808,7 +7802,7 @@
       <c r="A10" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="22" t="s">
         <v>792</v>
       </c>
     </row>
@@ -7816,7 +7810,7 @@
       <c r="A11" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="22" t="s">
         <v>793</v>
       </c>
     </row>
@@ -7824,7 +7818,7 @@
       <c r="A12" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="22" t="s">
         <v>794</v>
       </c>
     </row>
@@ -7832,7 +7826,7 @@
       <c r="A13" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="22" t="s">
         <v>795</v>
       </c>
     </row>
@@ -7840,7 +7834,7 @@
       <c r="A14" s="12" t="s">
         <v>343</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="22" t="s">
         <v>796</v>
       </c>
     </row>
@@ -7848,7 +7842,7 @@
       <c r="A15" s="8" t="s">
         <v>344</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="22" t="s">
         <v>797</v>
       </c>
     </row>
@@ -7856,7 +7850,7 @@
       <c r="A16" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="22" t="s">
         <v>798</v>
       </c>
     </row>
@@ -7864,7 +7858,7 @@
       <c r="A17" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="22" t="s">
         <v>799</v>
       </c>
     </row>
@@ -7872,7 +7866,7 @@
       <c r="A18" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="22" t="s">
         <v>800</v>
       </c>
     </row>
@@ -7880,7 +7874,7 @@
       <c r="A19" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="22" t="s">
         <v>801</v>
       </c>
     </row>
@@ -7888,7 +7882,7 @@
       <c r="A20" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="22" t="s">
         <v>802</v>
       </c>
     </row>
@@ -7896,7 +7890,7 @@
       <c r="A21" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="22" t="s">
         <v>803</v>
       </c>
     </row>
@@ -7904,7 +7898,7 @@
       <c r="A22" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="22" t="s">
         <v>804</v>
       </c>
     </row>
@@ -8197,7 +8191,7 @@
       <c r="A25" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="23" t="s">
         <v>120</v>
       </c>
     </row>
@@ -9193,8 +9187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61ED34DA-E2CB-4859-9A96-48DF7AE0B7A7}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9302,7 +9296,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9440,7 +9434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA74624B-4AE3-43E9-9C9C-696C43DB0CE5}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed bug with UI
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDS_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDS_2020_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\RHIT_IRPA_@\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061B5A39-2A1D-4B92-9CF8-9225DC4198EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86EC3253-1B22-4533-BFFE-58F00683722D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="21" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="10" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="23" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1531" uniqueCount="805">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1510" uniqueCount="803">
   <si>
     <t>Answer</t>
   </si>
@@ -1195,9 +1195,6 @@
     <t>How many Social sciences degrees are conferred?</t>
   </si>
   <si>
-    <t>Of previous units, how many lab units are recommended for admission?</t>
-  </si>
-  <si>
     <t>How many degree-seeking undergraduate students are enrolled?</t>
   </si>
   <si>
@@ -2164,12 +2161,6 @@
     <t>The (xor [^aggregation] [^percentile])  [^standarized_test] [^test_component] score for incoming freshmen is &lt;value&gt;</t>
   </si>
   <si>
-    <t>No other additional units are recommended for admission</t>
-  </si>
-  <si>
-    <t>What other units are recommended for admission? (please specify)</t>
-  </si>
-  <si>
     <t>What is the percentage of freshman students with act composite score below 6</t>
   </si>
   <si>
@@ -2359,69 +2350,9 @@
     <t>What type of college owned, operated, or affiliated housing is available at Rose-Hulman?</t>
   </si>
   <si>
-    <t>Four English units are required for admission.</t>
-  </si>
-  <si>
-    <t>Four Mathematics units are required for admission.</t>
-  </si>
-  <si>
-    <t>Three science units are required for admission.</t>
-  </si>
-  <si>
-    <t>Three lab units are required for admission from the previous units.</t>
-  </si>
-  <si>
-    <t>No foreign language units are required for admission.</t>
-  </si>
-  <si>
-    <t>Two social studies units are required for admission.</t>
-  </si>
-  <si>
-    <t>No history units are required for admission.</t>
-  </si>
-  <si>
-    <t>No academic elective units are required for admission.</t>
-  </si>
-  <si>
-    <t>No computer science units are required for admission.</t>
-  </si>
-  <si>
-    <t>No visual/performing art units are required for admission.</t>
-  </si>
-  <si>
     <t>Of the science credit, how many lab units required for admission?</t>
   </si>
   <si>
-    <t>No English units are recommended for admission.</t>
-  </si>
-  <si>
-    <t>Five Mathematics units are recommended for admission.</t>
-  </si>
-  <si>
-    <t>Four science units are recommended for admission.</t>
-  </si>
-  <si>
-    <t>No lab units are recommended for admission from the previous units.</t>
-  </si>
-  <si>
-    <t>No foreign language units are recommended for admission.</t>
-  </si>
-  <si>
-    <t>No social studies units are recommended for admission.</t>
-  </si>
-  <si>
-    <t>No history units are recommended for admission.</t>
-  </si>
-  <si>
-    <t>Four academic elective units are recommended for admission.</t>
-  </si>
-  <si>
-    <t>No computer science units are recommended for admission.</t>
-  </si>
-  <si>
-    <t>No visual/performing art units are recommended for admission.</t>
-  </si>
-  <si>
     <t>Complete-Sentence?</t>
   </si>
   <si>
@@ -2504,6 +2435,69 @@
   </si>
   <si>
     <t xml:space="preserve">Transfer Students must have a semester of calculus, as well as calculus-based physics and chemistry. </t>
+  </si>
+  <si>
+    <t>Of Science units, how many lab units are recommended for admission?</t>
+  </si>
+  <si>
+    <t>0 high school english units are recommended for admission.</t>
+  </si>
+  <si>
+    <t>Five high school mathematics units are recommended for admission.</t>
+  </si>
+  <si>
+    <t>Four science high school units are recommended for admission.</t>
+  </si>
+  <si>
+    <t>No high school social studies units are recommended for admission.</t>
+  </si>
+  <si>
+    <t>No high school foreign language units are recommended for admission.</t>
+  </si>
+  <si>
+    <t>No high school science lab units are recommended for admission.</t>
+  </si>
+  <si>
+    <t>No high school history units are recommended for admission.</t>
+  </si>
+  <si>
+    <t>Four high school academic elective units are recommended for admission.</t>
+  </si>
+  <si>
+    <t>No high school computer science units are recommended for admission.</t>
+  </si>
+  <si>
+    <t>No high school visual/performing art units are recommended for admission.</t>
+  </si>
+  <si>
+    <t>Four high school english units are required for admission.</t>
+  </si>
+  <si>
+    <t>Four high school mathematics units are required for admission.</t>
+  </si>
+  <si>
+    <t>Three high school science units are required for admission.</t>
+  </si>
+  <si>
+    <t>Three high school lab units are required for admission from the previous units.</t>
+  </si>
+  <si>
+    <t>Two high school social studies units are required for admission.</t>
+  </si>
+  <si>
+    <t>No high school foreign language units are required for admission.</t>
+  </si>
+  <si>
+    <t>No high school history units are required for admission.</t>
+  </si>
+  <si>
+    <t>No high school academic elective units are required for admission.</t>
+  </si>
+  <si>
+    <t>No high school computer science units are required for admission.</t>
+  </si>
+  <si>
+    <t>No high school visual/performing art units are required for admission.</t>
   </si>
 </sst>
 </file>
@@ -3125,7 +3119,7 @@
         <v>158</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -3189,7 +3183,7 @@
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B2" s="13">
         <v>2502</v>
@@ -3197,7 +3191,7 @@
     </row>
     <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B3" s="5">
         <v>851</v>
@@ -3208,7 +3202,7 @@
         <v>163</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -3216,7 +3210,7 @@
         <v>158</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -3224,7 +3218,7 @@
         <v>157</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -3288,7 +3282,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B2" s="5">
         <v>401</v>
@@ -3296,7 +3290,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
@@ -3304,7 +3298,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B4" s="5">
         <v>145</v>
@@ -3312,7 +3306,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>
@@ -3323,7 +3317,7 @@
         <v>163</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -3331,7 +3325,7 @@
         <v>158</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -3339,7 +3333,7 @@
         <v>157</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -3408,10 +3402,10 @@
     </row>
     <row r="2" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C2" t="s">
         <v>118</v>
@@ -3419,10 +3413,10 @@
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C3" t="s">
         <v>118</v>
@@ -3430,10 +3424,10 @@
     </row>
     <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>427</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>428</v>
       </c>
       <c r="C4" t="s">
         <v>118</v>
@@ -3441,10 +3435,10 @@
     </row>
     <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>429</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>430</v>
       </c>
       <c r="C5" t="s">
         <v>118</v>
@@ -3455,7 +3449,7 @@
         <v>163</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
@@ -3463,7 +3457,7 @@
         <v>158</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
   </sheetData>
@@ -3473,10 +3467,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5DC138E-AAA1-4452-BC05-6992F74BED09}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView zoomScale="74" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3486,128 +3480,95 @@
     <col min="3" max="3" width="24.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>350</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>756</v>
-      </c>
-      <c r="C2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>351</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>757</v>
-      </c>
-      <c r="C3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>352</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>758</v>
-      </c>
-      <c r="C4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>766</v>
+        <v>753</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>759</v>
-      </c>
-      <c r="C5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>344</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>760</v>
-      </c>
-      <c r="C6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>345</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>761</v>
-      </c>
-      <c r="C7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>346</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>762</v>
-      </c>
-      <c r="C8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>347</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>763</v>
-      </c>
-      <c r="C9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>348</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>764</v>
-      </c>
-      <c r="C10" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>349</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>765</v>
-      </c>
-      <c r="C11" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>163</v>
       </c>
@@ -3615,15 +3576,15 @@
         <v>161</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>158</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>159</v>
       </c>
@@ -3631,7 +3592,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>160</v>
       </c>
@@ -3639,7 +3600,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>164</v>
       </c>
@@ -3653,6 +3614,14 @@
       </c>
       <c r="B17" s="5" t="s">
         <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -3663,10 +3632,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B50A1A77-FCFF-4BA2-80DC-49E66C3D11B3}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3676,165 +3645,129 @@
     <col min="3" max="3" width="21.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>353</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>767</v>
-      </c>
-      <c r="C2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>354</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>768</v>
-      </c>
-      <c r="C3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>355</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>769</v>
-      </c>
-      <c r="C4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>369</v>
+        <v>782</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>770</v>
-      </c>
-      <c r="C5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>356</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>771</v>
-      </c>
-      <c r="C6" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>357</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>772</v>
-      </c>
-      <c r="C7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>358</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>773</v>
-      </c>
-      <c r="C8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>359</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>774</v>
-      </c>
-      <c r="C9" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>360</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>775</v>
-      </c>
-      <c r="C10" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>361</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>776</v>
-      </c>
-      <c r="C11" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>692</v>
+        <v>163</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>691</v>
-      </c>
-      <c r="C12" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
-        <v>158</v>
+        <v>511</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>159</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>155</v>
@@ -3842,18 +3775,18 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>162</v>
+      <c r="A18" s="5" t="s">
+        <v>185</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>155</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -3865,8 +3798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0908D19-61E8-460E-9695-3943D19E115C}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="105" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView zoomScale="105" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="58.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4019,7 +3952,7 @@
         <v>158</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
   </sheetData>
@@ -4055,7 +3988,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -4063,7 +3996,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -4071,7 +4004,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -4079,7 +4012,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -4087,7 +4020,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -4095,7 +4028,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -4103,7 +4036,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -4111,7 +4044,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -4119,7 +4052,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -4127,7 +4060,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -4135,7 +4068,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -4143,7 +4076,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -4151,7 +4084,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -4159,7 +4092,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -4167,7 +4100,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -4175,7 +4108,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -4183,7 +4116,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -4191,7 +4124,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -4199,7 +4132,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -4215,7 +4148,7 @@
         <v>158</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
@@ -4256,42 +4189,42 @@
     </row>
     <row r="2" spans="1:2" ht="79.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -4307,7 +4240,7 @@
         <v>158</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
   </sheetData>
@@ -4399,7 +4332,7 @@
         <v>158</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -4407,7 +4340,7 @@
         <v>157</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -4578,7 +4511,7 @@
         <v>158</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -4586,7 +4519,7 @@
         <v>157</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -4634,8 +4567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F776689-DE3B-468A-9224-18F5400CC444}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4654,7 +4587,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B2" s="5">
         <v>387</v>
@@ -4662,7 +4595,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B3" s="5">
         <v>143</v>
@@ -4670,7 +4603,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B4" s="5">
         <v>1</v>
@@ -4678,7 +4611,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>
@@ -4686,7 +4619,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B6" s="5">
         <v>9</v>
@@ -4694,7 +4627,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B7" s="5">
         <v>2</v>
@@ -4702,7 +4635,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -4710,7 +4643,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B9" s="5">
         <v>0</v>
@@ -4718,7 +4651,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B10" s="5">
         <v>1082</v>
@@ -4726,7 +4659,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B11" s="5">
         <v>329</v>
@@ -4734,7 +4667,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B12" s="5">
         <v>15</v>
@@ -4742,7 +4675,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B13" s="5">
         <v>1</v>
@@ -4889,7 +4822,7 @@
         <v>158</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -4897,7 +4830,7 @@
         <v>157</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -5002,7 +4935,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>65</v>
@@ -5021,7 +4954,7 @@
         <v>158</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -5029,7 +4962,7 @@
         <v>157</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -5181,7 +5114,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>65</v>
@@ -5200,7 +5133,7 @@
         <v>158</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -5208,7 +5141,7 @@
         <v>157</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -5219,7 +5152,7 @@
         <v>118</v>
       </c>
       <c r="D17" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -5257,7 +5190,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5279,7 +5212,7 @@
         <v>295</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>778</v>
+        <v>755</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -5287,7 +5220,7 @@
         <v>296</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>779</v>
+        <v>756</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -5295,7 +5228,7 @@
         <v>293</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>780</v>
+        <v>757</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -5303,7 +5236,7 @@
         <v>294</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>781</v>
+        <v>758</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -5319,7 +5252,7 @@
         <v>158</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -5327,7 +5260,7 @@
         <v>157</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -5364,7 +5297,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>777</v>
+        <v>754</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>118</v>
@@ -5402,7 +5335,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B2" s="6">
         <v>1270</v>
@@ -5410,7 +5343,7 @@
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B3" s="6">
         <v>610</v>
@@ -5418,7 +5351,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B4" s="6">
         <v>650</v>
@@ -5426,7 +5359,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>249</v>
@@ -5434,7 +5367,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B6" s="6">
         <v>1355</v>
@@ -5442,7 +5375,7 @@
     </row>
     <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B7" s="6">
         <v>650</v>
@@ -5450,7 +5383,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B8" s="6">
         <v>700</v>
@@ -5458,7 +5391,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>249</v>
@@ -5466,7 +5399,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B10" s="6">
         <v>1440</v>
@@ -5474,7 +5407,7 @@
     </row>
     <row r="11" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B11" s="6">
         <v>700</v>
@@ -5482,7 +5415,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B12" s="6">
         <v>760</v>
@@ -5490,7 +5423,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B13" s="6">
         <v>1352</v>
@@ -5498,7 +5431,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B14" s="6">
         <v>1352</v>
@@ -5506,7 +5439,7 @@
     </row>
     <row r="15" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B15" s="6">
         <v>652</v>
@@ -5514,7 +5447,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B16" s="6">
         <v>700</v>
@@ -5522,7 +5455,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>249</v>
@@ -5530,7 +5463,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B18" s="6">
         <v>27</v>
@@ -5538,15 +5471,15 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B20" s="6">
         <v>26</v>
@@ -5554,15 +5487,15 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B22" s="6">
         <v>31</v>
@@ -5570,7 +5503,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B23" s="6">
         <v>31</v>
@@ -5578,7 +5511,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B24" s="6">
         <v>31.5</v>
@@ -5586,7 +5519,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>249</v>
@@ -5594,7 +5527,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B26" s="6">
         <v>33</v>
@@ -5602,7 +5535,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B27" s="6">
         <v>34</v>
@@ -5610,7 +5543,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B28" s="6">
         <v>35</v>
@@ -5618,7 +5551,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>249</v>
@@ -5626,7 +5559,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B30" s="6">
         <v>30</v>
@@ -5634,7 +5567,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B31" s="6">
         <v>30</v>
@@ -5642,7 +5575,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B32" s="6">
         <v>30</v>
@@ -5650,7 +5583,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>249</v>
@@ -5669,7 +5602,7 @@
         <v>158</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -5677,7 +5610,7 @@
         <v>157</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -5754,7 +5687,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>54</v>
@@ -5886,7 +5819,7 @@
         <v>158</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -5894,7 +5827,7 @@
         <v>157</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -6021,7 +5954,7 @@
         <v>158</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -6029,7 +5962,7 @@
         <v>157</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -6074,7 +6007,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6094,7 +6027,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B2" s="6">
         <v>59</v>
@@ -6102,7 +6035,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B3" s="6">
         <v>30</v>
@@ -6110,7 +6043,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B4" s="6">
         <v>9</v>
@@ -6118,7 +6051,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B5" s="6">
         <v>23</v>
@@ -6126,7 +6059,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B6" s="6">
         <v>13</v>
@@ -6134,7 +6067,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B7" s="6">
         <v>2</v>
@@ -6153,7 +6086,7 @@
         <v>158</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -6161,7 +6094,7 @@
         <v>157</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -6205,8 +6138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75CD6236-1D5E-43C4-8447-268AAEF1A0C5}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6251,7 +6184,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>93</v>
@@ -6270,10 +6203,10 @@
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
+        <v>540</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>541</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>542</v>
       </c>
       <c r="C6" t="s">
         <v>118</v>
@@ -6281,10 +6214,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C7" t="s">
         <v>118</v>
@@ -6292,10 +6225,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C8" t="s">
         <v>118</v>
@@ -6303,10 +6236,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C9" t="s">
         <v>118</v>
@@ -6314,7 +6247,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>95</v>
@@ -6325,7 +6258,7 @@
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>96</v>
@@ -6336,10 +6269,10 @@
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C12" t="s">
         <v>118</v>
@@ -6347,7 +6280,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>186</v>
@@ -6372,7 +6305,7 @@
         <v>86</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>803</v>
+        <v>780</v>
       </c>
       <c r="C15" t="s">
         <v>118</v>
@@ -6380,10 +6313,10 @@
     </row>
     <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>804</v>
+        <v>781</v>
       </c>
       <c r="C16" t="s">
         <v>118</v>
@@ -6468,7 +6401,7 @@
         <v>158</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -6569,7 +6502,7 @@
         <v>158</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -6618,7 +6551,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6644,7 +6577,7 @@
         <v>104</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C2" t="s">
         <v>118</v>
@@ -6655,7 +6588,7 @@
         <v>107</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C3" t="s">
         <v>118</v>
@@ -6666,7 +6599,7 @@
         <v>108</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C4" t="s">
         <v>118</v>
@@ -6674,10 +6607,10 @@
     </row>
     <row r="5" spans="1:3" ht="76.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="C5" t="s">
         <v>118</v>
@@ -6688,7 +6621,7 @@
         <v>110</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="C6" t="s">
         <v>118</v>
@@ -6699,7 +6632,7 @@
         <v>112</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="C7" t="s">
         <v>118</v>
@@ -6740,7 +6673,7 @@
         <v>158</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -6805,7 +6738,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B2" s="5">
         <v>226</v>
@@ -6813,7 +6746,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B3" s="5">
         <v>104</v>
@@ -6821,7 +6754,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B4" s="5">
         <v>93</v>
@@ -6829,7 +6762,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B5" s="5">
         <v>1295</v>
@@ -6837,7 +6770,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B6" s="5">
         <v>3</v>
@@ -6845,7 +6778,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B7" s="5">
         <v>127</v>
@@ -6853,7 +6786,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -6888,7 +6821,7 @@
         <v>158</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -6896,7 +6829,7 @@
         <v>157</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -6936,7 +6869,7 @@
         <v>184</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -6977,7 +6910,7 @@
         <v>105</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C2" t="s">
         <v>118</v>
@@ -6988,7 +6921,7 @@
         <v>106</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C3" t="s">
         <v>118</v>
@@ -6999,7 +6932,7 @@
         <v>109</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C4" t="s">
         <v>118</v>
@@ -7007,10 +6940,10 @@
     </row>
     <row r="5" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="C5" t="s">
         <v>118</v>
@@ -7021,7 +6954,7 @@
         <v>111</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="C6" t="s">
         <v>118</v>
@@ -7032,7 +6965,7 @@
         <v>114</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="C7" t="s">
         <v>118</v>
@@ -7073,7 +7006,7 @@
         <v>158</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -7186,7 +7119,7 @@
     </row>
     <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>131</v>
@@ -7208,7 +7141,7 @@
         <v>158</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -7272,101 +7205,101 @@
     </row>
     <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>376</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>377</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
+        <v>586</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>587</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>588</v>
-      </c>
       <c r="C3" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -7382,7 +7315,7 @@
         <v>158</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
   </sheetData>
@@ -7416,61 +7349,61 @@
     </row>
     <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -7486,7 +7419,7 @@
         <v>158</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -7527,26 +7460,26 @@
     </row>
     <row r="2" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -7562,7 +7495,7 @@
         <v>158</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -7603,82 +7536,82 @@
     </row>
     <row r="2" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>398</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -7694,7 +7627,7 @@
         <v>158</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -7739,7 +7672,7 @@
         <v>191</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>782</v>
+        <v>759</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.3">
@@ -7747,7 +7680,7 @@
         <v>192</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>783</v>
+        <v>760</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.3">
@@ -7755,7 +7688,7 @@
         <v>193</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>784</v>
+        <v>761</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.3">
@@ -7763,7 +7696,7 @@
         <v>194</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>785</v>
+        <v>762</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.3">
@@ -7771,7 +7704,7 @@
         <v>195</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>786</v>
+        <v>763</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.3">
@@ -7779,7 +7712,7 @@
         <v>196</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>787</v>
+        <v>764</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.3">
@@ -7787,7 +7720,7 @@
         <v>197</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>788</v>
+        <v>765</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.3">
@@ -7795,7 +7728,7 @@
         <v>198</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>789</v>
+        <v>766</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.3">
@@ -7803,7 +7736,7 @@
         <v>199</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>790</v>
+        <v>767</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.3">
@@ -7811,7 +7744,7 @@
         <v>338</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>791</v>
+        <v>768</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.3">
@@ -7819,7 +7752,7 @@
         <v>339</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>792</v>
+        <v>769</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.3">
@@ -7827,7 +7760,7 @@
         <v>340</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>793</v>
+        <v>770</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.3">
@@ -7835,7 +7768,7 @@
         <v>341</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>794</v>
+        <v>771</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.3">
@@ -7843,7 +7776,7 @@
         <v>342</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>795</v>
+        <v>772</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.3">
@@ -7851,7 +7784,7 @@
         <v>343</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>796</v>
+        <v>773</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.3">
@@ -7859,7 +7792,7 @@
         <v>200</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>797</v>
+        <v>774</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.3">
@@ -7867,7 +7800,7 @@
         <v>201</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>798</v>
+        <v>775</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.3">
@@ -7875,7 +7808,7 @@
         <v>245</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>799</v>
+        <v>776</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.3">
@@ -7883,7 +7816,7 @@
         <v>246</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>800</v>
+        <v>777</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.3">
@@ -7891,7 +7824,7 @@
         <v>247</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>801</v>
+        <v>778</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.3">
@@ -7899,7 +7832,7 @@
         <v>248</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>802</v>
+        <v>779</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -7915,7 +7848,7 @@
         <v>158</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -7923,7 +7856,7 @@
         <v>157</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -7960,10 +7893,10 @@
     </row>
     <row r="30" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -8005,10 +7938,10 @@
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>601</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>602</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -8016,7 +7949,7 @@
         <v>202</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -8024,7 +7957,7 @@
         <v>203</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -8032,7 +7965,7 @@
         <v>204</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -8040,7 +7973,7 @@
         <v>205</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -8048,7 +7981,7 @@
         <v>206</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -8056,7 +7989,7 @@
         <v>207</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -8064,7 +7997,7 @@
         <v>208</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -8072,15 +8005,15 @@
         <v>209</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -8088,15 +8021,15 @@
         <v>210</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -8104,7 +8037,7 @@
         <v>212</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
@@ -8112,7 +8045,7 @@
         <v>215</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
@@ -8120,7 +8053,7 @@
         <v>213</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
@@ -8128,7 +8061,7 @@
         <v>214</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -8144,7 +8077,7 @@
         <v>158</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -8181,10 +8114,10 @@
     </row>
     <row r="24" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -8229,7 +8162,7 @@
         <v>216</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.3">
@@ -8237,7 +8170,7 @@
         <v>217</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.3">
@@ -8245,7 +8178,7 @@
         <v>218</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.3">
@@ -8253,7 +8186,7 @@
         <v>219</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.3">
@@ -8261,7 +8194,7 @@
         <v>220</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.3">
@@ -8269,7 +8202,7 @@
         <v>221</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.3">
@@ -8277,7 +8210,7 @@
         <v>222</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.3">
@@ -8285,7 +8218,7 @@
         <v>223</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.3">
@@ -8293,7 +8226,7 @@
         <v>224</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="45" x14ac:dyDescent="0.3">
@@ -8301,7 +8234,7 @@
         <v>225</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.3">
@@ -8309,7 +8242,7 @@
         <v>226</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.3">
@@ -8317,7 +8250,7 @@
         <v>315</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="60" x14ac:dyDescent="0.3">
@@ -8325,7 +8258,7 @@
         <v>227</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="75" x14ac:dyDescent="0.3">
@@ -8333,7 +8266,7 @@
         <v>228</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="75" x14ac:dyDescent="0.3">
@@ -8341,7 +8274,7 @@
         <v>229</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
@@ -8365,7 +8298,7 @@
         <v>158</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -8402,10 +8335,10 @@
     </row>
     <row r="24" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -8449,7 +8382,7 @@
         <v>231</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
@@ -8457,7 +8390,7 @@
         <v>232</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
@@ -8465,7 +8398,7 @@
         <v>233</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
@@ -8473,7 +8406,7 @@
         <v>234</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
@@ -8481,7 +8414,7 @@
         <v>235</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
@@ -8489,7 +8422,7 @@
         <v>236</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
@@ -8497,7 +8430,7 @@
         <v>237</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
@@ -8505,7 +8438,7 @@
         <v>238</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
@@ -8513,7 +8446,7 @@
         <v>239</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
@@ -8521,7 +8454,7 @@
         <v>240</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
@@ -8529,7 +8462,7 @@
         <v>241</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
@@ -8537,7 +8470,7 @@
         <v>211</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
@@ -8545,7 +8478,7 @@
         <v>242</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="69" x14ac:dyDescent="0.3">
@@ -8553,7 +8486,7 @@
         <v>243</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
@@ -8561,15 +8494,15 @@
         <v>244</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
+        <v>649</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>650</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>651</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -8585,7 +8518,7 @@
         <v>158</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -8622,10 +8555,10 @@
     </row>
     <row r="24" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -8666,7 +8599,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B2">
         <v>36</v>
@@ -8674,7 +8607,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B3">
         <v>34</v>
@@ -8682,7 +8615,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B4">
         <v>31</v>
@@ -8690,7 +8623,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B5">
         <v>356</v>
@@ -8698,7 +8631,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -8706,7 +8639,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B7">
         <v>36</v>
@@ -8714,7 +8647,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -8722,7 +8655,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B9">
         <v>31</v>
@@ -8730,7 +8663,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -8749,7 +8682,7 @@
         <v>158</v>
       </c>
       <c r="B12" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -8757,7 +8690,7 @@
         <v>157</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -8872,7 +8805,7 @@
         <v>158</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -8880,7 +8813,7 @@
         <v>157</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -8944,7 +8877,7 @@
     </row>
     <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="B2">
         <v>182</v>
@@ -8952,7 +8885,7 @@
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -9000,7 +8933,7 @@
     </row>
     <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -9019,7 +8952,7 @@
         <v>158</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -9027,7 +8960,7 @@
         <v>157</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -9134,7 +9067,7 @@
         <v>158</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -9142,7 +9075,7 @@
         <v>157</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -9219,7 +9152,7 @@
         <v>323</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -9243,7 +9176,7 @@
         <v>158</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -9383,7 +9316,7 @@
         <v>158</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -9391,7 +9324,7 @@
         <v>157</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -9522,7 +9455,7 @@
         <v>158</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -9530,7 +9463,7 @@
         <v>157</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -9595,10 +9528,10 @@
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -9606,7 +9539,7 @@
         <v>363</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -9614,7 +9547,7 @@
         <v>364</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -9622,7 +9555,7 @@
         <v>365</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -9630,7 +9563,7 @@
         <v>366</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -9638,7 +9571,7 @@
         <v>367</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -9646,15 +9579,15 @@
         <v>368</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -9670,7 +9603,7 @@
         <v>158</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -9711,18 +9644,18 @@
     </row>
     <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -9738,7 +9671,7 @@
         <v>158</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -9786,7 +9719,7 @@
         <v>156</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="C2" t="s">
         <v>118</v>
@@ -9794,10 +9727,10 @@
     </row>
     <row r="3" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="C3" t="s">
         <v>118</v>
@@ -9805,10 +9738,10 @@
     </row>
     <row r="4" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="C4" t="s">
         <v>118</v>
@@ -9830,7 +9763,7 @@
         <v>158</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C6" t="s">
         <v>118</v>
@@ -9907,10 +9840,10 @@
     </row>
     <row r="2" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="C2" t="s">
         <v>118</v>
@@ -9918,10 +9851,10 @@
     </row>
     <row r="3" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="C3" t="s">
         <v>118</v>
@@ -9929,10 +9862,10 @@
     </row>
     <row r="4" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="C4" t="s">
         <v>118</v>
@@ -9940,10 +9873,10 @@
     </row>
     <row r="5" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="C5" t="s">
         <v>118</v>
@@ -9951,10 +9884,10 @@
     </row>
     <row r="6" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="C6" t="s">
         <v>118</v>
@@ -9962,10 +9895,10 @@
     </row>
     <row r="7" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="C7" t="s">
         <v>118</v>
@@ -9973,10 +9906,10 @@
     </row>
     <row r="8" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="C8" t="s">
         <v>118</v>
@@ -9984,10 +9917,10 @@
     </row>
     <row r="9" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="C9" t="s">
         <v>118</v>
@@ -9995,10 +9928,10 @@
     </row>
     <row r="10" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="C10" t="s">
         <v>118</v>
@@ -10006,10 +9939,10 @@
     </row>
     <row r="11" spans="1:3" ht="66" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C11" t="s">
         <v>118</v>
@@ -10088,10 +10021,10 @@
     </row>
     <row r="2" spans="1:3" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="C2" t="s">
         <v>118</v>
@@ -10099,10 +10032,10 @@
     </row>
     <row r="3" spans="1:3" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="C3" t="s">
         <v>118</v>
@@ -10110,10 +10043,10 @@
     </row>
     <row r="4" spans="1:3" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="C4" t="s">
         <v>118</v>
@@ -10121,10 +10054,10 @@
     </row>
     <row r="5" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="C5" t="s">
         <v>118</v>
@@ -10132,10 +10065,10 @@
     </row>
     <row r="6" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
       <c r="C6" t="s">
         <v>118</v>
@@ -10143,10 +10076,10 @@
     </row>
     <row r="7" spans="1:3" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="C7" t="s">
         <v>118</v>
@@ -10154,10 +10087,10 @@
     </row>
     <row r="8" spans="1:3" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
       <c r="C8" t="s">
         <v>118</v>
@@ -10196,10 +10129,10 @@
     </row>
     <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="C2" t="s">
         <v>118</v>
@@ -10218,7 +10151,7 @@
         <v>158</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
   </sheetData>
@@ -10251,7 +10184,7 @@
     </row>
     <row r="2" spans="1:2" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B2" s="5">
         <v>3338</v>
@@ -10259,7 +10192,7 @@
     </row>
     <row r="3" spans="1:2" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B3" s="13">
         <v>1038</v>
@@ -10270,7 +10203,7 @@
         <v>163</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -10278,7 +10211,7 @@
         <v>158</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -10286,7 +10219,7 @@
         <v>157</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
refactor code for knowledgebase
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDS_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDS_2020_2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\RHIT_IRPA_@\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E22BE77-C86E-4345-B38F-C466BFF46E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8C96CC-A776-4BA6-96FA-9AF68D7C0A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="8" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="20" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="23" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="800">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="800">
   <si>
     <t>Question</t>
   </si>
@@ -966,9 +966,6 @@
   </si>
   <si>
     <t>The percentage of freshman students who submitted gpa is 94.9 % (504/531)</t>
-  </si>
-  <si>
-    <t>The percentage of freshman with gpa within a certain number of more than that number, or both.</t>
   </si>
   <si>
     <t>The percentage of freshman students with gpa (xor {[^range] [^number] and [^number]} {[^range] [^number]}) is &lt;value&gt;</t>
@@ -2489,6 +2486,9 @@
   </si>
   <si>
     <t>Of the science units, how many high school lab units are recommended for admission?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The percentage of freshman with gpa within a certain number of more than that number, or both. The percentage of freshman student who submitted gpa and the average high school gpa for incoming freshman student who submitted gpa </t>
   </si>
 </sst>
 </file>
@@ -2950,7 +2950,7 @@
     </row>
     <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>3</v>
@@ -2961,7 +2961,7 @@
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>5</v>
@@ -2972,7 +2972,7 @@
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>6</v>
@@ -2983,7 +2983,7 @@
     </row>
     <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>7</v>
@@ -2994,7 +2994,7 @@
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>8</v>
@@ -3005,7 +3005,7 @@
     </row>
     <row r="7" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>9</v>
@@ -3016,7 +3016,7 @@
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>10</v>
@@ -3027,7 +3027,7 @@
     </row>
     <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>11</v>
@@ -3038,7 +3038,7 @@
     </row>
     <row r="10" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>12</v>
@@ -3049,7 +3049,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>13</v>
@@ -3060,7 +3060,7 @@
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>14</v>
@@ -3071,7 +3071,7 @@
     </row>
     <row r="13" spans="1:3" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>15</v>
@@ -3082,7 +3082,7 @@
     </row>
     <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>16</v>
@@ -3478,7 +3478,7 @@
     </row>
     <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>82</v>
@@ -3486,7 +3486,7 @@
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>83</v>
@@ -3494,7 +3494,7 @@
     </row>
     <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B4" s="21" t="s">
         <v>84</v>
@@ -3502,15 +3502,15 @@
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="B6" s="21" t="s">
         <v>85</v>
@@ -3518,7 +3518,7 @@
     </row>
     <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B7" s="21" t="s">
         <v>86</v>
@@ -3526,7 +3526,7 @@
     </row>
     <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="B8" s="21" t="s">
         <v>87</v>
@@ -3534,15 +3534,15 @@
     </row>
     <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="B9" s="21" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="B10" s="21" t="s">
         <v>89</v>
@@ -3550,7 +3550,7 @@
     </row>
     <row r="11" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>90</v>
@@ -3643,7 +3643,7 @@
     </row>
     <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>92</v>
@@ -3651,7 +3651,7 @@
     </row>
     <row r="3" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>93</v>
@@ -3659,7 +3659,7 @@
     </row>
     <row r="4" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="B4" s="21" t="s">
         <v>94</v>
@@ -3667,7 +3667,7 @@
     </row>
     <row r="5" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="B5" s="21" t="s">
         <v>95</v>
@@ -3675,7 +3675,7 @@
     </row>
     <row r="6" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="B6" s="21" t="s">
         <v>96</v>
@@ -3683,7 +3683,7 @@
     </row>
     <row r="7" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="B7" s="21" t="s">
         <v>97</v>
@@ -3691,7 +3691,7 @@
     </row>
     <row r="8" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="B8" s="21" t="s">
         <v>98</v>
@@ -3699,7 +3699,7 @@
     </row>
     <row r="9" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B9" s="21" t="s">
         <v>99</v>
@@ -3707,7 +3707,7 @@
     </row>
     <row r="10" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B10" s="21" t="s">
         <v>100</v>
@@ -3715,7 +3715,7 @@
     </row>
     <row r="11" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>101</v>
@@ -3786,7 +3786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0908D19-61E8-460E-9695-3943D19E115C}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -3805,7 +3805,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>103</v>
@@ -3861,7 +3861,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>116</v>
@@ -3869,7 +3869,7 @@
     </row>
     <row r="10" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>117</v>
@@ -3877,7 +3877,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>118</v>
@@ -3885,7 +3885,7 @@
     </row>
     <row r="12" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>119</v>
@@ -4141,7 +4141,7 @@
     </row>
     <row r="2" spans="1:2" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>160</v>
@@ -4149,7 +4149,7 @@
     </row>
     <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>161</v>
@@ -4165,7 +4165,7 @@
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>164</v>
@@ -4173,7 +4173,7 @@
     </row>
     <row r="6" spans="1:2" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>165</v>
@@ -4206,7 +4206,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4539,7 +4539,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B2" s="5">
         <v>387</v>
@@ -4547,7 +4547,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B3" s="5">
         <v>143</v>
@@ -4555,7 +4555,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B4" s="5">
         <v>1</v>
@@ -4563,7 +4563,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>
@@ -4571,7 +4571,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B6" s="5">
         <v>9</v>
@@ -4579,7 +4579,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B7" s="5">
         <v>2</v>
@@ -4587,7 +4587,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -4595,7 +4595,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B9" s="5">
         <v>0</v>
@@ -4603,7 +4603,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B10" s="5">
         <v>1082</v>
@@ -4611,7 +4611,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B11" s="5">
         <v>329</v>
@@ -4619,7 +4619,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B12" s="5">
         <v>15</v>
@@ -4627,7 +4627,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B13" s="5">
         <v>1</v>
@@ -4635,7 +4635,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B14" s="5">
         <v>0</v>
@@ -4643,7 +4643,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B15" s="5">
         <v>0</v>
@@ -4651,7 +4651,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B16" s="5">
         <v>2</v>
@@ -4659,7 +4659,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B17" s="5">
         <v>1</v>
@@ -4667,7 +4667,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B18" s="5">
         <v>3</v>
@@ -4675,7 +4675,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B19" s="5">
         <v>0</v>
@@ -4683,7 +4683,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B20" s="5">
         <v>2</v>
@@ -4691,7 +4691,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="B21" s="5">
         <v>1</v>
@@ -4699,7 +4699,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B22" s="5">
         <v>6</v>
@@ -4707,7 +4707,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B23" s="5">
         <v>1</v>
@@ -4715,7 +4715,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B24" s="5">
         <v>5</v>
@@ -4723,7 +4723,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B25" s="5">
         <v>0</v>
@@ -4731,7 +4731,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B26" s="5">
         <v>0</v>
@@ -4739,7 +4739,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B27" s="5">
         <v>0</v>
@@ -4747,7 +4747,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B28" s="5">
         <v>0</v>
@@ -4755,7 +4755,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B29" s="5">
         <v>0</v>
@@ -4822,7 +4822,7 @@
         <v>29</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
   </sheetData>
@@ -4836,7 +4836,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5150,7 +5150,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:B12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5185,7 +5185,7 @@
     </row>
     <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>235</v>
@@ -5193,7 +5193,7 @@
     </row>
     <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>236</v>
@@ -5265,8 +5265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3892E9F-E7EA-42B9-AE4C-1275BBD6A387}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="80" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView topLeftCell="A15" zoomScale="80" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5605,10 +5605,10 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB852AE-A4C7-4284-9FBD-1CEEB9311916}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5618,139 +5618,103 @@
     <col min="3" max="3" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>275</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>277</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>279</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>281</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>283</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>285</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>287</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>288</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>289</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>290</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>292</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
@@ -5758,23 +5722,23 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
@@ -5819,8 +5783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDBBFCBD-BE53-4EBE-BC28-AF1024B4BD2D}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5839,39 +5803,39 @@
     </row>
     <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>296</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>298</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>300</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>302</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>174</v>
@@ -5879,10 +5843,10 @@
     </row>
     <row r="7" spans="1:2" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>305</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -5898,7 +5862,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -5906,7 +5870,7 @@
         <v>27</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -5951,7 +5915,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5969,25 +5933,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B2" s="6">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="B3" s="6">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="B4" s="6">
         <v>9</v>
@@ -5995,7 +5959,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="B5" s="6">
         <v>23</v>
@@ -6003,7 +5967,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B6" s="6">
         <v>13</v>
@@ -6011,7 +5975,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="B7" s="6">
         <v>2</v>
@@ -6030,7 +5994,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -6038,7 +6002,7 @@
         <v>27</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -6075,6 +6039,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
@@ -6106,10 +6071,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -6117,10 +6082,10 @@
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>312</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>313</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -6128,18 +6093,18 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>314</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>316</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>317</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -6147,10 +6112,10 @@
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6158,10 +6123,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -6169,10 +6134,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -6180,10 +6145,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -6191,10 +6156,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -6202,10 +6167,10 @@
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -6213,10 +6178,10 @@
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>324</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>325</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -6224,10 +6189,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>326</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>327</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -6235,10 +6200,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -6246,10 +6211,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>329</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>330</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -6257,10 +6222,10 @@
     </row>
     <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>331</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>332</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -6268,10 +6233,10 @@
     </row>
     <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>333</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>334</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -6279,10 +6244,10 @@
     </row>
     <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>335</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>336</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -6290,10 +6255,10 @@
     </row>
     <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>337</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>338</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -6301,10 +6266,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>339</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>340</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -6312,10 +6277,10 @@
     </row>
     <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>341</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>342</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -6323,10 +6288,10 @@
     </row>
     <row r="22" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>343</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>344</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
@@ -6345,7 +6310,7 @@
         <v>19</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -6413,10 +6378,10 @@
     </row>
     <row r="2" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>346</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>347</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -6424,10 +6389,10 @@
     </row>
     <row r="3" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>348</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>349</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -6446,7 +6411,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -6518,10 +6483,10 @@
     </row>
     <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>351</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>352</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -6529,10 +6494,10 @@
     </row>
     <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>353</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>354</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -6540,10 +6505,10 @@
     </row>
     <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>355</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>356</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -6551,10 +6516,10 @@
     </row>
     <row r="5" spans="1:3" ht="76.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>357</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>358</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -6562,10 +6527,10 @@
     </row>
     <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>359</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>360</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6573,10 +6538,10 @@
     </row>
     <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>361</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>362</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -6584,10 +6549,10 @@
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>363</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>364</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -6595,10 +6560,10 @@
     </row>
     <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>365</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>366</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -6617,7 +6582,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -6682,7 +6647,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B2" s="5">
         <v>226</v>
@@ -6690,7 +6655,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B3" s="5">
         <v>104</v>
@@ -6698,7 +6663,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B4" s="5">
         <v>93</v>
@@ -6706,7 +6671,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B5" s="5">
         <v>1295</v>
@@ -6714,7 +6679,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B6" s="5">
         <v>3</v>
@@ -6722,7 +6687,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B7" s="5">
         <v>127</v>
@@ -6730,7 +6695,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
@@ -6738,7 +6703,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B9" s="5">
         <v>99</v>
@@ -6746,7 +6711,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B10" s="5">
         <v>22</v>
@@ -6813,7 +6778,7 @@
         <v>29</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
   </sheetData>
@@ -6851,10 +6816,10 @@
     </row>
     <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>368</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>369</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -6862,10 +6827,10 @@
     </row>
     <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>370</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>371</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -6873,10 +6838,10 @@
     </row>
     <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>372</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>373</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -6884,10 +6849,10 @@
     </row>
     <row r="5" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>374</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>375</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -6895,10 +6860,10 @@
     </row>
     <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>376</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>377</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6906,10 +6871,10 @@
     </row>
     <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>378</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>379</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -6917,10 +6882,10 @@
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>380</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>381</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -6928,10 +6893,10 @@
     </row>
     <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>382</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>383</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -6950,7 +6915,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -7019,10 +6984,10 @@
     </row>
     <row r="2" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -7030,10 +6995,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -7041,10 +7006,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -7052,10 +7017,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -7063,10 +7028,10 @@
     </row>
     <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7085,7 +7050,7 @@
         <v>19</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -7149,101 +7114,101 @@
     </row>
     <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>391</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>392</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>394</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>395</v>
-      </c>
       <c r="C3" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>398</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>399</v>
-      </c>
       <c r="C6" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>401</v>
-      </c>
       <c r="C7" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>402</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>403</v>
-      </c>
       <c r="C8" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>404</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>405</v>
-      </c>
       <c r="C9" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>406</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>407</v>
-      </c>
       <c r="C10" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -7259,7 +7224,7 @@
         <v>19</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
   </sheetData>
@@ -7293,61 +7258,61 @@
     </row>
     <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>409</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>410</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>411</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>413</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>415</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>417</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>419</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>421</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -7363,7 +7328,7 @@
         <v>19</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -7404,26 +7369,26 @@
     </row>
     <row r="2" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>424</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>426</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>428</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -7439,7 +7404,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -7480,82 +7445,82 @@
     </row>
     <row r="2" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>431</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>433</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>435</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>437</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>439</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>441</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>443</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>445</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>447</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>449</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -7571,7 +7536,7 @@
         <v>19</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -7613,170 +7578,170 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="B2" s="23" t="s">
         <v>452</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
+        <v>453</v>
+      </c>
+      <c r="B3" s="23" t="s">
         <v>454</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
+        <v>455</v>
+      </c>
+      <c r="B4" s="23" t="s">
         <v>456</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
+        <v>457</v>
+      </c>
+      <c r="B5" s="23" t="s">
         <v>458</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
+        <v>459</v>
+      </c>
+      <c r="B6" s="23" t="s">
         <v>460</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
+        <v>461</v>
+      </c>
+      <c r="B7" s="23" t="s">
         <v>462</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
+        <v>463</v>
+      </c>
+      <c r="B8" s="23" t="s">
         <v>464</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="B9" s="23" t="s">
         <v>466</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="B10" s="23" t="s">
         <v>468</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
+        <v>469</v>
+      </c>
+      <c r="B11" s="23" t="s">
         <v>470</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="B12" s="23" t="s">
         <v>472</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
+        <v>473</v>
+      </c>
+      <c r="B13" s="23" t="s">
         <v>474</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
+        <v>475</v>
+      </c>
+      <c r="B14" s="23" t="s">
         <v>476</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
+        <v>477</v>
+      </c>
+      <c r="B15" s="23" t="s">
         <v>478</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
+        <v>479</v>
+      </c>
+      <c r="B16" s="23" t="s">
         <v>480</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="B17" s="23" t="s">
         <v>482</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
+        <v>483</v>
+      </c>
+      <c r="B18" s="23" t="s">
         <v>484</v>
-      </c>
-      <c r="B18" s="23" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
+        <v>485</v>
+      </c>
+      <c r="B19" s="23" t="s">
         <v>486</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
+        <v>487</v>
+      </c>
+      <c r="B20" s="23" t="s">
         <v>488</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
+        <v>489</v>
+      </c>
+      <c r="B21" s="23" t="s">
         <v>490</v>
-      </c>
-      <c r="B21" s="23" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="B22" s="23" t="s">
         <v>492</v>
-      </c>
-      <c r="B22" s="23" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -7792,7 +7757,7 @@
         <v>19</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -7829,10 +7794,10 @@
     </row>
     <row r="29" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="B29" s="22" t="s">
         <v>495</v>
-      </c>
-      <c r="B29" s="22" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -7874,130 +7839,130 @@
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>496</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>497</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
+        <v>498</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>499</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>501</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
+        <v>502</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>503</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
+        <v>504</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>505</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
+        <v>506</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>507</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
+        <v>508</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>509</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
+        <v>510</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>511</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
+        <v>512</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>513</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
+        <v>514</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>515</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
+        <v>516</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>517</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
+        <v>518</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>519</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
+        <v>520</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>521</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
+        <v>522</v>
+      </c>
+      <c r="B15" s="14" t="s">
         <v>523</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
+        <v>524</v>
+      </c>
+      <c r="B16" s="14" t="s">
         <v>525</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
+        <v>526</v>
+      </c>
+      <c r="B17" s="14" t="s">
         <v>527</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -8013,7 +7978,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -8050,10 +8015,10 @@
     </row>
     <row r="24" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>495</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -8095,130 +8060,130 @@
     </row>
     <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>530</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
+        <v>531</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>532</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
+        <v>533</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>534</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
+        <v>535</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>536</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
+        <v>537</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>538</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
+        <v>539</v>
+      </c>
+      <c r="B7" s="16" t="s">
         <v>540</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
+        <v>541</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>542</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
+        <v>543</v>
+      </c>
+      <c r="B9" s="16" t="s">
         <v>544</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
+        <v>545</v>
+      </c>
+      <c r="B10" s="16" t="s">
         <v>546</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="45" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
+        <v>547</v>
+      </c>
+      <c r="B11" s="16" t="s">
         <v>548</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
+        <v>549</v>
+      </c>
+      <c r="B12" s="16" t="s">
         <v>550</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
+        <v>551</v>
+      </c>
+      <c r="B13" s="16" t="s">
         <v>552</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="60" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
+        <v>553</v>
+      </c>
+      <c r="B14" s="16" t="s">
         <v>554</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="75" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
+        <v>555</v>
+      </c>
+      <c r="B15" s="16" t="s">
         <v>556</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="75" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
+        <v>557</v>
+      </c>
+      <c r="B16" s="16" t="s">
         <v>558</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="B17" s="15" t="s">
         <v>560</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -8234,7 +8199,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -8271,10 +8236,10 @@
     </row>
     <row r="24" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>495</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -8315,130 +8280,130 @@
     </row>
     <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>562</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>563</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
+        <v>564</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>565</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
+        <v>566</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>567</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
+        <v>568</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>569</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
+        <v>570</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>571</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
+        <v>572</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>573</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
+        <v>574</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>575</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
+        <v>576</v>
+      </c>
+      <c r="B9" s="14" t="s">
         <v>577</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
+        <v>578</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>579</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>581</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
+        <v>582</v>
+      </c>
+      <c r="B12" s="14" t="s">
         <v>583</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
+        <v>584</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>585</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
+        <v>586</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>587</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="69" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
+        <v>588</v>
+      </c>
+      <c r="B15" s="14" t="s">
         <v>589</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
+        <v>590</v>
+      </c>
+      <c r="B16" s="14" t="s">
         <v>591</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
+        <v>592</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>593</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -8454,7 +8419,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -8491,10 +8456,10 @@
     </row>
     <row r="24" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>495</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -8535,7 +8500,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B2">
         <v>36</v>
@@ -8543,7 +8508,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B3">
         <v>34</v>
@@ -8551,7 +8516,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B4">
         <v>31</v>
@@ -8559,7 +8524,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B5">
         <v>356</v>
@@ -8567,7 +8532,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -8575,7 +8540,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B7">
         <v>36</v>
@@ -8583,7 +8548,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -8591,7 +8556,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B9">
         <v>31</v>
@@ -8599,7 +8564,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -8666,7 +8631,7 @@
         <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
   </sheetData>
@@ -8699,7 +8664,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B2">
         <v>50</v>
@@ -8707,7 +8672,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -8715,7 +8680,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B4">
         <v>137</v>
@@ -8723,7 +8688,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -8742,7 +8707,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -8750,7 +8715,7 @@
         <v>27</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -8814,7 +8779,7 @@
     </row>
     <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B2">
         <v>182</v>
@@ -8822,7 +8787,7 @@
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -8830,7 +8795,7 @@
     </row>
     <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -8838,7 +8803,7 @@
     </row>
     <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -8846,7 +8811,7 @@
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -8854,7 +8819,7 @@
     </row>
     <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -8862,7 +8827,7 @@
     </row>
     <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -8870,7 +8835,7 @@
     </row>
     <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -8889,7 +8854,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -8897,7 +8862,7 @@
         <v>27</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -8961,7 +8926,7 @@
     </row>
     <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B2">
         <v>33</v>
@@ -8969,7 +8934,7 @@
     </row>
     <row r="3" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -8977,7 +8942,7 @@
     </row>
     <row r="4" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B4">
         <v>8</v>
@@ -8985,7 +8950,7 @@
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -9004,7 +8969,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -9012,7 +8977,7 @@
         <v>27</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -9078,26 +9043,26 @@
     </row>
     <row r="2" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>617</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>618</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>619</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -9113,7 +9078,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -9186,7 +9151,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B3">
         <v>76</v>
@@ -9194,7 +9159,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B4">
         <v>216</v>
@@ -9202,7 +9167,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B5">
         <v>129</v>
@@ -9210,7 +9175,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -9218,7 +9183,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -9226,7 +9191,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -9234,7 +9199,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -9253,7 +9218,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -9261,7 +9226,7 @@
         <v>27</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -9325,7 +9290,7 @@
     </row>
     <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -9333,7 +9298,7 @@
     </row>
     <row r="3" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B3">
         <v>33</v>
@@ -9341,7 +9306,7 @@
     </row>
     <row r="4" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B4">
         <v>31</v>
@@ -9349,7 +9314,7 @@
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -9357,7 +9322,7 @@
     </row>
     <row r="6" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -9365,7 +9330,7 @@
     </row>
     <row r="7" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -9373,7 +9338,7 @@
     </row>
     <row r="8" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -9392,7 +9357,7 @@
         <v>19</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -9400,7 +9365,7 @@
         <v>27</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -9465,66 +9430,66 @@
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -9540,7 +9505,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -9548,7 +9513,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
   </sheetData>
@@ -9581,18 +9546,18 @@
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="52.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -9608,7 +9573,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -9616,7 +9581,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
   </sheetData>
@@ -9650,7 +9615,7 @@
     </row>
     <row r="2" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>34</v>
@@ -9658,7 +9623,7 @@
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>35</v>
@@ -9666,7 +9631,7 @@
     </row>
     <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>36</v>
@@ -9761,7 +9726,7 @@
     </row>
     <row r="2" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>39</v>
@@ -9769,7 +9734,7 @@
     </row>
     <row r="3" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>40</v>
@@ -9777,7 +9742,7 @@
     </row>
     <row r="4" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>41</v>
@@ -9785,7 +9750,7 @@
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="B5" s="19" t="s">
         <v>42</v>
@@ -9793,7 +9758,7 @@
     </row>
     <row r="6" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>43</v>
@@ -9801,7 +9766,7 @@
     </row>
     <row r="7" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B7" s="19" t="s">
         <v>44</v>
@@ -9809,7 +9774,7 @@
     </row>
     <row r="8" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>45</v>
@@ -9817,7 +9782,7 @@
     </row>
     <row r="9" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>46</v>
@@ -9825,7 +9790,7 @@
     </row>
     <row r="10" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>47</v>
@@ -9921,7 +9886,7 @@
     </row>
     <row r="2" spans="1:3" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>50</v>
@@ -9932,7 +9897,7 @@
     </row>
     <row r="3" spans="1:3" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>50</v>
@@ -9943,7 +9908,7 @@
     </row>
     <row r="4" spans="1:3" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>51</v>
@@ -9954,7 +9919,7 @@
     </row>
     <row r="5" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B5" s="20" t="s">
         <v>52</v>
@@ -9965,7 +9930,7 @@
     </row>
     <row r="6" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>53</v>
@@ -9976,7 +9941,7 @@
     </row>
     <row r="7" spans="1:3" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B7" s="19" t="s">
         <v>54</v>
@@ -9987,7 +9952,7 @@
     </row>
     <row r="8" spans="1:3" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>55</v>
@@ -10045,7 +10010,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -10162,6 +10127,33 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="e087321b-8427-4435-894a-2aaead00236e">
+      <UserInfo>
+        <DisplayName>Domeika Ponsot, Brenda</DisplayName>
+        <AccountId>21</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e048074d-3639-4eff-bcc1-9fbc40a3e423">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="e087321b-8427-4435-894a-2aaead00236e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B366D4A85A89B74A9B45BFCC07AEDED5" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d8fec9556fe6b39abb6c801f923e75d5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e048074d-3639-4eff-bcc1-9fbc40a3e423" xmlns:ns3="e087321b-8427-4435-894a-2aaead00236e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bce2b814ab3f24009331a69a791f2225" ns2:_="" ns3:_="">
     <xsd:import namespace="e048074d-3639-4eff-bcc1-9fbc40a3e423"/>
@@ -10378,34 +10370,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{541D2107-39A4-4F1E-8E81-5FFFAAB18004}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="e087321b-8427-4435-894a-2aaead00236e"/>
+    <ds:schemaRef ds:uri="e048074d-3639-4eff-bcc1-9fbc40a3e423"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="e087321b-8427-4435-894a-2aaead00236e">
-      <UserInfo>
-        <DisplayName>Domeika Ponsot, Brenda</DisplayName>
-        <AccountId>21</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e048074d-3639-4eff-bcc1-9fbc40a3e423">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="e087321b-8427-4435-894a-2aaead00236e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5F4F942-7CDB-4C95-9954-DE123114A2FF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{711ADE17-97B7-4DD8-837D-39ED7E8DE6F3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10422,29 +10412,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5F4F942-7CDB-4C95-9954-DE123114A2FF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{541D2107-39A4-4F1E-8E81-5FFFAAB18004}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="e087321b-8427-4435-894a-2aaead00236e"/>
-    <ds:schemaRef ds:uri="e048074d-3639-4eff-bcc1-9fbc40a3e423"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixed bug for year
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDS_2020_2021.xlsx
+++ b/NewCDSDataFromClient/CDS_2020_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\RHIT_IRPA_@\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8C96CC-A776-4BA6-96FA-9AF68D7C0A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C4CE3C-1DDD-4DCF-9B91-3C461F488374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="20" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="23" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="800">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="800">
   <si>
     <t>Question</t>
   </si>
@@ -2924,10 +2924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E422E2F-D9FA-411F-968E-DE340F994DF5}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="96" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" zoomScale="96" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2937,161 +2937,119 @@
     <col min="3" max="3" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>659</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>660</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>661</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>662</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>663</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>664</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>665</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>666</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>658</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:2" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>667</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>668</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:2" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>669</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>670</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>17</v>
       </c>
@@ -3099,7 +3057,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>19</v>
       </c>
@@ -3786,8 +3744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0908D19-61E8-460E-9695-3943D19E115C}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="58.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5607,8 +5565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB852AE-A4C7-4284-9FBD-1CEEB9311916}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9594,8 +9552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7606B2B-8397-4A8E-AF38-C293D77D8867}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="91" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A3" zoomScale="91" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9705,8 +9663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{119C6780-FAAF-467C-AAE4-76FBEA215EAD}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9862,8 +9820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60EF61F8-9012-491B-B537-F5D367E2A90B}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10032,7 +9990,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>